<commit_message>
fix(Examples): Update excel template
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -9,21 +9,21 @@
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="ListExtractors" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="ListDigesters" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="ListReducers" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="ListAutoclusters" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="ListTrajectories" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Settings" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Files" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Bands" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Integrations" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Ranges" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Extractors" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Digesters" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Reducers" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Autoclusters" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Trajectories" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Settings" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Files" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Bands" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Integrations" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Ranges" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Extractors" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Digesters" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Reducers" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Autoclusters" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Trajectories" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="ListExtractors" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="ListDigesters" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="ListReducers" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="ListAutoclusters" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="ListTrajectories" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -34,7 +34,7 @@
 </workbook>
 </file>
 
-<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author> </author>
@@ -70,7 +70,7 @@
 </comments>
 </file>
 
-<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author> </author>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="140">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -559,15 +559,72 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:5531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">human</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vgg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silhouette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overlap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contingency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_cluster_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsilon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hdbscan-eom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_value</t>
+  </si>
+  <si>
     <t xml:space="preserve">indicator</t>
   </si>
   <si>
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">vgg</t>
-  </si>
-  <si>
     <t xml:space="preserve">The VGGish neural network.</t>
   </si>
   <si>
@@ -652,27 +709,15 @@
     <t xml:space="preserve">The distance between subtypes of a given cluster.</t>
   </si>
   <si>
-    <t xml:space="preserve">overlap</t>
-  </si>
-  <si>
     <t xml:space="preserve">The overlap between subtypes of a given cluster.</t>
   </si>
   <si>
-    <t xml:space="preserve">silhouette</t>
-  </si>
-  <si>
     <t xml:space="preserve">The silhouette between subtypes of a given cluster.</t>
   </si>
   <si>
-    <t xml:space="preserve">contingency</t>
-  </si>
-  <si>
     <t xml:space="preserve">Contingency between two clusters.</t>
   </si>
   <si>
-    <t xml:space="preserve">umap</t>
-  </si>
-  <si>
     <t xml:space="preserve">vae</t>
   </si>
   <si>
@@ -682,9 +727,6 @@
     <t xml:space="preserve">sparse_pca</t>
   </si>
   <si>
-    <t xml:space="preserve">hdbscan-eom</t>
-  </si>
-  <si>
     <t xml:space="preserve">hdbscan-leaf</t>
   </si>
   <si>
@@ -695,60 +737,6 @@
   </si>
   <si>
     <t xml:space="preserve">month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">setting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://localhost:5531</t>
-  </si>
-  <si>
-    <t xml:space="preserve">human</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min_cluster_size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min_samples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alpha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsilon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">day1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIEU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">naturel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">day2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">day3</t>
   </si>
 </sst>
 </file>
@@ -975,6 +963,86 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -993,86 +1061,6 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1551,346 +1539,6 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="18.97"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="32" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="28"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="28"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="28"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="32" width="20.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" s="33" t="n">
-        <v>44927</v>
-      </c>
-      <c r="C2" s="33" t="n">
-        <v>45292</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="28"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="15.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="5" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="28" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>132</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
-      <formula1>ListExtractors!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="15.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="31" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>Help!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1006" type="list">
-      <formula1>ListDigesters!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="32" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="32" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="32" width="25.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="32" t="n">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
-      <formula1>ListReducers!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1903,47 +1551,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="23" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>136</v>
+      <c r="B1" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>95</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="28" t="n">
-        <v>15</v>
-      </c>
-      <c r="C2" s="28" t="n">
-        <v>15</v>
-      </c>
-      <c r="D2" s="28" t="n">
+      <c r="A2" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="23" t="n">
+        <v>50</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="28" t="n">
-        <v>0.1</v>
+      <c r="E2" s="23" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1967,7 +1615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -1981,102 +1629,64 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="32" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="32" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="27" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="27" width="18.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="30" t="s">
+      <c r="D1" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="33" t="n">
-        <v>44881.5</v>
-      </c>
-      <c r="C2" s="33" t="n">
-        <v>44882.5416666667</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>123</v>
-      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="33" t="n">
-        <v>44887.5</v>
-      </c>
-      <c r="C3" s="33" t="n">
-        <v>44888.5416666667</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>123</v>
-      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="33" t="n">
-        <v>44907.5</v>
-      </c>
-      <c r="C4" s="33" t="n">
-        <v>44908.5416666667</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>123</v>
-      </c>
+      <c r="A4" s="31"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1004" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1001" type="list">
       <formula1>ListTrajectories!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2091,7 +1701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFEEEEEE"/>
@@ -2109,89 +1719,89 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
-        <v>80</v>
+      <c r="A1" s="35" t="s">
+        <v>100</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>83</v>
+      <c r="A2" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>85</v>
+      <c r="A3" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>87</v>
+      <c r="A4" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>89</v>
+      <c r="A5" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>91</v>
+      <c r="A6" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>93</v>
+      <c r="A7" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>95</v>
+      <c r="A8" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>97</v>
+      <c r="A9" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>99</v>
+      <c r="A10" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2205,7 +1815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFEEEEEE"/>
@@ -2223,85 +1833,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
-        <v>100</v>
+      <c r="A1" s="35" t="s">
+        <v>119</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>102</v>
+      <c r="A2" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>104</v>
+      <c r="A3" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>106</v>
+      <c r="A4" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>108</v>
+      <c r="A5" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>110</v>
+      <c r="A6" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>112</v>
+      <c r="A7" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>114</v>
+      <c r="A8" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>116</v>
+      <c r="A9" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="17"/>
+      <c r="B10" s="37"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2314,7 +1924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFEEEEEE"/>
@@ -2332,33 +1942,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="35" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>117</v>
+      <c r="A2" s="33" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>118</v>
+      <c r="A3" s="33" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>119</v>
+      <c r="A4" s="33" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>120</v>
+      <c r="A5" s="33" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2372,7 +1982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFEEEEEE"/>
@@ -2390,23 +2000,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="35" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>121</v>
+      <c r="A2" s="33" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>122</v>
+      <c r="A3" s="33" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2420,7 +2030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFEEEEEE"/>
@@ -2434,28 +2044,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="35" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>123</v>
+      <c r="A2" s="33" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>124</v>
+      <c r="A3" s="33" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>125</v>
+      <c r="A4" s="33" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2469,7 +2079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -2493,73 +2103,73 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>127</v>
+      <c r="A1" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="20" t="str">
+      <c r="B2" s="15" t="str">
         <f aca="false">"/path/to/your/audio/folder"</f>
         <v>/path/to/your/audio/folder</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>128</v>
+      <c r="B3" s="16" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="20" t="n">
+      <c r="B4" s="15" t="n">
         <v>44100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="22" t="n">
+      <c r="B5" s="17" t="n">
         <v>45089.8854166667</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="24" t="n">
+      <c r="B7" s="19" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="24" t="n">
+      <c r="B8" s="19" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="24" t="n">
+      <c r="B9" s="19" t="n">
         <v>42000</v>
       </c>
     </row>
@@ -2577,7 +2187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -2595,71 +2205,71 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="28" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="29" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="23" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="24" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="str">
+      <c r="A2" s="14" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="22" t="n">
+      <c r="C2" s="17" t="n">
         <v>45089.8854166667</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>127</v>
+      <c r="D2" s="23" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="22"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="20"/>
+      <c r="C7" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2672,7 +2282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFD7"/>
@@ -2690,44 +2300,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="32" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="27" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="25" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="32" t="n">
+      <c r="A2" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="27" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="32" t="n">
+      <c r="C2" s="27" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2738,4 +2348,334 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="18.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="27" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="23"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="23"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="23"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="27" width="20.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="28" t="n">
+        <v>44927</v>
+      </c>
+      <c r="C2" s="28" t="n">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="23"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="15.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="5" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+      <formula1>ListExtractors!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="15.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>Help!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1004" type="list">
+      <formula1>ListDigesters!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFD7"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="27" width="25.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
+      <formula1>ListReducers!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix(Examples): Update `new-campaign` template (remove YAML + Update xlsx)
BREAKING CHANGE: Configuration file has been changed (`storage_path` has
been added).
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="143">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -565,6 +565,15 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
+    <t xml:space="preserve">storage_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relative/or/absolute/path/to/file.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relative/or/absolute/path/to/audio/folder</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://localhost:5531</t>
   </si>
   <si>
@@ -743,10 +752,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -971,18 +979,18 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1023,7 +1031,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1035,11 +1043,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1564,28 +1572,28 @@
         <v>64</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B2" s="23" t="n">
         <v>50</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D2" s="23" t="n">
         <v>1</v>
@@ -1646,10 +1654,10 @@
         <v>49</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>56</v>
@@ -1726,82 +1734,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="33" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="33" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="33" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="33" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1840,74 +1848,74 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="33" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="33" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="33" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,22 +1961,22 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2011,12 +2019,12 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2055,17 +2063,17 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2085,7 +2093,7 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2112,70 +2120,77 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="15" t="str">
-        <f aca="false">"/path/to/your/audio/folder"</f>
-        <v>/path/to/your/audio/folder</v>
+        <v>82</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="15" t="n">
-        <v>44100</v>
+        <v>9</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="15" t="n">
+        <v>44100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="17" t="n">
+      <c r="B6" s="17" t="n">
         <v>45089.8854166667</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="19" t="n">
-        <v>5</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="19" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="19" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="19" t="n">
+      <c r="B10" s="19" t="n">
         <v>42000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="http://localhost:5531"/>
+    <hyperlink ref="B4" r:id="rId1" display="http://localhost:5531"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2318,7 +2333,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B2" s="27" t="n">
         <v>20</v>
@@ -2383,7 +2398,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B2" s="27" t="n">
         <v>15</v>
@@ -2445,7 +2460,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B2" s="28" t="n">
         <v>44927</v>
@@ -2510,7 +2525,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B2" s="27" t="n">
         <v>0</v>
@@ -2519,7 +2534,7 @@
         <v>1000</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2565,17 +2580,17 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2641,7 +2656,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B2" s="23" t="n">
         <v>2</v>
@@ -2652,7 +2667,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B3" s="27" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
feat(Config): Added `storage_path` + Update documentation
BREAKING CHANGE: `storage_path` has been added to the configuration.
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -94,12 +94,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="144">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
   <si>
-    <t xml:space="preserve">Version 10</t>
+    <t xml:space="preserve">Version 11</t>
   </si>
   <si>
     <t xml:space="preserve">Instructions</t>
@@ -117,11 +117,45 @@
     <t xml:space="preserve">Settings</t>
   </si>
   <si>
+    <t xml:space="preserve">storage_path</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The path to your storage file. Should end with `.h5`. Absolute or relative to this file.
+Examples: `storage.h5`, `</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">D:\storage.h5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">`.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">audio_path</t>
   </si>
   <si>
-    <t xml:space="preserve">The relative or absolute path to your audio folder.
-Examples: `./relative/path/to/audio` `/absolute/path/to/audio`.</t>
+    <t xml:space="preserve">The path to your audio folder. Absolute or relative to this file.
+Examples: `audio`, `C:\path\to\audio`.</t>
   </si>
   <si>
     <t xml:space="preserve">audio_host</t>
@@ -565,13 +599,10 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relative/or/absolute/path/to/file.h5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relative/or/absolute/path/to/audio/folder</t>
+    <t xml:space="preserve">storage.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\path\to\audio</t>
   </si>
   <si>
     <t xml:space="preserve">http://localhost:5531</t>
@@ -802,6 +833,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
@@ -812,13 +850,6 @@
     <font>
       <i val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -955,11 +986,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -983,22 +1014,22 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1039,7 +1070,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1063,11 +1094,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1149,7 +1180,7 @@
     <tabColor rgb="FFEEEEEE"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -1214,11 +1245,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1230,11 +1261,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1262,19 +1293,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B15" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
@@ -1293,26 +1324,26 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B21" s="12" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="7" t="s">
+      <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
@@ -1330,19 +1361,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B26" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="7" t="s">
+      <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
@@ -1352,19 +1383,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B30" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="7" t="s">
+      <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="B32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
@@ -1382,19 +1413,19 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B35" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="7" t="s">
+      <c r="A37" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="B37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
@@ -1420,54 +1451,54 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B41" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="7" t="s">
+      <c r="A43" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B44" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="7" t="s">
+      <c r="A46" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B47" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" s="12" t="s">
+      <c r="A49" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="B49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>48</v>
+        <v>69</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1478,21 +1509,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" s="7" t="s">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
         <v>72</v>
       </c>
@@ -1500,11 +1531,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9" t="s">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="7" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1522,6 +1553,14 @@
       </c>
       <c r="B58" s="10" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1530,6 +1569,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" location="readme" display="Find documentation here: https://github.com/sound-scape-explorer/sound-scape-explorer#readme"/>
+    <hyperlink ref="B7" r:id="rId2" display="D:\storage.h5"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1569,31 +1609,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B2" s="23" t="n">
         <v>50</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D2" s="23" t="n">
         <v>1</v>
@@ -1645,22 +1685,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,82 +1774,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="33" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="33" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="33" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="33" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1848,74 +1888,74 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="33" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,27 +1996,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2014,17 +2054,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2058,22 +2098,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2112,39 +2152,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="15" t="n">
         <v>44100</v>
@@ -2152,7 +2192,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" s="17" t="n">
         <v>45089.8854166667</v>
@@ -2160,29 +2200,29 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="19" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="19" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="19" t="n">
         <v>42000</v>
@@ -2230,16 +2270,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>26</v>
-      </c>
       <c r="D1" s="25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
@@ -2254,13 +2294,13 @@
         <v>/path/from/audio/folder</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2" s="17" t="n">
         <v>45089.8854166667</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,18 +2362,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B2" s="27" t="n">
         <v>20</v>
@@ -2390,15 +2430,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B2" s="27" t="n">
         <v>15</v>
@@ -2449,18 +2489,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B2" s="28" t="n">
         <v>44927</v>
@@ -2510,22 +2550,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B2" s="27" t="n">
         <v>0</v>
@@ -2534,7 +2574,7 @@
         <v>1000</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2575,22 +2615,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2638,25 +2678,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B2" s="23" t="n">
         <v>2</v>
@@ -2667,7 +2707,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B3" s="27" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
fix(Examples): Update Excel documentation
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -120,35 +120,8 @@
     <t xml:space="preserve">storage_path</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The path to your storage file. Should end with `.h5`. Absolute or relative to this file.
-Examples: `storage.h5`, `</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">D:\storage.h5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">`.</t>
-    </r>
+    <t xml:space="preserve">The path to your storage file. Absolute or relative to this file. Should end with `.h5`.
+Examples: `storage.h5`, `C:\path\to\storage.h5`.</t>
   </si>
   <si>
     <t xml:space="preserve">audio_path</t>
@@ -787,7 +760,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -834,10 +807,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -850,6 +821,13 @@
     <font>
       <i val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -949,7 +927,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -978,6 +956,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1014,7 +996,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1066,7 +1048,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1241,7 +1223,7 @@
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1249,7 +1231,7 @@
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1257,7 +1239,7 @@
       <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1265,39 +1247,39 @@
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1311,7 +1293,7 @@
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1319,7 +1301,7 @@
       <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1327,15 +1309,15 @@
       <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="13" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1349,7 +1331,7 @@
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1357,7 +1339,7 @@
       <c r="A25" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1365,7 +1347,7 @@
       <c r="A26" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1379,7 +1361,7 @@
       <c r="A29" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1387,7 +1369,7 @@
       <c r="A30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="8" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1401,7 +1383,7 @@
       <c r="A33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1409,7 +1391,7 @@
       <c r="A34" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1417,7 +1399,7 @@
       <c r="A35" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1431,7 +1413,7 @@
       <c r="A38" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1439,7 +1421,7 @@
       <c r="A39" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1447,7 +1429,7 @@
       <c r="A40" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1455,7 +1437,7 @@
       <c r="A41" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="8" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1469,7 +1451,7 @@
       <c r="A44" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="8" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1483,7 +1465,7 @@
       <c r="A47" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1497,7 +1479,7 @@
       <c r="A50" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="13" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1505,7 +1487,7 @@
       <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1513,7 +1495,7 @@
       <c r="A52" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1527,7 +1509,7 @@
       <c r="A55" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="8" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1535,31 +1517,31 @@
       <c r="A56" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="11" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1569,7 +1551,6 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" location="readme" display="Find documentation here: https://github.com/sound-scape-explorer/sound-scape-explorer#readme"/>
-    <hyperlink ref="B7" r:id="rId2" display="D:\storage.h5"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1599,46 +1580,46 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="23" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="24" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="26" t="s">
         <v>99</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="23" t="n">
+      <c r="B2" s="24" t="n">
         <v>50</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1677,60 +1658,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="27" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="27" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="28" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="28" width="18.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="26" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1767,13 +1748,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>104</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1781,74 +1762,74 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="38" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="38" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="38" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="38" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1881,13 +1862,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>123</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1895,71 +1876,71 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="37" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="37" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="37"/>
+      <c r="B10" s="38"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1990,32 +1971,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="34" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2048,22 +2029,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2092,27 +2073,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="16.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2151,80 +2132,80 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="15" t="n">
+      <c r="B5" s="16" t="n">
         <v>44100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="17" t="n">
+      <c r="B6" s="18" t="n">
         <v>45089.8854166667</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="19" t="n">
+      <c r="B8" s="20" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="19" t="n">
+      <c r="B9" s="20" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="19" t="n">
+      <c r="B10" s="20" t="n">
         <v>42000</v>
       </c>
     </row>
@@ -2260,71 +2241,71 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="23" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="24" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="24" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="25" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="str">
+      <c r="A2" s="15" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="17" t="n">
+      <c r="C2" s="18" t="n">
         <v>45089.8854166667</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="24" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="17"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="15"/>
+      <c r="C7" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2355,44 +2336,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="27" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="28" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="27" t="n">
+      <c r="B2" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="27" t="n">
+      <c r="C2" s="28" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2423,35 +2404,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="27" t="n">
+      <c r="B2" s="28" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="23"/>
+      <c r="B4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="23"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="23"/>
+      <c r="B6" s="24"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2482,39 +2463,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="27" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="28" width="20.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="28" t="n">
+      <c r="B2" s="29" t="n">
         <v>44927</v>
       </c>
-      <c r="C2" s="28" t="n">
+      <c r="C2" s="29" t="n">
         <v>45292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="23"/>
+      <c r="C4" s="24"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2541,39 +2522,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="15.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="5" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>60</v>
       </c>
       <c r="E1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="27" t="n">
+      <c r="B2" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="24" t="n">
         <v>1000</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2609,27 +2590,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2668,48 +2649,48 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="27" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="30" t="s">
         <v>80</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="23" t="n">
+      <c r="B2" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="27" t="n">
+      <c r="B3" s="28" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(Config): Update default configuration's ergonomy
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -14,11 +14,11 @@
     <sheet name="Bands" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Integrations" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Ranges" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Extractors" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Digesters" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Reducers" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Autoclusters" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Trajectories" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Trajectories" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Extractors" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Digesters" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Reducers" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Autoclusters" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="ListExtractors" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="ListDigesters" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="ListReducers" sheetId="14" state="visible" r:id="rId15"/>
@@ -34,7 +34,76 @@
 </workbook>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Use 2 or 3 unless not human</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Should end with `.h5`</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Should start with a “/”</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author> </author>
@@ -70,48 +139,26 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Use 2 or 3 unless not human</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="144">
   <si>
-    <t xml:space="preserve">Sound Scape Explorer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version 11</t>
-  </si>
-  <si>
     <t xml:space="preserve">Instructions</t>
   </si>
   <si>
+    <t xml:space="preserve">SoundScapeExplorer
+Version 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fill the yellow tabs</t>
   </si>
   <si>
-    <t xml:space="preserve">See help below</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Find documentation here: https://github.com/sound-scape-explorer/sound-scape-explorer#readme</t>
+    <t xml:space="preserve">Configure the blue tabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find more information in grey tabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiki: https://github.com/sound-scape-explorer/sound-scape-explorer/wiki</t>
   </si>
   <si>
     <t xml:space="preserve">Settings</t>
@@ -590,6 +637,12 @@
     <t xml:space="preserve">r2023</t>
   </si>
   <si>
+    <t xml:space="preserve">label_property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_value</t>
+  </si>
+  <si>
     <t xml:space="preserve">vgg</t>
   </si>
   <si>
@@ -624,12 +677,6 @@
   </si>
   <si>
     <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_value</t>
   </si>
   <si>
     <t xml:space="preserve">indicator</t>
@@ -760,7 +807,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -806,11 +853,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
@@ -842,7 +884,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,8 +899,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
+        <fgColor rgb="FF111111"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFDEE6EF"/>
       </patternFill>
     </fill>
     <fill>
@@ -869,20 +917,38 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFDEE6EF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF443205"/>
+        <bgColor rgb="FF383D3C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFD7"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFDEE6EF"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF443205"/>
-        <bgColor rgb="FF333333"/>
+        <fgColor rgb="FF383D3C"/>
+        <bgColor rgb="FF443205"/>
       </patternFill>
     </fill>
   </fills>
@@ -927,7 +993,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -936,151 +1002,179 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1109,16 +1203,16 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFD7"/>
-      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFDEE6EF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1128,7 +1222,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFFA6"/>
       <rgbColor rgb="FF99CCFF"/>
@@ -1145,12 +1239,12 @@
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF111111"/>
       <rgbColor rgb="FF443205"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF383D3C"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1159,398 +1253,402 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFEEEEEE"/>
+    <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="0" ySplit="5" topLeftCell="B18" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="90.96"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B11" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B12" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B13" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B14" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B15" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B16" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B19" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B21" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B22" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B25" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B26" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B27" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
+      <c r="B29" s="9"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B30" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B31" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
+      <c r="B33" s="9"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B34" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B35" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="s">
+      <c r="B38" s="9"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B39" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B40" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B41" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B42" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
+      <c r="B44" s="9"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B45" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
+      <c r="B47" s="9"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B48" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6" t="s">
+      <c r="B50" s="9"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B51" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="6" t="s">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B52" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B53" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6" t="s">
+      <c r="B55" s="9"/>
+    </row>
+    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B56" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="s">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B57" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="10" t="s">
+    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B58" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="s">
+    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B59" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="10" t="s">
+    <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B60" s="14" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" location="readme" display="Find documentation here: https://github.com/sound-scape-explorer/sound-scape-explorer#readme"/>
+    <hyperlink ref="B5" r:id="rId1" display="Wiki: https://github.com/sound-scape-explorer/sound-scape-explorer/wiki"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1565,7 +1663,88 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
+    <tabColor rgb="FFB4C7DC"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="36" width="25.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="36" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+      <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
+      <formula1>ListReducers!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F2"/>
@@ -1580,46 +1759,46 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="24" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="37" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="37" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="37" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="26" t="s">
+      <c r="B1" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="C1" s="38" t="s">
         <v>99</v>
       </c>
+      <c r="D1" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>101</v>
+      </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="24" t="n">
+      <c r="A2" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="37" t="n">
         <v>50</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="24" t="n">
+      <c r="C2" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="24" t="n">
+      <c r="E2" s="37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1644,96 +1823,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="28" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="28" width="18.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="7" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1001" type="list">
-      <formula1>ListTrajectories!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFEEEEEE"/>
+    <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
@@ -1743,93 +1836,93 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="42" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="43" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" s="37" t="s">
+      <c r="A2" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="44" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="44" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="44" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="44" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="45" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="45" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="45" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="45" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1847,7 +1940,7 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFEEEEEE"/>
+    <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
@@ -1857,90 +1950,90 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="42" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="43" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="44" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="44" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="44" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="44" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="44" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="37" t="s">
+      <c r="A7" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="44" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="37" t="s">
+      <c r="A8" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="44" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="37" t="s">
+      <c r="A9" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="44" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="38"/>
+      <c r="B10" s="45"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1956,7 +2049,7 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFEEEEEE"/>
+    <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A5"/>
@@ -1971,32 +2064,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
-        <v>95</v>
+      <c r="A2" s="15" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="15" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="15" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="15" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2014,7 +2107,7 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFEEEEEE"/>
+    <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
@@ -2024,27 +2117,27 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
-        <v>100</v>
+      <c r="A2" s="15" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="15" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2062,38 +2155,38 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFEEEEEE"/>
+    <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="15" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="15" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="15" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2111,7 +2204,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
+    <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
@@ -2132,86 +2225,86 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="19" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="20" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="16" t="n">
+      <c r="B5" s="19" t="n">
         <v>44100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="18" t="n">
-        <v>45089.8854166667</v>
+      <c r="B6" s="21" t="n">
+        <v>36526</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="20"/>
+      <c r="B7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="20" t="n">
+      <c r="B8" s="23" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="20" t="n">
+      <c r="B9" s="23" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="20" t="n">
+      <c r="B10" s="23" t="n">
         <v>42000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="http://localhost:5531"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://localhost:5531"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2220,13 +2313,14 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
+    <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J7"/>
@@ -2241,71 +2335,71 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="24" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="25" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="27" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="28" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="str">
+      <c r="A2" s="18" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="18" t="n">
+      <c r="C2" s="21" t="n">
         <v>45089.8854166667</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="18"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="16"/>
+      <c r="C7" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2315,13 +2409,14 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
+    <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C6"/>
@@ -2336,44 +2431,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="28" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="28" t="n">
+      <c r="B2" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="28" t="n">
+      <c r="C2" s="31" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2389,7 +2484,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
+    <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B6"/>
@@ -2404,35 +2499,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="28" t="n">
+      <c r="B2" s="31" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="24"/>
+      <c r="B4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="24"/>
+      <c r="B5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="24"/>
+      <c r="B6" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2448,7 +2543,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
+    <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C4"/>
@@ -2463,39 +2558,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="28" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="20.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="29" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="29" t="n">
+      <c r="B2" s="32" t="n">
         <v>44927</v>
       </c>
-      <c r="C2" s="29" t="n">
+      <c r="C2" s="32" t="n">
         <v>45292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="24"/>
+      <c r="C4" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2511,10 +2606,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
+    <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2522,40 +2617,1134 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="31" width="18.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="7" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="33"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1001" type="list">
+      <formula1>ListTrajectories!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFB4C7DC"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:ALY2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="37" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="37" width="15.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="5" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="38" t="s">
         <v>60</v>
       </c>
       <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="0"/>
+      <c r="S1" s="0"/>
+      <c r="T1" s="0"/>
+      <c r="U1" s="0"/>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
+      <c r="AG1" s="0"/>
+      <c r="AH1" s="0"/>
+      <c r="AI1" s="0"/>
+      <c r="AJ1" s="0"/>
+      <c r="AK1" s="0"/>
+      <c r="AL1" s="0"/>
+      <c r="AM1" s="0"/>
+      <c r="AN1" s="0"/>
+      <c r="AO1" s="0"/>
+      <c r="AP1" s="0"/>
+      <c r="AQ1" s="0"/>
+      <c r="AR1" s="0"/>
+      <c r="AS1" s="0"/>
+      <c r="AT1" s="0"/>
+      <c r="AU1" s="0"/>
+      <c r="AV1" s="0"/>
+      <c r="AW1" s="0"/>
+      <c r="AX1" s="0"/>
+      <c r="AY1" s="0"/>
+      <c r="AZ1" s="0"/>
+      <c r="BA1" s="0"/>
+      <c r="BB1" s="0"/>
+      <c r="BC1" s="0"/>
+      <c r="BD1" s="0"/>
+      <c r="BE1" s="0"/>
+      <c r="BF1" s="0"/>
+      <c r="BG1" s="0"/>
+      <c r="BH1" s="0"/>
+      <c r="BI1" s="0"/>
+      <c r="BJ1" s="0"/>
+      <c r="BK1" s="0"/>
+      <c r="BL1" s="0"/>
+      <c r="BM1" s="0"/>
+      <c r="BN1" s="0"/>
+      <c r="BO1" s="0"/>
+      <c r="BP1" s="0"/>
+      <c r="BQ1" s="0"/>
+      <c r="BR1" s="0"/>
+      <c r="BS1" s="0"/>
+      <c r="BT1" s="0"/>
+      <c r="BU1" s="0"/>
+      <c r="BV1" s="0"/>
+      <c r="BW1" s="0"/>
+      <c r="BX1" s="0"/>
+      <c r="BY1" s="0"/>
+      <c r="BZ1" s="0"/>
+      <c r="CA1" s="0"/>
+      <c r="CB1" s="0"/>
+      <c r="CC1" s="0"/>
+      <c r="CD1" s="0"/>
+      <c r="CE1" s="0"/>
+      <c r="CF1" s="0"/>
+      <c r="CG1" s="0"/>
+      <c r="CH1" s="0"/>
+      <c r="CI1" s="0"/>
+      <c r="CJ1" s="0"/>
+      <c r="CK1" s="0"/>
+      <c r="CL1" s="0"/>
+      <c r="CM1" s="0"/>
+      <c r="CN1" s="0"/>
+      <c r="CO1" s="0"/>
+      <c r="CP1" s="0"/>
+      <c r="CQ1" s="0"/>
+      <c r="CR1" s="0"/>
+      <c r="CS1" s="0"/>
+      <c r="CT1" s="0"/>
+      <c r="CU1" s="0"/>
+      <c r="CV1" s="0"/>
+      <c r="CW1" s="0"/>
+      <c r="CX1" s="0"/>
+      <c r="CY1" s="0"/>
+      <c r="CZ1" s="0"/>
+      <c r="DA1" s="0"/>
+      <c r="DB1" s="0"/>
+      <c r="DC1" s="0"/>
+      <c r="DD1" s="0"/>
+      <c r="DE1" s="0"/>
+      <c r="DF1" s="0"/>
+      <c r="DG1" s="0"/>
+      <c r="DH1" s="0"/>
+      <c r="DI1" s="0"/>
+      <c r="DJ1" s="0"/>
+      <c r="DK1" s="0"/>
+      <c r="DL1" s="0"/>
+      <c r="DM1" s="0"/>
+      <c r="DN1" s="0"/>
+      <c r="DO1" s="0"/>
+      <c r="DP1" s="0"/>
+      <c r="DQ1" s="0"/>
+      <c r="DR1" s="0"/>
+      <c r="DS1" s="0"/>
+      <c r="DT1" s="0"/>
+      <c r="DU1" s="0"/>
+      <c r="DV1" s="0"/>
+      <c r="DW1" s="0"/>
+      <c r="DX1" s="0"/>
+      <c r="DY1" s="0"/>
+      <c r="DZ1" s="0"/>
+      <c r="EA1" s="0"/>
+      <c r="EB1" s="0"/>
+      <c r="EC1" s="0"/>
+      <c r="ED1" s="0"/>
+      <c r="EE1" s="0"/>
+      <c r="EF1" s="0"/>
+      <c r="EG1" s="0"/>
+      <c r="EH1" s="0"/>
+      <c r="EI1" s="0"/>
+      <c r="EJ1" s="0"/>
+      <c r="EK1" s="0"/>
+      <c r="EL1" s="0"/>
+      <c r="EM1" s="0"/>
+      <c r="EN1" s="0"/>
+      <c r="EO1" s="0"/>
+      <c r="EP1" s="0"/>
+      <c r="EQ1" s="0"/>
+      <c r="ER1" s="0"/>
+      <c r="ES1" s="0"/>
+      <c r="ET1" s="0"/>
+      <c r="EU1" s="0"/>
+      <c r="EV1" s="0"/>
+      <c r="EW1" s="0"/>
+      <c r="EX1" s="0"/>
+      <c r="EY1" s="0"/>
+      <c r="EZ1" s="0"/>
+      <c r="FA1" s="0"/>
+      <c r="FB1" s="0"/>
+      <c r="FC1" s="0"/>
+      <c r="FD1" s="0"/>
+      <c r="FE1" s="0"/>
+      <c r="FF1" s="0"/>
+      <c r="FG1" s="0"/>
+      <c r="FH1" s="0"/>
+      <c r="FI1" s="0"/>
+      <c r="FJ1" s="0"/>
+      <c r="FK1" s="0"/>
+      <c r="FL1" s="0"/>
+      <c r="FM1" s="0"/>
+      <c r="FN1" s="0"/>
+      <c r="FO1" s="0"/>
+      <c r="FP1" s="0"/>
+      <c r="FQ1" s="0"/>
+      <c r="FR1" s="0"/>
+      <c r="FS1" s="0"/>
+      <c r="FT1" s="0"/>
+      <c r="FU1" s="0"/>
+      <c r="FV1" s="0"/>
+      <c r="FW1" s="0"/>
+      <c r="FX1" s="0"/>
+      <c r="FY1" s="0"/>
+      <c r="FZ1" s="0"/>
+      <c r="GA1" s="0"/>
+      <c r="GB1" s="0"/>
+      <c r="GC1" s="0"/>
+      <c r="GD1" s="0"/>
+      <c r="GE1" s="0"/>
+      <c r="GF1" s="0"/>
+      <c r="GG1" s="0"/>
+      <c r="GH1" s="0"/>
+      <c r="GI1" s="0"/>
+      <c r="GJ1" s="0"/>
+      <c r="GK1" s="0"/>
+      <c r="GL1" s="0"/>
+      <c r="GM1" s="0"/>
+      <c r="GN1" s="0"/>
+      <c r="GO1" s="0"/>
+      <c r="GP1" s="0"/>
+      <c r="GQ1" s="0"/>
+      <c r="GR1" s="0"/>
+      <c r="GS1" s="0"/>
+      <c r="GT1" s="0"/>
+      <c r="GU1" s="0"/>
+      <c r="GV1" s="0"/>
+      <c r="GW1" s="0"/>
+      <c r="GX1" s="0"/>
+      <c r="GY1" s="0"/>
+      <c r="GZ1" s="0"/>
+      <c r="HA1" s="0"/>
+      <c r="HB1" s="0"/>
+      <c r="HC1" s="0"/>
+      <c r="HD1" s="0"/>
+      <c r="HE1" s="0"/>
+      <c r="HF1" s="0"/>
+      <c r="HG1" s="0"/>
+      <c r="HH1" s="0"/>
+      <c r="HI1" s="0"/>
+      <c r="HJ1" s="0"/>
+      <c r="HK1" s="0"/>
+      <c r="HL1" s="0"/>
+      <c r="HM1" s="0"/>
+      <c r="HN1" s="0"/>
+      <c r="HO1" s="0"/>
+      <c r="HP1" s="0"/>
+      <c r="HQ1" s="0"/>
+      <c r="HR1" s="0"/>
+      <c r="HS1" s="0"/>
+      <c r="HT1" s="0"/>
+      <c r="HU1" s="0"/>
+      <c r="HV1" s="0"/>
+      <c r="HW1" s="0"/>
+      <c r="HX1" s="0"/>
+      <c r="HY1" s="0"/>
+      <c r="HZ1" s="0"/>
+      <c r="IA1" s="0"/>
+      <c r="IB1" s="0"/>
+      <c r="IC1" s="0"/>
+      <c r="ID1" s="0"/>
+      <c r="IE1" s="0"/>
+      <c r="IF1" s="0"/>
+      <c r="IG1" s="0"/>
+      <c r="IH1" s="0"/>
+      <c r="II1" s="0"/>
+      <c r="IJ1" s="0"/>
+      <c r="IK1" s="0"/>
+      <c r="IL1" s="0"/>
+      <c r="IM1" s="0"/>
+      <c r="IN1" s="0"/>
+      <c r="IO1" s="0"/>
+      <c r="IP1" s="0"/>
+      <c r="IQ1" s="0"/>
+      <c r="IR1" s="0"/>
+      <c r="IS1" s="0"/>
+      <c r="IT1" s="0"/>
+      <c r="IU1" s="0"/>
+      <c r="IV1" s="0"/>
+      <c r="IW1" s="0"/>
+      <c r="IX1" s="0"/>
+      <c r="IY1" s="0"/>
+      <c r="IZ1" s="0"/>
+      <c r="JA1" s="0"/>
+      <c r="JB1" s="0"/>
+      <c r="JC1" s="0"/>
+      <c r="JD1" s="0"/>
+      <c r="JE1" s="0"/>
+      <c r="JF1" s="0"/>
+      <c r="JG1" s="0"/>
+      <c r="JH1" s="0"/>
+      <c r="JI1" s="0"/>
+      <c r="JJ1" s="0"/>
+      <c r="JK1" s="0"/>
+      <c r="JL1" s="0"/>
+      <c r="JM1" s="0"/>
+      <c r="JN1" s="0"/>
+      <c r="JO1" s="0"/>
+      <c r="JP1" s="0"/>
+      <c r="JQ1" s="0"/>
+      <c r="JR1" s="0"/>
+      <c r="JS1" s="0"/>
+      <c r="JT1" s="0"/>
+      <c r="JU1" s="0"/>
+      <c r="JV1" s="0"/>
+      <c r="JW1" s="0"/>
+      <c r="JX1" s="0"/>
+      <c r="JY1" s="0"/>
+      <c r="JZ1" s="0"/>
+      <c r="KA1" s="0"/>
+      <c r="KB1" s="0"/>
+      <c r="KC1" s="0"/>
+      <c r="KD1" s="0"/>
+      <c r="KE1" s="0"/>
+      <c r="KF1" s="0"/>
+      <c r="KG1" s="0"/>
+      <c r="KH1" s="0"/>
+      <c r="KI1" s="0"/>
+      <c r="KJ1" s="0"/>
+      <c r="KK1" s="0"/>
+      <c r="KL1" s="0"/>
+      <c r="KM1" s="0"/>
+      <c r="KN1" s="0"/>
+      <c r="KO1" s="0"/>
+      <c r="KP1" s="0"/>
+      <c r="KQ1" s="0"/>
+      <c r="KR1" s="0"/>
+      <c r="KS1" s="0"/>
+      <c r="KT1" s="0"/>
+      <c r="KU1" s="0"/>
+      <c r="KV1" s="0"/>
+      <c r="KW1" s="0"/>
+      <c r="KX1" s="0"/>
+      <c r="KY1" s="0"/>
+      <c r="KZ1" s="0"/>
+      <c r="LA1" s="0"/>
+      <c r="LB1" s="0"/>
+      <c r="LC1" s="0"/>
+      <c r="LD1" s="0"/>
+      <c r="LE1" s="0"/>
+      <c r="LF1" s="0"/>
+      <c r="LG1" s="0"/>
+      <c r="LH1" s="0"/>
+      <c r="LI1" s="0"/>
+      <c r="LJ1" s="0"/>
+      <c r="LK1" s="0"/>
+      <c r="LL1" s="0"/>
+      <c r="LM1" s="0"/>
+      <c r="LN1" s="0"/>
+      <c r="LO1" s="0"/>
+      <c r="LP1" s="0"/>
+      <c r="LQ1" s="0"/>
+      <c r="LR1" s="0"/>
+      <c r="LS1" s="0"/>
+      <c r="LT1" s="0"/>
+      <c r="LU1" s="0"/>
+      <c r="LV1" s="0"/>
+      <c r="LW1" s="0"/>
+      <c r="LX1" s="0"/>
+      <c r="LY1" s="0"/>
+      <c r="LZ1" s="0"/>
+      <c r="MA1" s="0"/>
+      <c r="MB1" s="0"/>
+      <c r="MC1" s="0"/>
+      <c r="MD1" s="0"/>
+      <c r="ME1" s="0"/>
+      <c r="MF1" s="0"/>
+      <c r="MG1" s="0"/>
+      <c r="MH1" s="0"/>
+      <c r="MI1" s="0"/>
+      <c r="MJ1" s="0"/>
+      <c r="MK1" s="0"/>
+      <c r="ML1" s="0"/>
+      <c r="MM1" s="0"/>
+      <c r="MN1" s="0"/>
+      <c r="MO1" s="0"/>
+      <c r="MP1" s="0"/>
+      <c r="MQ1" s="0"/>
+      <c r="MR1" s="0"/>
+      <c r="MS1" s="0"/>
+      <c r="MT1" s="0"/>
+      <c r="MU1" s="0"/>
+      <c r="MV1" s="0"/>
+      <c r="MW1" s="0"/>
+      <c r="MX1" s="0"/>
+      <c r="MY1" s="0"/>
+      <c r="MZ1" s="0"/>
+      <c r="NA1" s="0"/>
+      <c r="NB1" s="0"/>
+      <c r="NC1" s="0"/>
+      <c r="ND1" s="0"/>
+      <c r="NE1" s="0"/>
+      <c r="NF1" s="0"/>
+      <c r="NG1" s="0"/>
+      <c r="NH1" s="0"/>
+      <c r="NI1" s="0"/>
+      <c r="NJ1" s="0"/>
+      <c r="NK1" s="0"/>
+      <c r="NL1" s="0"/>
+      <c r="NM1" s="0"/>
+      <c r="NN1" s="0"/>
+      <c r="NO1" s="0"/>
+      <c r="NP1" s="0"/>
+      <c r="NQ1" s="0"/>
+      <c r="NR1" s="0"/>
+      <c r="NS1" s="0"/>
+      <c r="NT1" s="0"/>
+      <c r="NU1" s="0"/>
+      <c r="NV1" s="0"/>
+      <c r="NW1" s="0"/>
+      <c r="NX1" s="0"/>
+      <c r="NY1" s="0"/>
+      <c r="NZ1" s="0"/>
+      <c r="OA1" s="0"/>
+      <c r="OB1" s="0"/>
+      <c r="OC1" s="0"/>
+      <c r="OD1" s="0"/>
+      <c r="OE1" s="0"/>
+      <c r="OF1" s="0"/>
+      <c r="OG1" s="0"/>
+      <c r="OH1" s="0"/>
+      <c r="OI1" s="0"/>
+      <c r="OJ1" s="0"/>
+      <c r="OK1" s="0"/>
+      <c r="OL1" s="0"/>
+      <c r="OM1" s="0"/>
+      <c r="ON1" s="0"/>
+      <c r="OO1" s="0"/>
+      <c r="OP1" s="0"/>
+      <c r="OQ1" s="0"/>
+      <c r="OR1" s="0"/>
+      <c r="OS1" s="0"/>
+      <c r="OT1" s="0"/>
+      <c r="OU1" s="0"/>
+      <c r="OV1" s="0"/>
+      <c r="OW1" s="0"/>
+      <c r="OX1" s="0"/>
+      <c r="OY1" s="0"/>
+      <c r="OZ1" s="0"/>
+      <c r="PA1" s="0"/>
+      <c r="PB1" s="0"/>
+      <c r="PC1" s="0"/>
+      <c r="PD1" s="0"/>
+      <c r="PE1" s="0"/>
+      <c r="PF1" s="0"/>
+      <c r="PG1" s="0"/>
+      <c r="PH1" s="0"/>
+      <c r="PI1" s="0"/>
+      <c r="PJ1" s="0"/>
+      <c r="PK1" s="0"/>
+      <c r="PL1" s="0"/>
+      <c r="PM1" s="0"/>
+      <c r="PN1" s="0"/>
+      <c r="PO1" s="0"/>
+      <c r="PP1" s="0"/>
+      <c r="PQ1" s="0"/>
+      <c r="PR1" s="0"/>
+      <c r="PS1" s="0"/>
+      <c r="PT1" s="0"/>
+      <c r="PU1" s="0"/>
+      <c r="PV1" s="0"/>
+      <c r="PW1" s="0"/>
+      <c r="PX1" s="0"/>
+      <c r="PY1" s="0"/>
+      <c r="PZ1" s="0"/>
+      <c r="QA1" s="0"/>
+      <c r="QB1" s="0"/>
+      <c r="QC1" s="0"/>
+      <c r="QD1" s="0"/>
+      <c r="QE1" s="0"/>
+      <c r="QF1" s="0"/>
+      <c r="QG1" s="0"/>
+      <c r="QH1" s="0"/>
+      <c r="QI1" s="0"/>
+      <c r="QJ1" s="0"/>
+      <c r="QK1" s="0"/>
+      <c r="QL1" s="0"/>
+      <c r="QM1" s="0"/>
+      <c r="QN1" s="0"/>
+      <c r="QO1" s="0"/>
+      <c r="QP1" s="0"/>
+      <c r="QQ1" s="0"/>
+      <c r="QR1" s="0"/>
+      <c r="QS1" s="0"/>
+      <c r="QT1" s="0"/>
+      <c r="QU1" s="0"/>
+      <c r="QV1" s="0"/>
+      <c r="QW1" s="0"/>
+      <c r="QX1" s="0"/>
+      <c r="QY1" s="0"/>
+      <c r="QZ1" s="0"/>
+      <c r="RA1" s="0"/>
+      <c r="RB1" s="0"/>
+      <c r="RC1" s="0"/>
+      <c r="RD1" s="0"/>
+      <c r="RE1" s="0"/>
+      <c r="RF1" s="0"/>
+      <c r="RG1" s="0"/>
+      <c r="RH1" s="0"/>
+      <c r="RI1" s="0"/>
+      <c r="RJ1" s="0"/>
+      <c r="RK1" s="0"/>
+      <c r="RL1" s="0"/>
+      <c r="RM1" s="0"/>
+      <c r="RN1" s="0"/>
+      <c r="RO1" s="0"/>
+      <c r="RP1" s="0"/>
+      <c r="RQ1" s="0"/>
+      <c r="RR1" s="0"/>
+      <c r="RS1" s="0"/>
+      <c r="RT1" s="0"/>
+      <c r="RU1" s="0"/>
+      <c r="RV1" s="0"/>
+      <c r="RW1" s="0"/>
+      <c r="RX1" s="0"/>
+      <c r="RY1" s="0"/>
+      <c r="RZ1" s="0"/>
+      <c r="SA1" s="0"/>
+      <c r="SB1" s="0"/>
+      <c r="SC1" s="0"/>
+      <c r="SD1" s="0"/>
+      <c r="SE1" s="0"/>
+      <c r="SF1" s="0"/>
+      <c r="SG1" s="0"/>
+      <c r="SH1" s="0"/>
+      <c r="SI1" s="0"/>
+      <c r="SJ1" s="0"/>
+      <c r="SK1" s="0"/>
+      <c r="SL1" s="0"/>
+      <c r="SM1" s="0"/>
+      <c r="SN1" s="0"/>
+      <c r="SO1" s="0"/>
+      <c r="SP1" s="0"/>
+      <c r="SQ1" s="0"/>
+      <c r="SR1" s="0"/>
+      <c r="SS1" s="0"/>
+      <c r="ST1" s="0"/>
+      <c r="SU1" s="0"/>
+      <c r="SV1" s="0"/>
+      <c r="SW1" s="0"/>
+      <c r="SX1" s="0"/>
+      <c r="SY1" s="0"/>
+      <c r="SZ1" s="0"/>
+      <c r="TA1" s="0"/>
+      <c r="TB1" s="0"/>
+      <c r="TC1" s="0"/>
+      <c r="TD1" s="0"/>
+      <c r="TE1" s="0"/>
+      <c r="TF1" s="0"/>
+      <c r="TG1" s="0"/>
+      <c r="TH1" s="0"/>
+      <c r="TI1" s="0"/>
+      <c r="TJ1" s="0"/>
+      <c r="TK1" s="0"/>
+      <c r="TL1" s="0"/>
+      <c r="TM1" s="0"/>
+      <c r="TN1" s="0"/>
+      <c r="TO1" s="0"/>
+      <c r="TP1" s="0"/>
+      <c r="TQ1" s="0"/>
+      <c r="TR1" s="0"/>
+      <c r="TS1" s="0"/>
+      <c r="TT1" s="0"/>
+      <c r="TU1" s="0"/>
+      <c r="TV1" s="0"/>
+      <c r="TW1" s="0"/>
+      <c r="TX1" s="0"/>
+      <c r="TY1" s="0"/>
+      <c r="TZ1" s="0"/>
+      <c r="UA1" s="0"/>
+      <c r="UB1" s="0"/>
+      <c r="UC1" s="0"/>
+      <c r="UD1" s="0"/>
+      <c r="UE1" s="0"/>
+      <c r="UF1" s="0"/>
+      <c r="UG1" s="0"/>
+      <c r="UH1" s="0"/>
+      <c r="UI1" s="0"/>
+      <c r="UJ1" s="0"/>
+      <c r="UK1" s="0"/>
+      <c r="UL1" s="0"/>
+      <c r="UM1" s="0"/>
+      <c r="UN1" s="0"/>
+      <c r="UO1" s="0"/>
+      <c r="UP1" s="0"/>
+      <c r="UQ1" s="0"/>
+      <c r="UR1" s="0"/>
+      <c r="US1" s="0"/>
+      <c r="UT1" s="0"/>
+      <c r="UU1" s="0"/>
+      <c r="UV1" s="0"/>
+      <c r="UW1" s="0"/>
+      <c r="UX1" s="0"/>
+      <c r="UY1" s="0"/>
+      <c r="UZ1" s="0"/>
+      <c r="VA1" s="0"/>
+      <c r="VB1" s="0"/>
+      <c r="VC1" s="0"/>
+      <c r="VD1" s="0"/>
+      <c r="VE1" s="0"/>
+      <c r="VF1" s="0"/>
+      <c r="VG1" s="0"/>
+      <c r="VH1" s="0"/>
+      <c r="VI1" s="0"/>
+      <c r="VJ1" s="0"/>
+      <c r="VK1" s="0"/>
+      <c r="VL1" s="0"/>
+      <c r="VM1" s="0"/>
+      <c r="VN1" s="0"/>
+      <c r="VO1" s="0"/>
+      <c r="VP1" s="0"/>
+      <c r="VQ1" s="0"/>
+      <c r="VR1" s="0"/>
+      <c r="VS1" s="0"/>
+      <c r="VT1" s="0"/>
+      <c r="VU1" s="0"/>
+      <c r="VV1" s="0"/>
+      <c r="VW1" s="0"/>
+      <c r="VX1" s="0"/>
+      <c r="VY1" s="0"/>
+      <c r="VZ1" s="0"/>
+      <c r="WA1" s="0"/>
+      <c r="WB1" s="0"/>
+      <c r="WC1" s="0"/>
+      <c r="WD1" s="0"/>
+      <c r="WE1" s="0"/>
+      <c r="WF1" s="0"/>
+      <c r="WG1" s="0"/>
+      <c r="WH1" s="0"/>
+      <c r="WI1" s="0"/>
+      <c r="WJ1" s="0"/>
+      <c r="WK1" s="0"/>
+      <c r="WL1" s="0"/>
+      <c r="WM1" s="0"/>
+      <c r="WN1" s="0"/>
+      <c r="WO1" s="0"/>
+      <c r="WP1" s="0"/>
+      <c r="WQ1" s="0"/>
+      <c r="WR1" s="0"/>
+      <c r="WS1" s="0"/>
+      <c r="WT1" s="0"/>
+      <c r="WU1" s="0"/>
+      <c r="WV1" s="0"/>
+      <c r="WW1" s="0"/>
+      <c r="WX1" s="0"/>
+      <c r="WY1" s="0"/>
+      <c r="WZ1" s="0"/>
+      <c r="XA1" s="0"/>
+      <c r="XB1" s="0"/>
+      <c r="XC1" s="0"/>
+      <c r="XD1" s="0"/>
+      <c r="XE1" s="0"/>
+      <c r="XF1" s="0"/>
+      <c r="XG1" s="0"/>
+      <c r="XH1" s="0"/>
+      <c r="XI1" s="0"/>
+      <c r="XJ1" s="0"/>
+      <c r="XK1" s="0"/>
+      <c r="XL1" s="0"/>
+      <c r="XM1" s="0"/>
+      <c r="XN1" s="0"/>
+      <c r="XO1" s="0"/>
+      <c r="XP1" s="0"/>
+      <c r="XQ1" s="0"/>
+      <c r="XR1" s="0"/>
+      <c r="XS1" s="0"/>
+      <c r="XT1" s="0"/>
+      <c r="XU1" s="0"/>
+      <c r="XV1" s="0"/>
+      <c r="XW1" s="0"/>
+      <c r="XX1" s="0"/>
+      <c r="XY1" s="0"/>
+      <c r="XZ1" s="0"/>
+      <c r="YA1" s="0"/>
+      <c r="YB1" s="0"/>
+      <c r="YC1" s="0"/>
+      <c r="YD1" s="0"/>
+      <c r="YE1" s="0"/>
+      <c r="YF1" s="0"/>
+      <c r="YG1" s="0"/>
+      <c r="YH1" s="0"/>
+      <c r="YI1" s="0"/>
+      <c r="YJ1" s="0"/>
+      <c r="YK1" s="0"/>
+      <c r="YL1" s="0"/>
+      <c r="YM1" s="0"/>
+      <c r="YN1" s="0"/>
+      <c r="YO1" s="0"/>
+      <c r="YP1" s="0"/>
+      <c r="YQ1" s="0"/>
+      <c r="YR1" s="0"/>
+      <c r="YS1" s="0"/>
+      <c r="YT1" s="0"/>
+      <c r="YU1" s="0"/>
+      <c r="YV1" s="0"/>
+      <c r="YW1" s="0"/>
+      <c r="YX1" s="0"/>
+      <c r="YY1" s="0"/>
+      <c r="YZ1" s="0"/>
+      <c r="ZA1" s="0"/>
+      <c r="ZB1" s="0"/>
+      <c r="ZC1" s="0"/>
+      <c r="ZD1" s="0"/>
+      <c r="ZE1" s="0"/>
+      <c r="ZF1" s="0"/>
+      <c r="ZG1" s="0"/>
+      <c r="ZH1" s="0"/>
+      <c r="ZI1" s="0"/>
+      <c r="ZJ1" s="0"/>
+      <c r="ZK1" s="0"/>
+      <c r="ZL1" s="0"/>
+      <c r="ZM1" s="0"/>
+      <c r="ZN1" s="0"/>
+      <c r="ZO1" s="0"/>
+      <c r="ZP1" s="0"/>
+      <c r="ZQ1" s="0"/>
+      <c r="ZR1" s="0"/>
+      <c r="ZS1" s="0"/>
+      <c r="ZT1" s="0"/>
+      <c r="ZU1" s="0"/>
+      <c r="ZV1" s="0"/>
+      <c r="ZW1" s="0"/>
+      <c r="ZX1" s="0"/>
+      <c r="ZY1" s="0"/>
+      <c r="ZZ1" s="0"/>
+      <c r="AAA1" s="0"/>
+      <c r="AAB1" s="0"/>
+      <c r="AAC1" s="0"/>
+      <c r="AAD1" s="0"/>
+      <c r="AAE1" s="0"/>
+      <c r="AAF1" s="0"/>
+      <c r="AAG1" s="0"/>
+      <c r="AAH1" s="0"/>
+      <c r="AAI1" s="0"/>
+      <c r="AAJ1" s="0"/>
+      <c r="AAK1" s="0"/>
+      <c r="AAL1" s="0"/>
+      <c r="AAM1" s="0"/>
+      <c r="AAN1" s="0"/>
+      <c r="AAO1" s="0"/>
+      <c r="AAP1" s="0"/>
+      <c r="AAQ1" s="0"/>
+      <c r="AAR1" s="0"/>
+      <c r="AAS1" s="0"/>
+      <c r="AAT1" s="0"/>
+      <c r="AAU1" s="0"/>
+      <c r="AAV1" s="0"/>
+      <c r="AAW1" s="0"/>
+      <c r="AAX1" s="0"/>
+      <c r="AAY1" s="0"/>
+      <c r="AAZ1" s="0"/>
+      <c r="ABA1" s="0"/>
+      <c r="ABB1" s="0"/>
+      <c r="ABC1" s="0"/>
+      <c r="ABD1" s="0"/>
+      <c r="ABE1" s="0"/>
+      <c r="ABF1" s="0"/>
+      <c r="ABG1" s="0"/>
+      <c r="ABH1" s="0"/>
+      <c r="ABI1" s="0"/>
+      <c r="ABJ1" s="0"/>
+      <c r="ABK1" s="0"/>
+      <c r="ABL1" s="0"/>
+      <c r="ABM1" s="0"/>
+      <c r="ABN1" s="0"/>
+      <c r="ABO1" s="0"/>
+      <c r="ABP1" s="0"/>
+      <c r="ABQ1" s="0"/>
+      <c r="ABR1" s="0"/>
+      <c r="ABS1" s="0"/>
+      <c r="ABT1" s="0"/>
+      <c r="ABU1" s="0"/>
+      <c r="ABV1" s="0"/>
+      <c r="ABW1" s="0"/>
+      <c r="ABX1" s="0"/>
+      <c r="ABY1" s="0"/>
+      <c r="ABZ1" s="0"/>
+      <c r="ACA1" s="0"/>
+      <c r="ACB1" s="0"/>
+      <c r="ACC1" s="0"/>
+      <c r="ACD1" s="0"/>
+      <c r="ACE1" s="0"/>
+      <c r="ACF1" s="0"/>
+      <c r="ACG1" s="0"/>
+      <c r="ACH1" s="0"/>
+      <c r="ACI1" s="0"/>
+      <c r="ACJ1" s="0"/>
+      <c r="ACK1" s="0"/>
+      <c r="ACL1" s="0"/>
+      <c r="ACM1" s="0"/>
+      <c r="ACN1" s="0"/>
+      <c r="ACO1" s="0"/>
+      <c r="ACP1" s="0"/>
+      <c r="ACQ1" s="0"/>
+      <c r="ACR1" s="0"/>
+      <c r="ACS1" s="0"/>
+      <c r="ACT1" s="0"/>
+      <c r="ACU1" s="0"/>
+      <c r="ACV1" s="0"/>
+      <c r="ACW1" s="0"/>
+      <c r="ACX1" s="0"/>
+      <c r="ACY1" s="0"/>
+      <c r="ACZ1" s="0"/>
+      <c r="ADA1" s="0"/>
+      <c r="ADB1" s="0"/>
+      <c r="ADC1" s="0"/>
+      <c r="ADD1" s="0"/>
+      <c r="ADE1" s="0"/>
+      <c r="ADF1" s="0"/>
+      <c r="ADG1" s="0"/>
+      <c r="ADH1" s="0"/>
+      <c r="ADI1" s="0"/>
+      <c r="ADJ1" s="0"/>
+      <c r="ADK1" s="0"/>
+      <c r="ADL1" s="0"/>
+      <c r="ADM1" s="0"/>
+      <c r="ADN1" s="0"/>
+      <c r="ADO1" s="0"/>
+      <c r="ADP1" s="0"/>
+      <c r="ADQ1" s="0"/>
+      <c r="ADR1" s="0"/>
+      <c r="ADS1" s="0"/>
+      <c r="ADT1" s="0"/>
+      <c r="ADU1" s="0"/>
+      <c r="ADV1" s="0"/>
+      <c r="ADW1" s="0"/>
+      <c r="ADX1" s="0"/>
+      <c r="ADY1" s="0"/>
+      <c r="ADZ1" s="0"/>
+      <c r="AEA1" s="0"/>
+      <c r="AEB1" s="0"/>
+      <c r="AEC1" s="0"/>
+      <c r="AED1" s="0"/>
+      <c r="AEE1" s="0"/>
+      <c r="AEF1" s="0"/>
+      <c r="AEG1" s="0"/>
+      <c r="AEH1" s="0"/>
+      <c r="AEI1" s="0"/>
+      <c r="AEJ1" s="0"/>
+      <c r="AEK1" s="0"/>
+      <c r="AEL1" s="0"/>
+      <c r="AEM1" s="0"/>
+      <c r="AEN1" s="0"/>
+      <c r="AEO1" s="0"/>
+      <c r="AEP1" s="0"/>
+      <c r="AEQ1" s="0"/>
+      <c r="AER1" s="0"/>
+      <c r="AES1" s="0"/>
+      <c r="AET1" s="0"/>
+      <c r="AEU1" s="0"/>
+      <c r="AEV1" s="0"/>
+      <c r="AEW1" s="0"/>
+      <c r="AEX1" s="0"/>
+      <c r="AEY1" s="0"/>
+      <c r="AEZ1" s="0"/>
+      <c r="AFA1" s="0"/>
+      <c r="AFB1" s="0"/>
+      <c r="AFC1" s="0"/>
+      <c r="AFD1" s="0"/>
+      <c r="AFE1" s="0"/>
+      <c r="AFF1" s="0"/>
+      <c r="AFG1" s="0"/>
+      <c r="AFH1" s="0"/>
+      <c r="AFI1" s="0"/>
+      <c r="AFJ1" s="0"/>
+      <c r="AFK1" s="0"/>
+      <c r="AFL1" s="0"/>
+      <c r="AFM1" s="0"/>
+      <c r="AFN1" s="0"/>
+      <c r="AFO1" s="0"/>
+      <c r="AFP1" s="0"/>
+      <c r="AFQ1" s="0"/>
+      <c r="AFR1" s="0"/>
+      <c r="AFS1" s="0"/>
+      <c r="AFT1" s="0"/>
+      <c r="AFU1" s="0"/>
+      <c r="AFV1" s="0"/>
+      <c r="AFW1" s="0"/>
+      <c r="AFX1" s="0"/>
+      <c r="AFY1" s="0"/>
+      <c r="AFZ1" s="0"/>
+      <c r="AGA1" s="0"/>
+      <c r="AGB1" s="0"/>
+      <c r="AGC1" s="0"/>
+      <c r="AGD1" s="0"/>
+      <c r="AGE1" s="0"/>
+      <c r="AGF1" s="0"/>
+      <c r="AGG1" s="0"/>
+      <c r="AGH1" s="0"/>
+      <c r="AGI1" s="0"/>
+      <c r="AGJ1" s="0"/>
+      <c r="AGK1" s="0"/>
+      <c r="AGL1" s="0"/>
+      <c r="AGM1" s="0"/>
+      <c r="AGN1" s="0"/>
+      <c r="AGO1" s="0"/>
+      <c r="AGP1" s="0"/>
+      <c r="AGQ1" s="0"/>
+      <c r="AGR1" s="0"/>
+      <c r="AGS1" s="0"/>
+      <c r="AGT1" s="0"/>
+      <c r="AGU1" s="0"/>
+      <c r="AGV1" s="0"/>
+      <c r="AGW1" s="0"/>
+      <c r="AGX1" s="0"/>
+      <c r="AGY1" s="0"/>
+      <c r="AGZ1" s="0"/>
+      <c r="AHA1" s="0"/>
+      <c r="AHB1" s="0"/>
+      <c r="AHC1" s="0"/>
+      <c r="AHD1" s="0"/>
+      <c r="AHE1" s="0"/>
+      <c r="AHF1" s="0"/>
+      <c r="AHG1" s="0"/>
+      <c r="AHH1" s="0"/>
+      <c r="AHI1" s="0"/>
+      <c r="AHJ1" s="0"/>
+      <c r="AHK1" s="0"/>
+      <c r="AHL1" s="0"/>
+      <c r="AHM1" s="0"/>
+      <c r="AHN1" s="0"/>
+      <c r="AHO1" s="0"/>
+      <c r="AHP1" s="0"/>
+      <c r="AHQ1" s="0"/>
+      <c r="AHR1" s="0"/>
+      <c r="AHS1" s="0"/>
+      <c r="AHT1" s="0"/>
+      <c r="AHU1" s="0"/>
+      <c r="AHV1" s="0"/>
+      <c r="AHW1" s="0"/>
+      <c r="AHX1" s="0"/>
+      <c r="AHY1" s="0"/>
+      <c r="AHZ1" s="0"/>
+      <c r="AIA1" s="0"/>
+      <c r="AIB1" s="0"/>
+      <c r="AIC1" s="0"/>
+      <c r="AID1" s="0"/>
+      <c r="AIE1" s="0"/>
+      <c r="AIF1" s="0"/>
+      <c r="AIG1" s="0"/>
+      <c r="AIH1" s="0"/>
+      <c r="AII1" s="0"/>
+      <c r="AIJ1" s="0"/>
+      <c r="AIK1" s="0"/>
+      <c r="AIL1" s="0"/>
+      <c r="AIM1" s="0"/>
+      <c r="AIN1" s="0"/>
+      <c r="AIO1" s="0"/>
+      <c r="AIP1" s="0"/>
+      <c r="AIQ1" s="0"/>
+      <c r="AIR1" s="0"/>
+      <c r="AIS1" s="0"/>
+      <c r="AIT1" s="0"/>
+      <c r="AIU1" s="0"/>
+      <c r="AIV1" s="0"/>
+      <c r="AIW1" s="0"/>
+      <c r="AIX1" s="0"/>
+      <c r="AIY1" s="0"/>
+      <c r="AIZ1" s="0"/>
+      <c r="AJA1" s="0"/>
+      <c r="AJB1" s="0"/>
+      <c r="AJC1" s="0"/>
+      <c r="AJD1" s="0"/>
+      <c r="AJE1" s="0"/>
+      <c r="AJF1" s="0"/>
+      <c r="AJG1" s="0"/>
+      <c r="AJH1" s="0"/>
+      <c r="AJI1" s="0"/>
+      <c r="AJJ1" s="0"/>
+      <c r="AJK1" s="0"/>
+      <c r="AJL1" s="0"/>
+      <c r="AJM1" s="0"/>
+      <c r="AJN1" s="0"/>
+      <c r="AJO1" s="0"/>
+      <c r="AJP1" s="0"/>
+      <c r="AJQ1" s="0"/>
+      <c r="AJR1" s="0"/>
+      <c r="AJS1" s="0"/>
+      <c r="AJT1" s="0"/>
+      <c r="AJU1" s="0"/>
+      <c r="AJV1" s="0"/>
+      <c r="AJW1" s="0"/>
+      <c r="AJX1" s="0"/>
+      <c r="AJY1" s="0"/>
+      <c r="AJZ1" s="0"/>
+      <c r="AKA1" s="0"/>
+      <c r="AKB1" s="0"/>
+      <c r="AKC1" s="0"/>
+      <c r="AKD1" s="0"/>
+      <c r="AKE1" s="0"/>
+      <c r="AKF1" s="0"/>
+      <c r="AKG1" s="0"/>
+      <c r="AKH1" s="0"/>
+      <c r="AKI1" s="0"/>
+      <c r="AKJ1" s="0"/>
+      <c r="AKK1" s="0"/>
+      <c r="AKL1" s="0"/>
+      <c r="AKM1" s="0"/>
+      <c r="AKN1" s="0"/>
+      <c r="AKO1" s="0"/>
+      <c r="AKP1" s="0"/>
+      <c r="AKQ1" s="0"/>
+      <c r="AKR1" s="0"/>
+      <c r="AKS1" s="0"/>
+      <c r="AKT1" s="0"/>
+      <c r="AKU1" s="0"/>
+      <c r="AKV1" s="0"/>
+      <c r="AKW1" s="0"/>
+      <c r="AKX1" s="0"/>
+      <c r="AKY1" s="0"/>
+      <c r="AKZ1" s="0"/>
+      <c r="ALA1" s="0"/>
+      <c r="ALB1" s="0"/>
+      <c r="ALC1" s="0"/>
+      <c r="ALD1" s="0"/>
+      <c r="ALE1" s="0"/>
+      <c r="ALF1" s="0"/>
+      <c r="ALG1" s="0"/>
+      <c r="ALH1" s="0"/>
+      <c r="ALI1" s="0"/>
+      <c r="ALJ1" s="0"/>
+      <c r="ALK1" s="0"/>
+      <c r="ALL1" s="0"/>
+      <c r="ALM1" s="0"/>
+      <c r="ALN1" s="0"/>
+      <c r="ALO1" s="0"/>
+      <c r="ALP1" s="0"/>
+      <c r="ALQ1" s="0"/>
+      <c r="ALR1" s="0"/>
+      <c r="ALS1" s="0"/>
+      <c r="ALT1" s="0"/>
+      <c r="ALU1" s="0"/>
+      <c r="ALV1" s="0"/>
+      <c r="ALW1" s="0"/>
+      <c r="ALX1" s="0"/>
+      <c r="ALY1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" s="28" t="n">
+      <c r="A2" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="36" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="n">
+      <c r="C2" s="37" t="n">
         <v>1000</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>91</v>
+      <c r="D2" s="37" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2576,10 +3765,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
+    <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A4"/>
@@ -2590,28 +3779,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="38" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
-        <v>92</v>
+      <c r="A2" s="39" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>93</v>
+      <c r="A3" s="39" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
-        <v>94</v>
+      <c r="A4" s="39" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2633,85 +3822,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <tabColor rgb="FFFFFFD7"/>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="25.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="28" t="n">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
-      <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
-      <formula1>ListReducers!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(Config): Add inline help + Improve UX
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -40,6 +40,19 @@
     <author> </author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Add reducers with the dropdown menu.
+Available reducers are listed in the tab `ListReducers`.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0">
       <text>
         <r>
@@ -47,9 +60,110 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Use 2 or 3 unless not human</t>
+          <t xml:space="preserve">The number of dimensions to reduce to.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <i val="true"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The list of band names to consider.
+Separate with `,`. If empty, all bands will be processed.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <i val="true"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Optional, Default</t>
+        </r>
+        <r>
+          <rPr>
+            <i val="true"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> all bands</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <i val="true"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The list of integration names to consider.
+Separate with `,`. If empty, all integrations will be processed.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <i val="true"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Optional, Default</t>
+        </r>
+        <r>
+          <rPr>
+            <i val="true"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> all integrations</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <i val="true"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The list of range names to consider.
+Separate with `,`. If empty, all ranges will be processed.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <i val="true"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Optional, Default</t>
+        </r>
+        <r>
+          <rPr>
+            <i val="true"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> all ranges</t>
         </r>
       </text>
     </comment>
@@ -57,22 +171,70 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Should end with `.h5`</t>
+          <t xml:space="preserve">Add autoclusters with the dropdown menu.
+Available autoclusters are listed in the tab `ListAutoclusters`.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The minimum size of clusters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The number of samples in the neighbourhood for a point to be considered a core point.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">A distance scaling parameter as used in robust single linkage.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">A distance threshold. Clusters below this value will be merged.</t>
         </r>
       </text>
     </comment>
@@ -93,9 +255,253 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Should start with a “/”</t>
+          <t xml:space="preserve">The file path, relative to your `audio_folder`.
+Should start with `/`.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The site name. Useful to gather multiple recordings together.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The file date (ISO 8601 format).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">One label property. Rename PROPERTY accordingly and add your label values.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The band name.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The low frequency in Hertz.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The high frequency in Hertz.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The integration name.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The number of seconds.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The range name.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The start date (ISO 8601 format).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The end date (ISO 8601 format).</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The trajectory name.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The start date (ISO 8601 format).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The end date (ISO 8601 format).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The label property to filter intervals from.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The specific label value for the above property to filter intervals from.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The rolling step.</t>
         </r>
       </text>
     </comment>
@@ -109,6 +515,19 @@
     <author> </author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Add extractors with the dropdown menu.
+Available extractors are listed in the tab `ListExtractors`.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0">
       <text>
         <r>
@@ -116,9 +535,8 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">milliseconds</t>
+          <t xml:space="preserve">The offset for each file in milliseconds.</t>
         </r>
       </text>
     </comment>
@@ -129,9 +547,44 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The step to iterate in milliseconds.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Whether the extracted data should be stored. (Not consumed by Visualisation Modules)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">milliseconds</t>
+          <t xml:space="preserve">Add digesters with the dropdown menu.
+Available digesters are listed in the tab `ListDigesters`.</t>
         </r>
       </text>
     </comment>
@@ -140,31 +593,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="144">
-  <si>
-    <t xml:space="preserve">Instructions</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
   <si>
     <t xml:space="preserve">SoundScapeExplorer
 Version 11</t>
   </si>
   <si>
-    <t xml:space="preserve">Fill the yellow tabs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Configure the blue tabs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Find more information in grey tabs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wiki: https://github.com/sound-scape-explorer/sound-scape-explorer/wiki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Settings</t>
+    <t xml:space="preserve">Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Fill the yellow tabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Configure the blue tabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read comments for each columns for Help.
+Find more information in grey tabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/sound-scape-explorer/sound-scape-explorer/wiki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Found a bug?
+Want to suggest a new feature?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/sound-scape-explorer/sound-scape-explorer/issues/new/choose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need help?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/sound-scape-explorer/sound-scape-explorer/discussions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sound-scape-explorer.github.io/sound-scape-explorer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
   </si>
   <si>
     <t xml:space="preserve">storage_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage.h5</t>
   </si>
   <si>
     <t xml:space="preserve">The path to your storage file. Absolute or relative to this file. Should end with `.h5`.
@@ -174,11 +656,17 @@
     <t xml:space="preserve">audio_path</t>
   </si>
   <si>
+    <t xml:space="preserve">C:\path\to\audio</t>
+  </si>
+  <si>
     <t xml:space="preserve">The path to your audio folder. Absolute or relative to this file.
 Examples: `audio`, `C:\path\to\audio`.</t>
   </si>
   <si>
     <t xml:space="preserve">audio_host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:5531</t>
   </si>
   <si>
     <t xml:space="preserve">The host name serving your audio files.
@@ -220,17 +708,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Optional, Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> None</t>
+      <t xml:space="preserve">Optional</t>
     </r>
   </si>
   <si>
@@ -257,17 +735,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Optional, Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 5</t>
+      <t xml:space="preserve">Optional</t>
     </r>
   </si>
   <si>
@@ -294,17 +762,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Optional, Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 50</t>
+      <t xml:space="preserve">Optional</t>
     </r>
   </si>
   <si>
@@ -331,334 +789,113 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Optional, Default</t>
+      <t xml:space="preserve">Optional</t>
     </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 42000</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Files</t>
   </si>
   <si>
     <t xml:space="preserve">file</t>
   </si>
   <si>
-    <t xml:space="preserve">The file path, relative to your `audio_folder`. Must start with `/`.</t>
+    <t xml:space="preserve">site</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">The file date (ISO 8601 format).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The site.</t>
-  </si>
-  <si>
     <t xml:space="preserve">label_PROPERTY</t>
   </si>
   <si>
-    <t xml:space="preserve">The label properties. Rename PROPERTY accordingly and add your label values.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bands</t>
-  </si>
-  <si>
     <t xml:space="preserve">band</t>
   </si>
   <si>
-    <t xml:space="preserve">The band name.</t>
-  </si>
-  <si>
     <t xml:space="preserve">low</t>
   </si>
   <si>
-    <t xml:space="preserve">The low frequency.</t>
-  </si>
-  <si>
     <t xml:space="preserve">high</t>
   </si>
   <si>
-    <t xml:space="preserve">The high frequency.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrations</t>
+    <t xml:space="preserve">human</t>
   </si>
   <si>
     <t xml:space="preserve">integration</t>
   </si>
   <si>
-    <t xml:space="preserve">The integration name.</t>
-  </si>
-  <si>
     <t xml:space="preserve">seconds</t>
   </si>
   <si>
-    <t xml:space="preserve">The number of seconds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ranges</t>
+    <t xml:space="preserve">i15</t>
   </si>
   <si>
     <t xml:space="preserve">range</t>
   </si>
   <si>
-    <t xml:space="preserve">The range name.</t>
-  </si>
-  <si>
     <t xml:space="preserve">start</t>
   </si>
   <si>
-    <t xml:space="preserve">The start date (ISO 8601 format).</t>
-  </si>
-  <si>
     <t xml:space="preserve">end</t>
   </si>
   <si>
-    <t xml:space="preserve">The end date (ISO 8601 format).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extractors</t>
+    <t xml:space="preserve">r2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trajectory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">step</t>
   </si>
   <si>
     <t xml:space="preserve">extractor</t>
   </si>
   <si>
-    <t xml:space="preserve">The extractor name.</t>
-  </si>
-  <si>
     <t xml:space="preserve">offset</t>
   </si>
   <si>
-    <t xml:space="preserve">The offset for each file in milliseconds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">step</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The step to iterate in milliseconds.</t>
-  </si>
-  <si>
     <t xml:space="preserve">persist</t>
   </si>
   <si>
-    <t xml:space="preserve">Whether the extracted data should be stored.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digesters</t>
+    <t xml:space="preserve">vgg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">digester</t>
   </si>
   <si>
-    <t xml:space="preserve">The digester name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autoclusters</t>
+    <t xml:space="preserve">silhouette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overlap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contingency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reducer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dimensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integrations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">umap</t>
   </si>
   <si>
     <t xml:space="preserve">autocluster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The autoclustering algorithm.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trajectories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trajectory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The trajectory name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reducers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reducer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The reducer name.
-See `HelpReducers` tab for available options.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dimensions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of dimensions to reduce to.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bands</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The list of band names to consider.
-Separate with `,`. If empty, all bands will be processed.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional, Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> all bands</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">integrations</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The list of integration names to consider.
-Separate with `,`. If empty, all integrations will be processed.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional, Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> all integrations</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ranges</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The list of range names to consider.
-Separate with `,`. If empty, all ranges will be processed.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional, Default</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> all ranges</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">setting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage.h5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\path\to\audio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://localhost:5531</t>
-  </si>
-  <si>
-    <t xml:space="preserve">human</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vgg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">silhouette</t>
-  </si>
-  <si>
-    <t xml:space="preserve">overlap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contingency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">umap</t>
   </si>
   <si>
     <t xml:space="preserve">min_cluster_size</t>
@@ -803,11 +1040,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -853,12 +1091,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -878,10 +1114,30 @@
       <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -899,14 +1155,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF111111"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFDEE6EF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFDEE6EF"/>
+        <fgColor rgb="FF111111"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -993,7 +1249,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1002,71 +1258,119 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1074,46 +1378,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1154,7 +1422,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1162,11 +1430,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1256,399 +1532,123 @@
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:AMI17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="B18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="90.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="72.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="AMI1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="3"/>
+      <c r="AMI2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="AMI3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="AMI4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="AMI5" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="7" t="s">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="8" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="B11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="9"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="9"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="9"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="9"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="9"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="9"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B47" s="9"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B50" s="9"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B51" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B55" s="9"/>
-    </row>
-    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A5"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:B5"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="Wiki: https://github.com/sound-scape-explorer/sound-scape-explorer/wiki"/>
+    <hyperlink ref="B11" r:id="rId1" display="https://github.com/sound-scape-explorer/sound-scape-explorer/wiki"/>
+    <hyperlink ref="B13" r:id="rId2" display="https://github.com/sound-scape-explorer/sound-scape-explorer/issues/new/choose"/>
+    <hyperlink ref="B15" r:id="rId3" display="https://github.com/sound-scape-explorer/sound-scape-explorer/discussions"/>
+    <hyperlink ref="B17" r:id="rId4" display="https://sound-scape-explorer.github.io/sound-scape-explorer"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1674,48 +1674,48 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="36" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="39" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="39" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="39" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>80</v>
+      <c r="A1" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>68</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="37" t="n">
+      <c r="A2" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="36" t="n">
+      <c r="A3" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="39" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1759,46 +1759,46 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="37" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="37" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="37" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="39" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>101</v>
+      <c r="A1" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>74</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="37" t="n">
+      <c r="A2" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="40" t="n">
         <v>50</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="37" t="n">
+      <c r="C2" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="37" t="n">
+      <c r="E2" s="40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1820,6 +1820,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1841,89 +1842,89 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="42" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>105</v>
+      <c r="A1" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="45" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>120</v>
+      <c r="B9" s="50" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B10" s="45" t="s">
-        <v>122</v>
+      <c r="A10" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1955,85 +1956,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="42" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="43" t="s">
+      <c r="A1" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="45" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>133</v>
+      <c r="B6" s="49" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>134</v>
+      <c r="A7" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>135</v>
+      <c r="A8" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>136</v>
+      <c r="A9" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="45"/>
+      <c r="B10" s="50"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2064,33 +2065,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>72</v>
+      <c r="A1" s="47" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>97</v>
+      <c r="A2" s="45" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>137</v>
+      <c r="A3" s="45" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>138</v>
+      <c r="A4" s="45" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>139</v>
+      <c r="A5" s="45" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2122,23 +2123,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>66</v>
+      <c r="A1" s="47" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>102</v>
+      <c r="A2" s="45" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>140</v>
+      <c r="A3" s="45" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2166,28 +2167,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>58</v>
+      <c r="A1" s="47" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>141</v>
+      <c r="A2" s="45" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>142</v>
+      <c r="A3" s="45" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>143</v>
+      <c r="A4" s="45" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2207,7 +2208,7 @@
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:AMJ10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2221,90 +2222,128 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
+    <row r="1" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="19" t="n">
+      <c r="B1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AMJ1" s="14"/>
+    </row>
+    <row r="2" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="AMJ2" s="14"/>
+    </row>
+    <row r="3" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AMJ3" s="14"/>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="AMJ4" s="14"/>
+    </row>
+    <row r="5" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="16" t="n">
         <v>44100</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="21" t="n">
+      <c r="C5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="AMJ5" s="14"/>
+    </row>
+    <row r="6" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="20" t="n">
         <v>36526</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="23" t="n">
+      <c r="C6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AMJ6" s="14"/>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="AMJ7" s="14"/>
+    </row>
+    <row r="8" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="22" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="23" t="n">
+      <c r="C8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AMJ8" s="14"/>
+    </row>
+    <row r="9" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="22" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="23" t="n">
+      <c r="C9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AMJ9" s="14"/>
+    </row>
+    <row r="10" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="22" t="n">
         <v>42000</v>
       </c>
+      <c r="C10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="AMJ10" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId2" display="http://localhost:5531"/>
+    <hyperlink ref="B4" r:id="rId1" display="http://localhost:5531"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2313,7 +2352,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2323,7 +2361,7 @@
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2335,71 +2373,65 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="27" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="11" style="28" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="35" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="5" style="27" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1003" min="29" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>28</v>
+      <c r="A1" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="str">
+      <c r="A2" s="30" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="21" t="n">
+      <c r="B2" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="32" t="n">
         <v>45089.8854166667</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>83</v>
+      <c r="D2" s="26" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="19"/>
+      <c r="C7" s="31"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2431,44 +2463,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="31" t="n">
+      <c r="A2" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="34" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="31" t="n">
+      <c r="C2" s="34" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2478,6 +2510,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2494,40 +2527,40 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="31" t="n">
+      <c r="A2" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="34" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="27"/>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="27"/>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="27"/>
+      <c r="B6" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2537,6 +2570,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2558,8 +2592,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="20.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -2568,29 +2602,29 @@
         <v>47</v>
       </c>
       <c r="B1" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="32" t="n">
+      <c r="A2" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="35" t="n">
         <v>44927</v>
       </c>
-      <c r="C2" s="32" t="n">
+      <c r="C2" s="35" t="n">
         <v>45292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="27"/>
+      <c r="C4" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2600,6 +2634,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2617,60 +2652,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="31" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="31" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="34" width="18.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B1" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>51</v>
-      </c>
       <c r="D1" s="29" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2686,6 +2721,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2703,25 +2739,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="37" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="37" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="39" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="15.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="5" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>60</v>
+      <c r="D1" s="41" t="s">
+        <v>57</v>
       </c>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
@@ -3734,17 +3770,17 @@
       <c r="ALY1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="36" t="n">
+      <c r="A2" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="37" t="n">
+      <c r="C2" s="40" t="n">
         <v>1000</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>93</v>
+      <c r="D2" s="40" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3779,28 +3815,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="42" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="42" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3821,5 +3857,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(Examples/DefaultConfig): Replace audio_path with relative
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -47,6 +47,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Add reducers with the dropdown menu.
 Available reducers are listed in the tab `ListReducers`.</t>
@@ -60,6 +61,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The number of dimensions to reduce to.</t>
         </r>
@@ -69,10 +71,10 @@
       <text>
         <r>
           <rPr>
-            <i val="true"/>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The list of band names to consider.
 Separate with `,`. If empty, all bands will be processed.
@@ -85,6 +87,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Optional, Default</t>
         </r>
@@ -94,6 +97,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> all bands</t>
         </r>
@@ -103,10 +107,10 @@
       <text>
         <r>
           <rPr>
-            <i val="true"/>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The list of integration names to consider.
 Separate with `,`. If empty, all integrations will be processed.
@@ -119,6 +123,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Optional, Default</t>
         </r>
@@ -128,6 +133,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> all integrations</t>
         </r>
@@ -137,10 +143,10 @@
       <text>
         <r>
           <rPr>
-            <i val="true"/>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The list of range names to consider.
 Separate with `,`. If empty, all ranges will be processed.
@@ -153,6 +159,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Optional, Default</t>
         </r>
@@ -162,6 +169,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> all ranges</t>
         </r>
@@ -184,6 +192,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Add autoclusters with the dropdown menu.
 Available autoclusters are listed in the tab `ListAutoclusters`.</t>
@@ -197,6 +206,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The minimum size of clusters.</t>
         </r>
@@ -209,6 +219,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The number of samples in the neighbourhood for a point to be considered a core point.</t>
         </r>
@@ -221,6 +232,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">A distance scaling parameter as used in robust single linkage.</t>
         </r>
@@ -233,6 +245,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">A distance threshold. Clusters below this value will be merged.</t>
         </r>
@@ -255,6 +268,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The file path, relative to your `audio_folder`.
 Should start with `/`.</t>
@@ -268,6 +282,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The site name. Useful to gather multiple recordings together.</t>
         </r>
@@ -280,6 +295,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The file date (ISO 8601 format).</t>
         </r>
@@ -292,6 +308,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">One label property. Rename PROPERTY accordingly and add your label values.</t>
         </r>
@@ -314,6 +331,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The band name.</t>
         </r>
@@ -326,6 +344,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The low frequency in Hertz.</t>
         </r>
@@ -338,6 +357,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The high frequency in Hertz.</t>
         </r>
@@ -360,6 +380,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The integration name.</t>
         </r>
@@ -372,6 +393,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The number of seconds.</t>
         </r>
@@ -394,6 +416,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The range name.</t>
         </r>
@@ -406,6 +429,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The start date (ISO 8601 format).</t>
         </r>
@@ -418,6 +442,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The end date (ISO 8601 format).</t>
         </r>
@@ -440,6 +465,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The trajectory name.</t>
         </r>
@@ -452,6 +478,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The start date (ISO 8601 format).</t>
         </r>
@@ -464,6 +491,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The end date (ISO 8601 format).</t>
         </r>
@@ -476,6 +504,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The label property to filter intervals from.</t>
         </r>
@@ -488,6 +517,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The specific label value for the above property to filter intervals from.</t>
         </r>
@@ -500,6 +530,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The rolling step.</t>
         </r>
@@ -522,6 +553,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Add extractors with the dropdown menu.
 Available extractors are listed in the tab `ListExtractors`.</t>
@@ -535,6 +567,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The offset for each file in milliseconds.</t>
         </r>
@@ -547,6 +580,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The step to iterate in milliseconds.</t>
         </r>
@@ -559,6 +593,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Whether the extracted data should be stored. (Not consumed by Visualisation Modules)</t>
         </r>
@@ -656,11 +691,11 @@
     <t xml:space="preserve">audio_path</t>
   </si>
   <si>
-    <t xml:space="preserve">C:\path\to\audio</t>
+    <t xml:space="preserve">audio</t>
   </si>
   <si>
     <t xml:space="preserve">The path to your audio folder. Absolute or relative to this file.
-Examples: `audio`, `C:\path\to\audio`.</t>
+Examples: `audio`, `C:\path\to\audio`, `/home/user/audio`</t>
   </si>
   <si>
     <t xml:space="preserve">audio_host</t>
@@ -1045,7 +1080,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1095,12 +1130,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1119,11 +1148,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
@@ -1131,13 +1155,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1254,203 +1271,203 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1527,7 +1544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -1547,95 +1564,95 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
-      <c r="AMI1" s="0"/>
+      <c r="AMI1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="AMI2" s="0"/>
+      <c r="B2" s="4"/>
+      <c r="AMI2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="AMI3" s="0"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="AMI3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="AMI4" s="0"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="AMI4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="AMI5" s="0"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="AMI5" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1652,7 +1669,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1661,7 +1678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
@@ -1698,7 +1715,7 @@
       <c r="E1" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="0"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
@@ -1721,18 +1738,18 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
       <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
       <formula1>ListReducers!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1742,7 +1759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
@@ -1783,7 +1800,7 @@
       <c r="E1" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="0"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
@@ -1804,18 +1821,18 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
       <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
       <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1825,7 +1842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -1930,7 +1947,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1939,7 +1956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2039,7 +2056,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2048,7 +2065,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2097,7 +2114,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2106,7 +2123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2145,7 +2162,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2154,7 +2171,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2194,7 +2211,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2203,7 +2220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2220,47 +2237,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AMJ1" s="14"/>
-    </row>
-    <row r="2" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="AMJ1" s="15"/>
+    </row>
+    <row r="2" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="AMJ2" s="14"/>
-    </row>
-    <row r="3" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+      <c r="AMJ2" s="15"/>
+    </row>
+    <row r="3" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AMJ3" s="14"/>
-    </row>
-    <row r="4" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
+      <c r="AMJ3" s="15"/>
+    </row>
+    <row r="4" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="19" t="s">
@@ -2269,22 +2286,22 @@
       <c r="C4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="AMJ4" s="14"/>
-    </row>
-    <row r="5" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
+      <c r="AMJ4" s="15"/>
+    </row>
+    <row r="5" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="16" t="n">
+      <c r="B5" s="17" t="n">
         <v>44100</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="AMJ5" s="14"/>
-    </row>
-    <row r="6" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="AMJ5" s="15"/>
+    </row>
+    <row r="6" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="20" t="n">
@@ -2293,9 +2310,9 @@
       <c r="C6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="AMJ6" s="14"/>
-    </row>
-    <row r="7" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMJ6" s="15"/>
+    </row>
+    <row r="7" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="21" t="s">
         <v>28</v>
       </c>
@@ -2303,9 +2320,9 @@
       <c r="C7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="AMJ7" s="14"/>
-    </row>
-    <row r="8" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMJ7" s="15"/>
+    </row>
+    <row r="8" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="21" t="s">
         <v>30</v>
       </c>
@@ -2315,9 +2332,9 @@
       <c r="C8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AMJ8" s="14"/>
-    </row>
-    <row r="9" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMJ8" s="15"/>
+    </row>
+    <row r="9" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
         <v>32</v>
       </c>
@@ -2327,9 +2344,9 @@
       <c r="C9" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AMJ9" s="14"/>
-    </row>
-    <row r="10" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMJ9" s="15"/>
+    </row>
+    <row r="10" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
         <v>34</v>
       </c>
@@ -2339,7 +2356,7 @@
       <c r="C10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AMJ10" s="14"/>
+      <c r="AMJ10" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2347,7 +2364,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2356,7 +2373,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2436,7 +2453,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2446,7 +2463,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2505,7 +2522,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2515,7 +2532,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2565,7 +2582,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2575,7 +2592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2629,7 +2646,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2639,7 +2656,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2709,14 +2726,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1001" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1001" type="list">
       <formula1>ListTrajectories!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2726,7 +2743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2739,7 +2756,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="10.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="39" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="15.45"/>
@@ -2759,1015 +2776,1015 @@
       <c r="D1" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
-      <c r="L1" s="0"/>
-      <c r="M1" s="0"/>
-      <c r="N1" s="0"/>
-      <c r="O1" s="0"/>
-      <c r="P1" s="0"/>
-      <c r="Q1" s="0"/>
-      <c r="R1" s="0"/>
-      <c r="S1" s="0"/>
-      <c r="T1" s="0"/>
-      <c r="U1" s="0"/>
-      <c r="V1" s="0"/>
-      <c r="W1" s="0"/>
-      <c r="X1" s="0"/>
-      <c r="Y1" s="0"/>
-      <c r="Z1" s="0"/>
-      <c r="AA1" s="0"/>
-      <c r="AB1" s="0"/>
-      <c r="AC1" s="0"/>
-      <c r="AD1" s="0"/>
-      <c r="AE1" s="0"/>
-      <c r="AF1" s="0"/>
-      <c r="AG1" s="0"/>
-      <c r="AH1" s="0"/>
-      <c r="AI1" s="0"/>
-      <c r="AJ1" s="0"/>
-      <c r="AK1" s="0"/>
-      <c r="AL1" s="0"/>
-      <c r="AM1" s="0"/>
-      <c r="AN1" s="0"/>
-      <c r="AO1" s="0"/>
-      <c r="AP1" s="0"/>
-      <c r="AQ1" s="0"/>
-      <c r="AR1" s="0"/>
-      <c r="AS1" s="0"/>
-      <c r="AT1" s="0"/>
-      <c r="AU1" s="0"/>
-      <c r="AV1" s="0"/>
-      <c r="AW1" s="0"/>
-      <c r="AX1" s="0"/>
-      <c r="AY1" s="0"/>
-      <c r="AZ1" s="0"/>
-      <c r="BA1" s="0"/>
-      <c r="BB1" s="0"/>
-      <c r="BC1" s="0"/>
-      <c r="BD1" s="0"/>
-      <c r="BE1" s="0"/>
-      <c r="BF1" s="0"/>
-      <c r="BG1" s="0"/>
-      <c r="BH1" s="0"/>
-      <c r="BI1" s="0"/>
-      <c r="BJ1" s="0"/>
-      <c r="BK1" s="0"/>
-      <c r="BL1" s="0"/>
-      <c r="BM1" s="0"/>
-      <c r="BN1" s="0"/>
-      <c r="BO1" s="0"/>
-      <c r="BP1" s="0"/>
-      <c r="BQ1" s="0"/>
-      <c r="BR1" s="0"/>
-      <c r="BS1" s="0"/>
-      <c r="BT1" s="0"/>
-      <c r="BU1" s="0"/>
-      <c r="BV1" s="0"/>
-      <c r="BW1" s="0"/>
-      <c r="BX1" s="0"/>
-      <c r="BY1" s="0"/>
-      <c r="BZ1" s="0"/>
-      <c r="CA1" s="0"/>
-      <c r="CB1" s="0"/>
-      <c r="CC1" s="0"/>
-      <c r="CD1" s="0"/>
-      <c r="CE1" s="0"/>
-      <c r="CF1" s="0"/>
-      <c r="CG1" s="0"/>
-      <c r="CH1" s="0"/>
-      <c r="CI1" s="0"/>
-      <c r="CJ1" s="0"/>
-      <c r="CK1" s="0"/>
-      <c r="CL1" s="0"/>
-      <c r="CM1" s="0"/>
-      <c r="CN1" s="0"/>
-      <c r="CO1" s="0"/>
-      <c r="CP1" s="0"/>
-      <c r="CQ1" s="0"/>
-      <c r="CR1" s="0"/>
-      <c r="CS1" s="0"/>
-      <c r="CT1" s="0"/>
-      <c r="CU1" s="0"/>
-      <c r="CV1" s="0"/>
-      <c r="CW1" s="0"/>
-      <c r="CX1" s="0"/>
-      <c r="CY1" s="0"/>
-      <c r="CZ1" s="0"/>
-      <c r="DA1" s="0"/>
-      <c r="DB1" s="0"/>
-      <c r="DC1" s="0"/>
-      <c r="DD1" s="0"/>
-      <c r="DE1" s="0"/>
-      <c r="DF1" s="0"/>
-      <c r="DG1" s="0"/>
-      <c r="DH1" s="0"/>
-      <c r="DI1" s="0"/>
-      <c r="DJ1" s="0"/>
-      <c r="DK1" s="0"/>
-      <c r="DL1" s="0"/>
-      <c r="DM1" s="0"/>
-      <c r="DN1" s="0"/>
-      <c r="DO1" s="0"/>
-      <c r="DP1" s="0"/>
-      <c r="DQ1" s="0"/>
-      <c r="DR1" s="0"/>
-      <c r="DS1" s="0"/>
-      <c r="DT1" s="0"/>
-      <c r="DU1" s="0"/>
-      <c r="DV1" s="0"/>
-      <c r="DW1" s="0"/>
-      <c r="DX1" s="0"/>
-      <c r="DY1" s="0"/>
-      <c r="DZ1" s="0"/>
-      <c r="EA1" s="0"/>
-      <c r="EB1" s="0"/>
-      <c r="EC1" s="0"/>
-      <c r="ED1" s="0"/>
-      <c r="EE1" s="0"/>
-      <c r="EF1" s="0"/>
-      <c r="EG1" s="0"/>
-      <c r="EH1" s="0"/>
-      <c r="EI1" s="0"/>
-      <c r="EJ1" s="0"/>
-      <c r="EK1" s="0"/>
-      <c r="EL1" s="0"/>
-      <c r="EM1" s="0"/>
-      <c r="EN1" s="0"/>
-      <c r="EO1" s="0"/>
-      <c r="EP1" s="0"/>
-      <c r="EQ1" s="0"/>
-      <c r="ER1" s="0"/>
-      <c r="ES1" s="0"/>
-      <c r="ET1" s="0"/>
-      <c r="EU1" s="0"/>
-      <c r="EV1" s="0"/>
-      <c r="EW1" s="0"/>
-      <c r="EX1" s="0"/>
-      <c r="EY1" s="0"/>
-      <c r="EZ1" s="0"/>
-      <c r="FA1" s="0"/>
-      <c r="FB1" s="0"/>
-      <c r="FC1" s="0"/>
-      <c r="FD1" s="0"/>
-      <c r="FE1" s="0"/>
-      <c r="FF1" s="0"/>
-      <c r="FG1" s="0"/>
-      <c r="FH1" s="0"/>
-      <c r="FI1" s="0"/>
-      <c r="FJ1" s="0"/>
-      <c r="FK1" s="0"/>
-      <c r="FL1" s="0"/>
-      <c r="FM1" s="0"/>
-      <c r="FN1" s="0"/>
-      <c r="FO1" s="0"/>
-      <c r="FP1" s="0"/>
-      <c r="FQ1" s="0"/>
-      <c r="FR1" s="0"/>
-      <c r="FS1" s="0"/>
-      <c r="FT1" s="0"/>
-      <c r="FU1" s="0"/>
-      <c r="FV1" s="0"/>
-      <c r="FW1" s="0"/>
-      <c r="FX1" s="0"/>
-      <c r="FY1" s="0"/>
-      <c r="FZ1" s="0"/>
-      <c r="GA1" s="0"/>
-      <c r="GB1" s="0"/>
-      <c r="GC1" s="0"/>
-      <c r="GD1" s="0"/>
-      <c r="GE1" s="0"/>
-      <c r="GF1" s="0"/>
-      <c r="GG1" s="0"/>
-      <c r="GH1" s="0"/>
-      <c r="GI1" s="0"/>
-      <c r="GJ1" s="0"/>
-      <c r="GK1" s="0"/>
-      <c r="GL1" s="0"/>
-      <c r="GM1" s="0"/>
-      <c r="GN1" s="0"/>
-      <c r="GO1" s="0"/>
-      <c r="GP1" s="0"/>
-      <c r="GQ1" s="0"/>
-      <c r="GR1" s="0"/>
-      <c r="GS1" s="0"/>
-      <c r="GT1" s="0"/>
-      <c r="GU1" s="0"/>
-      <c r="GV1" s="0"/>
-      <c r="GW1" s="0"/>
-      <c r="GX1" s="0"/>
-      <c r="GY1" s="0"/>
-      <c r="GZ1" s="0"/>
-      <c r="HA1" s="0"/>
-      <c r="HB1" s="0"/>
-      <c r="HC1" s="0"/>
-      <c r="HD1" s="0"/>
-      <c r="HE1" s="0"/>
-      <c r="HF1" s="0"/>
-      <c r="HG1" s="0"/>
-      <c r="HH1" s="0"/>
-      <c r="HI1" s="0"/>
-      <c r="HJ1" s="0"/>
-      <c r="HK1" s="0"/>
-      <c r="HL1" s="0"/>
-      <c r="HM1" s="0"/>
-      <c r="HN1" s="0"/>
-      <c r="HO1" s="0"/>
-      <c r="HP1" s="0"/>
-      <c r="HQ1" s="0"/>
-      <c r="HR1" s="0"/>
-      <c r="HS1" s="0"/>
-      <c r="HT1" s="0"/>
-      <c r="HU1" s="0"/>
-      <c r="HV1" s="0"/>
-      <c r="HW1" s="0"/>
-      <c r="HX1" s="0"/>
-      <c r="HY1" s="0"/>
-      <c r="HZ1" s="0"/>
-      <c r="IA1" s="0"/>
-      <c r="IB1" s="0"/>
-      <c r="IC1" s="0"/>
-      <c r="ID1" s="0"/>
-      <c r="IE1" s="0"/>
-      <c r="IF1" s="0"/>
-      <c r="IG1" s="0"/>
-      <c r="IH1" s="0"/>
-      <c r="II1" s="0"/>
-      <c r="IJ1" s="0"/>
-      <c r="IK1" s="0"/>
-      <c r="IL1" s="0"/>
-      <c r="IM1" s="0"/>
-      <c r="IN1" s="0"/>
-      <c r="IO1" s="0"/>
-      <c r="IP1" s="0"/>
-      <c r="IQ1" s="0"/>
-      <c r="IR1" s="0"/>
-      <c r="IS1" s="0"/>
-      <c r="IT1" s="0"/>
-      <c r="IU1" s="0"/>
-      <c r="IV1" s="0"/>
-      <c r="IW1" s="0"/>
-      <c r="IX1" s="0"/>
-      <c r="IY1" s="0"/>
-      <c r="IZ1" s="0"/>
-      <c r="JA1" s="0"/>
-      <c r="JB1" s="0"/>
-      <c r="JC1" s="0"/>
-      <c r="JD1" s="0"/>
-      <c r="JE1" s="0"/>
-      <c r="JF1" s="0"/>
-      <c r="JG1" s="0"/>
-      <c r="JH1" s="0"/>
-      <c r="JI1" s="0"/>
-      <c r="JJ1" s="0"/>
-      <c r="JK1" s="0"/>
-      <c r="JL1" s="0"/>
-      <c r="JM1" s="0"/>
-      <c r="JN1" s="0"/>
-      <c r="JO1" s="0"/>
-      <c r="JP1" s="0"/>
-      <c r="JQ1" s="0"/>
-      <c r="JR1" s="0"/>
-      <c r="JS1" s="0"/>
-      <c r="JT1" s="0"/>
-      <c r="JU1" s="0"/>
-      <c r="JV1" s="0"/>
-      <c r="JW1" s="0"/>
-      <c r="JX1" s="0"/>
-      <c r="JY1" s="0"/>
-      <c r="JZ1" s="0"/>
-      <c r="KA1" s="0"/>
-      <c r="KB1" s="0"/>
-      <c r="KC1" s="0"/>
-      <c r="KD1" s="0"/>
-      <c r="KE1" s="0"/>
-      <c r="KF1" s="0"/>
-      <c r="KG1" s="0"/>
-      <c r="KH1" s="0"/>
-      <c r="KI1" s="0"/>
-      <c r="KJ1" s="0"/>
-      <c r="KK1" s="0"/>
-      <c r="KL1" s="0"/>
-      <c r="KM1" s="0"/>
-      <c r="KN1" s="0"/>
-      <c r="KO1" s="0"/>
-      <c r="KP1" s="0"/>
-      <c r="KQ1" s="0"/>
-      <c r="KR1" s="0"/>
-      <c r="KS1" s="0"/>
-      <c r="KT1" s="0"/>
-      <c r="KU1" s="0"/>
-      <c r="KV1" s="0"/>
-      <c r="KW1" s="0"/>
-      <c r="KX1" s="0"/>
-      <c r="KY1" s="0"/>
-      <c r="KZ1" s="0"/>
-      <c r="LA1" s="0"/>
-      <c r="LB1" s="0"/>
-      <c r="LC1" s="0"/>
-      <c r="LD1" s="0"/>
-      <c r="LE1" s="0"/>
-      <c r="LF1" s="0"/>
-      <c r="LG1" s="0"/>
-      <c r="LH1" s="0"/>
-      <c r="LI1" s="0"/>
-      <c r="LJ1" s="0"/>
-      <c r="LK1" s="0"/>
-      <c r="LL1" s="0"/>
-      <c r="LM1" s="0"/>
-      <c r="LN1" s="0"/>
-      <c r="LO1" s="0"/>
-      <c r="LP1" s="0"/>
-      <c r="LQ1" s="0"/>
-      <c r="LR1" s="0"/>
-      <c r="LS1" s="0"/>
-      <c r="LT1" s="0"/>
-      <c r="LU1" s="0"/>
-      <c r="LV1" s="0"/>
-      <c r="LW1" s="0"/>
-      <c r="LX1" s="0"/>
-      <c r="LY1" s="0"/>
-      <c r="LZ1" s="0"/>
-      <c r="MA1" s="0"/>
-      <c r="MB1" s="0"/>
-      <c r="MC1" s="0"/>
-      <c r="MD1" s="0"/>
-      <c r="ME1" s="0"/>
-      <c r="MF1" s="0"/>
-      <c r="MG1" s="0"/>
-      <c r="MH1" s="0"/>
-      <c r="MI1" s="0"/>
-      <c r="MJ1" s="0"/>
-      <c r="MK1" s="0"/>
-      <c r="ML1" s="0"/>
-      <c r="MM1" s="0"/>
-      <c r="MN1" s="0"/>
-      <c r="MO1" s="0"/>
-      <c r="MP1" s="0"/>
-      <c r="MQ1" s="0"/>
-      <c r="MR1" s="0"/>
-      <c r="MS1" s="0"/>
-      <c r="MT1" s="0"/>
-      <c r="MU1" s="0"/>
-      <c r="MV1" s="0"/>
-      <c r="MW1" s="0"/>
-      <c r="MX1" s="0"/>
-      <c r="MY1" s="0"/>
-      <c r="MZ1" s="0"/>
-      <c r="NA1" s="0"/>
-      <c r="NB1" s="0"/>
-      <c r="NC1" s="0"/>
-      <c r="ND1" s="0"/>
-      <c r="NE1" s="0"/>
-      <c r="NF1" s="0"/>
-      <c r="NG1" s="0"/>
-      <c r="NH1" s="0"/>
-      <c r="NI1" s="0"/>
-      <c r="NJ1" s="0"/>
-      <c r="NK1" s="0"/>
-      <c r="NL1" s="0"/>
-      <c r="NM1" s="0"/>
-      <c r="NN1" s="0"/>
-      <c r="NO1" s="0"/>
-      <c r="NP1" s="0"/>
-      <c r="NQ1" s="0"/>
-      <c r="NR1" s="0"/>
-      <c r="NS1" s="0"/>
-      <c r="NT1" s="0"/>
-      <c r="NU1" s="0"/>
-      <c r="NV1" s="0"/>
-      <c r="NW1" s="0"/>
-      <c r="NX1" s="0"/>
-      <c r="NY1" s="0"/>
-      <c r="NZ1" s="0"/>
-      <c r="OA1" s="0"/>
-      <c r="OB1" s="0"/>
-      <c r="OC1" s="0"/>
-      <c r="OD1" s="0"/>
-      <c r="OE1" s="0"/>
-      <c r="OF1" s="0"/>
-      <c r="OG1" s="0"/>
-      <c r="OH1" s="0"/>
-      <c r="OI1" s="0"/>
-      <c r="OJ1" s="0"/>
-      <c r="OK1" s="0"/>
-      <c r="OL1" s="0"/>
-      <c r="OM1" s="0"/>
-      <c r="ON1" s="0"/>
-      <c r="OO1" s="0"/>
-      <c r="OP1" s="0"/>
-      <c r="OQ1" s="0"/>
-      <c r="OR1" s="0"/>
-      <c r="OS1" s="0"/>
-      <c r="OT1" s="0"/>
-      <c r="OU1" s="0"/>
-      <c r="OV1" s="0"/>
-      <c r="OW1" s="0"/>
-      <c r="OX1" s="0"/>
-      <c r="OY1" s="0"/>
-      <c r="OZ1" s="0"/>
-      <c r="PA1" s="0"/>
-      <c r="PB1" s="0"/>
-      <c r="PC1" s="0"/>
-      <c r="PD1" s="0"/>
-      <c r="PE1" s="0"/>
-      <c r="PF1" s="0"/>
-      <c r="PG1" s="0"/>
-      <c r="PH1" s="0"/>
-      <c r="PI1" s="0"/>
-      <c r="PJ1" s="0"/>
-      <c r="PK1" s="0"/>
-      <c r="PL1" s="0"/>
-      <c r="PM1" s="0"/>
-      <c r="PN1" s="0"/>
-      <c r="PO1" s="0"/>
-      <c r="PP1" s="0"/>
-      <c r="PQ1" s="0"/>
-      <c r="PR1" s="0"/>
-      <c r="PS1" s="0"/>
-      <c r="PT1" s="0"/>
-      <c r="PU1" s="0"/>
-      <c r="PV1" s="0"/>
-      <c r="PW1" s="0"/>
-      <c r="PX1" s="0"/>
-      <c r="PY1" s="0"/>
-      <c r="PZ1" s="0"/>
-      <c r="QA1" s="0"/>
-      <c r="QB1" s="0"/>
-      <c r="QC1" s="0"/>
-      <c r="QD1" s="0"/>
-      <c r="QE1" s="0"/>
-      <c r="QF1" s="0"/>
-      <c r="QG1" s="0"/>
-      <c r="QH1" s="0"/>
-      <c r="QI1" s="0"/>
-      <c r="QJ1" s="0"/>
-      <c r="QK1" s="0"/>
-      <c r="QL1" s="0"/>
-      <c r="QM1" s="0"/>
-      <c r="QN1" s="0"/>
-      <c r="QO1" s="0"/>
-      <c r="QP1" s="0"/>
-      <c r="QQ1" s="0"/>
-      <c r="QR1" s="0"/>
-      <c r="QS1" s="0"/>
-      <c r="QT1" s="0"/>
-      <c r="QU1" s="0"/>
-      <c r="QV1" s="0"/>
-      <c r="QW1" s="0"/>
-      <c r="QX1" s="0"/>
-      <c r="QY1" s="0"/>
-      <c r="QZ1" s="0"/>
-      <c r="RA1" s="0"/>
-      <c r="RB1" s="0"/>
-      <c r="RC1" s="0"/>
-      <c r="RD1" s="0"/>
-      <c r="RE1" s="0"/>
-      <c r="RF1" s="0"/>
-      <c r="RG1" s="0"/>
-      <c r="RH1" s="0"/>
-      <c r="RI1" s="0"/>
-      <c r="RJ1" s="0"/>
-      <c r="RK1" s="0"/>
-      <c r="RL1" s="0"/>
-      <c r="RM1" s="0"/>
-      <c r="RN1" s="0"/>
-      <c r="RO1" s="0"/>
-      <c r="RP1" s="0"/>
-      <c r="RQ1" s="0"/>
-      <c r="RR1" s="0"/>
-      <c r="RS1" s="0"/>
-      <c r="RT1" s="0"/>
-      <c r="RU1" s="0"/>
-      <c r="RV1" s="0"/>
-      <c r="RW1" s="0"/>
-      <c r="RX1" s="0"/>
-      <c r="RY1" s="0"/>
-      <c r="RZ1" s="0"/>
-      <c r="SA1" s="0"/>
-      <c r="SB1" s="0"/>
-      <c r="SC1" s="0"/>
-      <c r="SD1" s="0"/>
-      <c r="SE1" s="0"/>
-      <c r="SF1" s="0"/>
-      <c r="SG1" s="0"/>
-      <c r="SH1" s="0"/>
-      <c r="SI1" s="0"/>
-      <c r="SJ1" s="0"/>
-      <c r="SK1" s="0"/>
-      <c r="SL1" s="0"/>
-      <c r="SM1" s="0"/>
-      <c r="SN1" s="0"/>
-      <c r="SO1" s="0"/>
-      <c r="SP1" s="0"/>
-      <c r="SQ1" s="0"/>
-      <c r="SR1" s="0"/>
-      <c r="SS1" s="0"/>
-      <c r="ST1" s="0"/>
-      <c r="SU1" s="0"/>
-      <c r="SV1" s="0"/>
-      <c r="SW1" s="0"/>
-      <c r="SX1" s="0"/>
-      <c r="SY1" s="0"/>
-      <c r="SZ1" s="0"/>
-      <c r="TA1" s="0"/>
-      <c r="TB1" s="0"/>
-      <c r="TC1" s="0"/>
-      <c r="TD1" s="0"/>
-      <c r="TE1" s="0"/>
-      <c r="TF1" s="0"/>
-      <c r="TG1" s="0"/>
-      <c r="TH1" s="0"/>
-      <c r="TI1" s="0"/>
-      <c r="TJ1" s="0"/>
-      <c r="TK1" s="0"/>
-      <c r="TL1" s="0"/>
-      <c r="TM1" s="0"/>
-      <c r="TN1" s="0"/>
-      <c r="TO1" s="0"/>
-      <c r="TP1" s="0"/>
-      <c r="TQ1" s="0"/>
-      <c r="TR1" s="0"/>
-      <c r="TS1" s="0"/>
-      <c r="TT1" s="0"/>
-      <c r="TU1" s="0"/>
-      <c r="TV1" s="0"/>
-      <c r="TW1" s="0"/>
-      <c r="TX1" s="0"/>
-      <c r="TY1" s="0"/>
-      <c r="TZ1" s="0"/>
-      <c r="UA1" s="0"/>
-      <c r="UB1" s="0"/>
-      <c r="UC1" s="0"/>
-      <c r="UD1" s="0"/>
-      <c r="UE1" s="0"/>
-      <c r="UF1" s="0"/>
-      <c r="UG1" s="0"/>
-      <c r="UH1" s="0"/>
-      <c r="UI1" s="0"/>
-      <c r="UJ1" s="0"/>
-      <c r="UK1" s="0"/>
-      <c r="UL1" s="0"/>
-      <c r="UM1" s="0"/>
-      <c r="UN1" s="0"/>
-      <c r="UO1" s="0"/>
-      <c r="UP1" s="0"/>
-      <c r="UQ1" s="0"/>
-      <c r="UR1" s="0"/>
-      <c r="US1" s="0"/>
-      <c r="UT1" s="0"/>
-      <c r="UU1" s="0"/>
-      <c r="UV1" s="0"/>
-      <c r="UW1" s="0"/>
-      <c r="UX1" s="0"/>
-      <c r="UY1" s="0"/>
-      <c r="UZ1" s="0"/>
-      <c r="VA1" s="0"/>
-      <c r="VB1" s="0"/>
-      <c r="VC1" s="0"/>
-      <c r="VD1" s="0"/>
-      <c r="VE1" s="0"/>
-      <c r="VF1" s="0"/>
-      <c r="VG1" s="0"/>
-      <c r="VH1" s="0"/>
-      <c r="VI1" s="0"/>
-      <c r="VJ1" s="0"/>
-      <c r="VK1" s="0"/>
-      <c r="VL1" s="0"/>
-      <c r="VM1" s="0"/>
-      <c r="VN1" s="0"/>
-      <c r="VO1" s="0"/>
-      <c r="VP1" s="0"/>
-      <c r="VQ1" s="0"/>
-      <c r="VR1" s="0"/>
-      <c r="VS1" s="0"/>
-      <c r="VT1" s="0"/>
-      <c r="VU1" s="0"/>
-      <c r="VV1" s="0"/>
-      <c r="VW1" s="0"/>
-      <c r="VX1" s="0"/>
-      <c r="VY1" s="0"/>
-      <c r="VZ1" s="0"/>
-      <c r="WA1" s="0"/>
-      <c r="WB1" s="0"/>
-      <c r="WC1" s="0"/>
-      <c r="WD1" s="0"/>
-      <c r="WE1" s="0"/>
-      <c r="WF1" s="0"/>
-      <c r="WG1" s="0"/>
-      <c r="WH1" s="0"/>
-      <c r="WI1" s="0"/>
-      <c r="WJ1" s="0"/>
-      <c r="WK1" s="0"/>
-      <c r="WL1" s="0"/>
-      <c r="WM1" s="0"/>
-      <c r="WN1" s="0"/>
-      <c r="WO1" s="0"/>
-      <c r="WP1" s="0"/>
-      <c r="WQ1" s="0"/>
-      <c r="WR1" s="0"/>
-      <c r="WS1" s="0"/>
-      <c r="WT1" s="0"/>
-      <c r="WU1" s="0"/>
-      <c r="WV1" s="0"/>
-      <c r="WW1" s="0"/>
-      <c r="WX1" s="0"/>
-      <c r="WY1" s="0"/>
-      <c r="WZ1" s="0"/>
-      <c r="XA1" s="0"/>
-      <c r="XB1" s="0"/>
-      <c r="XC1" s="0"/>
-      <c r="XD1" s="0"/>
-      <c r="XE1" s="0"/>
-      <c r="XF1" s="0"/>
-      <c r="XG1" s="0"/>
-      <c r="XH1" s="0"/>
-      <c r="XI1" s="0"/>
-      <c r="XJ1" s="0"/>
-      <c r="XK1" s="0"/>
-      <c r="XL1" s="0"/>
-      <c r="XM1" s="0"/>
-      <c r="XN1" s="0"/>
-      <c r="XO1" s="0"/>
-      <c r="XP1" s="0"/>
-      <c r="XQ1" s="0"/>
-      <c r="XR1" s="0"/>
-      <c r="XS1" s="0"/>
-      <c r="XT1" s="0"/>
-      <c r="XU1" s="0"/>
-      <c r="XV1" s="0"/>
-      <c r="XW1" s="0"/>
-      <c r="XX1" s="0"/>
-      <c r="XY1" s="0"/>
-      <c r="XZ1" s="0"/>
-      <c r="YA1" s="0"/>
-      <c r="YB1" s="0"/>
-      <c r="YC1" s="0"/>
-      <c r="YD1" s="0"/>
-      <c r="YE1" s="0"/>
-      <c r="YF1" s="0"/>
-      <c r="YG1" s="0"/>
-      <c r="YH1" s="0"/>
-      <c r="YI1" s="0"/>
-      <c r="YJ1" s="0"/>
-      <c r="YK1" s="0"/>
-      <c r="YL1" s="0"/>
-      <c r="YM1" s="0"/>
-      <c r="YN1" s="0"/>
-      <c r="YO1" s="0"/>
-      <c r="YP1" s="0"/>
-      <c r="YQ1" s="0"/>
-      <c r="YR1" s="0"/>
-      <c r="YS1" s="0"/>
-      <c r="YT1" s="0"/>
-      <c r="YU1" s="0"/>
-      <c r="YV1" s="0"/>
-      <c r="YW1" s="0"/>
-      <c r="YX1" s="0"/>
-      <c r="YY1" s="0"/>
-      <c r="YZ1" s="0"/>
-      <c r="ZA1" s="0"/>
-      <c r="ZB1" s="0"/>
-      <c r="ZC1" s="0"/>
-      <c r="ZD1" s="0"/>
-      <c r="ZE1" s="0"/>
-      <c r="ZF1" s="0"/>
-      <c r="ZG1" s="0"/>
-      <c r="ZH1" s="0"/>
-      <c r="ZI1" s="0"/>
-      <c r="ZJ1" s="0"/>
-      <c r="ZK1" s="0"/>
-      <c r="ZL1" s="0"/>
-      <c r="ZM1" s="0"/>
-      <c r="ZN1" s="0"/>
-      <c r="ZO1" s="0"/>
-      <c r="ZP1" s="0"/>
-      <c r="ZQ1" s="0"/>
-      <c r="ZR1" s="0"/>
-      <c r="ZS1" s="0"/>
-      <c r="ZT1" s="0"/>
-      <c r="ZU1" s="0"/>
-      <c r="ZV1" s="0"/>
-      <c r="ZW1" s="0"/>
-      <c r="ZX1" s="0"/>
-      <c r="ZY1" s="0"/>
-      <c r="ZZ1" s="0"/>
-      <c r="AAA1" s="0"/>
-      <c r="AAB1" s="0"/>
-      <c r="AAC1" s="0"/>
-      <c r="AAD1" s="0"/>
-      <c r="AAE1" s="0"/>
-      <c r="AAF1" s="0"/>
-      <c r="AAG1" s="0"/>
-      <c r="AAH1" s="0"/>
-      <c r="AAI1" s="0"/>
-      <c r="AAJ1" s="0"/>
-      <c r="AAK1" s="0"/>
-      <c r="AAL1" s="0"/>
-      <c r="AAM1" s="0"/>
-      <c r="AAN1" s="0"/>
-      <c r="AAO1" s="0"/>
-      <c r="AAP1" s="0"/>
-      <c r="AAQ1" s="0"/>
-      <c r="AAR1" s="0"/>
-      <c r="AAS1" s="0"/>
-      <c r="AAT1" s="0"/>
-      <c r="AAU1" s="0"/>
-      <c r="AAV1" s="0"/>
-      <c r="AAW1" s="0"/>
-      <c r="AAX1" s="0"/>
-      <c r="AAY1" s="0"/>
-      <c r="AAZ1" s="0"/>
-      <c r="ABA1" s="0"/>
-      <c r="ABB1" s="0"/>
-      <c r="ABC1" s="0"/>
-      <c r="ABD1" s="0"/>
-      <c r="ABE1" s="0"/>
-      <c r="ABF1" s="0"/>
-      <c r="ABG1" s="0"/>
-      <c r="ABH1" s="0"/>
-      <c r="ABI1" s="0"/>
-      <c r="ABJ1" s="0"/>
-      <c r="ABK1" s="0"/>
-      <c r="ABL1" s="0"/>
-      <c r="ABM1" s="0"/>
-      <c r="ABN1" s="0"/>
-      <c r="ABO1" s="0"/>
-      <c r="ABP1" s="0"/>
-      <c r="ABQ1" s="0"/>
-      <c r="ABR1" s="0"/>
-      <c r="ABS1" s="0"/>
-      <c r="ABT1" s="0"/>
-      <c r="ABU1" s="0"/>
-      <c r="ABV1" s="0"/>
-      <c r="ABW1" s="0"/>
-      <c r="ABX1" s="0"/>
-      <c r="ABY1" s="0"/>
-      <c r="ABZ1" s="0"/>
-      <c r="ACA1" s="0"/>
-      <c r="ACB1" s="0"/>
-      <c r="ACC1" s="0"/>
-      <c r="ACD1" s="0"/>
-      <c r="ACE1" s="0"/>
-      <c r="ACF1" s="0"/>
-      <c r="ACG1" s="0"/>
-      <c r="ACH1" s="0"/>
-      <c r="ACI1" s="0"/>
-      <c r="ACJ1" s="0"/>
-      <c r="ACK1" s="0"/>
-      <c r="ACL1" s="0"/>
-      <c r="ACM1" s="0"/>
-      <c r="ACN1" s="0"/>
-      <c r="ACO1" s="0"/>
-      <c r="ACP1" s="0"/>
-      <c r="ACQ1" s="0"/>
-      <c r="ACR1" s="0"/>
-      <c r="ACS1" s="0"/>
-      <c r="ACT1" s="0"/>
-      <c r="ACU1" s="0"/>
-      <c r="ACV1" s="0"/>
-      <c r="ACW1" s="0"/>
-      <c r="ACX1" s="0"/>
-      <c r="ACY1" s="0"/>
-      <c r="ACZ1" s="0"/>
-      <c r="ADA1" s="0"/>
-      <c r="ADB1" s="0"/>
-      <c r="ADC1" s="0"/>
-      <c r="ADD1" s="0"/>
-      <c r="ADE1" s="0"/>
-      <c r="ADF1" s="0"/>
-      <c r="ADG1" s="0"/>
-      <c r="ADH1" s="0"/>
-      <c r="ADI1" s="0"/>
-      <c r="ADJ1" s="0"/>
-      <c r="ADK1" s="0"/>
-      <c r="ADL1" s="0"/>
-      <c r="ADM1" s="0"/>
-      <c r="ADN1" s="0"/>
-      <c r="ADO1" s="0"/>
-      <c r="ADP1" s="0"/>
-      <c r="ADQ1" s="0"/>
-      <c r="ADR1" s="0"/>
-      <c r="ADS1" s="0"/>
-      <c r="ADT1" s="0"/>
-      <c r="ADU1" s="0"/>
-      <c r="ADV1" s="0"/>
-      <c r="ADW1" s="0"/>
-      <c r="ADX1" s="0"/>
-      <c r="ADY1" s="0"/>
-      <c r="ADZ1" s="0"/>
-      <c r="AEA1" s="0"/>
-      <c r="AEB1" s="0"/>
-      <c r="AEC1" s="0"/>
-      <c r="AED1" s="0"/>
-      <c r="AEE1" s="0"/>
-      <c r="AEF1" s="0"/>
-      <c r="AEG1" s="0"/>
-      <c r="AEH1" s="0"/>
-      <c r="AEI1" s="0"/>
-      <c r="AEJ1" s="0"/>
-      <c r="AEK1" s="0"/>
-      <c r="AEL1" s="0"/>
-      <c r="AEM1" s="0"/>
-      <c r="AEN1" s="0"/>
-      <c r="AEO1" s="0"/>
-      <c r="AEP1" s="0"/>
-      <c r="AEQ1" s="0"/>
-      <c r="AER1" s="0"/>
-      <c r="AES1" s="0"/>
-      <c r="AET1" s="0"/>
-      <c r="AEU1" s="0"/>
-      <c r="AEV1" s="0"/>
-      <c r="AEW1" s="0"/>
-      <c r="AEX1" s="0"/>
-      <c r="AEY1" s="0"/>
-      <c r="AEZ1" s="0"/>
-      <c r="AFA1" s="0"/>
-      <c r="AFB1" s="0"/>
-      <c r="AFC1" s="0"/>
-      <c r="AFD1" s="0"/>
-      <c r="AFE1" s="0"/>
-      <c r="AFF1" s="0"/>
-      <c r="AFG1" s="0"/>
-      <c r="AFH1" s="0"/>
-      <c r="AFI1" s="0"/>
-      <c r="AFJ1" s="0"/>
-      <c r="AFK1" s="0"/>
-      <c r="AFL1" s="0"/>
-      <c r="AFM1" s="0"/>
-      <c r="AFN1" s="0"/>
-      <c r="AFO1" s="0"/>
-      <c r="AFP1" s="0"/>
-      <c r="AFQ1" s="0"/>
-      <c r="AFR1" s="0"/>
-      <c r="AFS1" s="0"/>
-      <c r="AFT1" s="0"/>
-      <c r="AFU1" s="0"/>
-      <c r="AFV1" s="0"/>
-      <c r="AFW1" s="0"/>
-      <c r="AFX1" s="0"/>
-      <c r="AFY1" s="0"/>
-      <c r="AFZ1" s="0"/>
-      <c r="AGA1" s="0"/>
-      <c r="AGB1" s="0"/>
-      <c r="AGC1" s="0"/>
-      <c r="AGD1" s="0"/>
-      <c r="AGE1" s="0"/>
-      <c r="AGF1" s="0"/>
-      <c r="AGG1" s="0"/>
-      <c r="AGH1" s="0"/>
-      <c r="AGI1" s="0"/>
-      <c r="AGJ1" s="0"/>
-      <c r="AGK1" s="0"/>
-      <c r="AGL1" s="0"/>
-      <c r="AGM1" s="0"/>
-      <c r="AGN1" s="0"/>
-      <c r="AGO1" s="0"/>
-      <c r="AGP1" s="0"/>
-      <c r="AGQ1" s="0"/>
-      <c r="AGR1" s="0"/>
-      <c r="AGS1" s="0"/>
-      <c r="AGT1" s="0"/>
-      <c r="AGU1" s="0"/>
-      <c r="AGV1" s="0"/>
-      <c r="AGW1" s="0"/>
-      <c r="AGX1" s="0"/>
-      <c r="AGY1" s="0"/>
-      <c r="AGZ1" s="0"/>
-      <c r="AHA1" s="0"/>
-      <c r="AHB1" s="0"/>
-      <c r="AHC1" s="0"/>
-      <c r="AHD1" s="0"/>
-      <c r="AHE1" s="0"/>
-      <c r="AHF1" s="0"/>
-      <c r="AHG1" s="0"/>
-      <c r="AHH1" s="0"/>
-      <c r="AHI1" s="0"/>
-      <c r="AHJ1" s="0"/>
-      <c r="AHK1" s="0"/>
-      <c r="AHL1" s="0"/>
-      <c r="AHM1" s="0"/>
-      <c r="AHN1" s="0"/>
-      <c r="AHO1" s="0"/>
-      <c r="AHP1" s="0"/>
-      <c r="AHQ1" s="0"/>
-      <c r="AHR1" s="0"/>
-      <c r="AHS1" s="0"/>
-      <c r="AHT1" s="0"/>
-      <c r="AHU1" s="0"/>
-      <c r="AHV1" s="0"/>
-      <c r="AHW1" s="0"/>
-      <c r="AHX1" s="0"/>
-      <c r="AHY1" s="0"/>
-      <c r="AHZ1" s="0"/>
-      <c r="AIA1" s="0"/>
-      <c r="AIB1" s="0"/>
-      <c r="AIC1" s="0"/>
-      <c r="AID1" s="0"/>
-      <c r="AIE1" s="0"/>
-      <c r="AIF1" s="0"/>
-      <c r="AIG1" s="0"/>
-      <c r="AIH1" s="0"/>
-      <c r="AII1" s="0"/>
-      <c r="AIJ1" s="0"/>
-      <c r="AIK1" s="0"/>
-      <c r="AIL1" s="0"/>
-      <c r="AIM1" s="0"/>
-      <c r="AIN1" s="0"/>
-      <c r="AIO1" s="0"/>
-      <c r="AIP1" s="0"/>
-      <c r="AIQ1" s="0"/>
-      <c r="AIR1" s="0"/>
-      <c r="AIS1" s="0"/>
-      <c r="AIT1" s="0"/>
-      <c r="AIU1" s="0"/>
-      <c r="AIV1" s="0"/>
-      <c r="AIW1" s="0"/>
-      <c r="AIX1" s="0"/>
-      <c r="AIY1" s="0"/>
-      <c r="AIZ1" s="0"/>
-      <c r="AJA1" s="0"/>
-      <c r="AJB1" s="0"/>
-      <c r="AJC1" s="0"/>
-      <c r="AJD1" s="0"/>
-      <c r="AJE1" s="0"/>
-      <c r="AJF1" s="0"/>
-      <c r="AJG1" s="0"/>
-      <c r="AJH1" s="0"/>
-      <c r="AJI1" s="0"/>
-      <c r="AJJ1" s="0"/>
-      <c r="AJK1" s="0"/>
-      <c r="AJL1" s="0"/>
-      <c r="AJM1" s="0"/>
-      <c r="AJN1" s="0"/>
-      <c r="AJO1" s="0"/>
-      <c r="AJP1" s="0"/>
-      <c r="AJQ1" s="0"/>
-      <c r="AJR1" s="0"/>
-      <c r="AJS1" s="0"/>
-      <c r="AJT1" s="0"/>
-      <c r="AJU1" s="0"/>
-      <c r="AJV1" s="0"/>
-      <c r="AJW1" s="0"/>
-      <c r="AJX1" s="0"/>
-      <c r="AJY1" s="0"/>
-      <c r="AJZ1" s="0"/>
-      <c r="AKA1" s="0"/>
-      <c r="AKB1" s="0"/>
-      <c r="AKC1" s="0"/>
-      <c r="AKD1" s="0"/>
-      <c r="AKE1" s="0"/>
-      <c r="AKF1" s="0"/>
-      <c r="AKG1" s="0"/>
-      <c r="AKH1" s="0"/>
-      <c r="AKI1" s="0"/>
-      <c r="AKJ1" s="0"/>
-      <c r="AKK1" s="0"/>
-      <c r="AKL1" s="0"/>
-      <c r="AKM1" s="0"/>
-      <c r="AKN1" s="0"/>
-      <c r="AKO1" s="0"/>
-      <c r="AKP1" s="0"/>
-      <c r="AKQ1" s="0"/>
-      <c r="AKR1" s="0"/>
-      <c r="AKS1" s="0"/>
-      <c r="AKT1" s="0"/>
-      <c r="AKU1" s="0"/>
-      <c r="AKV1" s="0"/>
-      <c r="AKW1" s="0"/>
-      <c r="AKX1" s="0"/>
-      <c r="AKY1" s="0"/>
-      <c r="AKZ1" s="0"/>
-      <c r="ALA1" s="0"/>
-      <c r="ALB1" s="0"/>
-      <c r="ALC1" s="0"/>
-      <c r="ALD1" s="0"/>
-      <c r="ALE1" s="0"/>
-      <c r="ALF1" s="0"/>
-      <c r="ALG1" s="0"/>
-      <c r="ALH1" s="0"/>
-      <c r="ALI1" s="0"/>
-      <c r="ALJ1" s="0"/>
-      <c r="ALK1" s="0"/>
-      <c r="ALL1" s="0"/>
-      <c r="ALM1" s="0"/>
-      <c r="ALN1" s="0"/>
-      <c r="ALO1" s="0"/>
-      <c r="ALP1" s="0"/>
-      <c r="ALQ1" s="0"/>
-      <c r="ALR1" s="0"/>
-      <c r="ALS1" s="0"/>
-      <c r="ALT1" s="0"/>
-      <c r="ALU1" s="0"/>
-      <c r="ALV1" s="0"/>
-      <c r="ALW1" s="0"/>
-      <c r="ALX1" s="0"/>
-      <c r="ALY1" s="0"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
+      <c r="AN1" s="3"/>
+      <c r="AO1" s="3"/>
+      <c r="AP1" s="3"/>
+      <c r="AQ1" s="3"/>
+      <c r="AR1" s="3"/>
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3"/>
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="3"/>
+      <c r="AW1" s="3"/>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
+      <c r="AZ1" s="3"/>
+      <c r="BA1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
+      <c r="BE1" s="3"/>
+      <c r="BF1" s="3"/>
+      <c r="BG1" s="3"/>
+      <c r="BH1" s="3"/>
+      <c r="BI1" s="3"/>
+      <c r="BJ1" s="3"/>
+      <c r="BK1" s="3"/>
+      <c r="BL1" s="3"/>
+      <c r="BM1" s="3"/>
+      <c r="BN1" s="3"/>
+      <c r="BO1" s="3"/>
+      <c r="BP1" s="3"/>
+      <c r="BQ1" s="3"/>
+      <c r="BR1" s="3"/>
+      <c r="BS1" s="3"/>
+      <c r="BT1" s="3"/>
+      <c r="BU1" s="3"/>
+      <c r="BV1" s="3"/>
+      <c r="BW1" s="3"/>
+      <c r="BX1" s="3"/>
+      <c r="BY1" s="3"/>
+      <c r="BZ1" s="3"/>
+      <c r="CA1" s="3"/>
+      <c r="CB1" s="3"/>
+      <c r="CC1" s="3"/>
+      <c r="CD1" s="3"/>
+      <c r="CE1" s="3"/>
+      <c r="CF1" s="3"/>
+      <c r="CG1" s="3"/>
+      <c r="CH1" s="3"/>
+      <c r="CI1" s="3"/>
+      <c r="CJ1" s="3"/>
+      <c r="CK1" s="3"/>
+      <c r="CL1" s="3"/>
+      <c r="CM1" s="3"/>
+      <c r="CN1" s="3"/>
+      <c r="CO1" s="3"/>
+      <c r="CP1" s="3"/>
+      <c r="CQ1" s="3"/>
+      <c r="CR1" s="3"/>
+      <c r="CS1" s="3"/>
+      <c r="CT1" s="3"/>
+      <c r="CU1" s="3"/>
+      <c r="CV1" s="3"/>
+      <c r="CW1" s="3"/>
+      <c r="CX1" s="3"/>
+      <c r="CY1" s="3"/>
+      <c r="CZ1" s="3"/>
+      <c r="DA1" s="3"/>
+      <c r="DB1" s="3"/>
+      <c r="DC1" s="3"/>
+      <c r="DD1" s="3"/>
+      <c r="DE1" s="3"/>
+      <c r="DF1" s="3"/>
+      <c r="DG1" s="3"/>
+      <c r="DH1" s="3"/>
+      <c r="DI1" s="3"/>
+      <c r="DJ1" s="3"/>
+      <c r="DK1" s="3"/>
+      <c r="DL1" s="3"/>
+      <c r="DM1" s="3"/>
+      <c r="DN1" s="3"/>
+      <c r="DO1" s="3"/>
+      <c r="DP1" s="3"/>
+      <c r="DQ1" s="3"/>
+      <c r="DR1" s="3"/>
+      <c r="DS1" s="3"/>
+      <c r="DT1" s="3"/>
+      <c r="DU1" s="3"/>
+      <c r="DV1" s="3"/>
+      <c r="DW1" s="3"/>
+      <c r="DX1" s="3"/>
+      <c r="DY1" s="3"/>
+      <c r="DZ1" s="3"/>
+      <c r="EA1" s="3"/>
+      <c r="EB1" s="3"/>
+      <c r="EC1" s="3"/>
+      <c r="ED1" s="3"/>
+      <c r="EE1" s="3"/>
+      <c r="EF1" s="3"/>
+      <c r="EG1" s="3"/>
+      <c r="EH1" s="3"/>
+      <c r="EI1" s="3"/>
+      <c r="EJ1" s="3"/>
+      <c r="EK1" s="3"/>
+      <c r="EL1" s="3"/>
+      <c r="EM1" s="3"/>
+      <c r="EN1" s="3"/>
+      <c r="EO1" s="3"/>
+      <c r="EP1" s="3"/>
+      <c r="EQ1" s="3"/>
+      <c r="ER1" s="3"/>
+      <c r="ES1" s="3"/>
+      <c r="ET1" s="3"/>
+      <c r="EU1" s="3"/>
+      <c r="EV1" s="3"/>
+      <c r="EW1" s="3"/>
+      <c r="EX1" s="3"/>
+      <c r="EY1" s="3"/>
+      <c r="EZ1" s="3"/>
+      <c r="FA1" s="3"/>
+      <c r="FB1" s="3"/>
+      <c r="FC1" s="3"/>
+      <c r="FD1" s="3"/>
+      <c r="FE1" s="3"/>
+      <c r="FF1" s="3"/>
+      <c r="FG1" s="3"/>
+      <c r="FH1" s="3"/>
+      <c r="FI1" s="3"/>
+      <c r="FJ1" s="3"/>
+      <c r="FK1" s="3"/>
+      <c r="FL1" s="3"/>
+      <c r="FM1" s="3"/>
+      <c r="FN1" s="3"/>
+      <c r="FO1" s="3"/>
+      <c r="FP1" s="3"/>
+      <c r="FQ1" s="3"/>
+      <c r="FR1" s="3"/>
+      <c r="FS1" s="3"/>
+      <c r="FT1" s="3"/>
+      <c r="FU1" s="3"/>
+      <c r="FV1" s="3"/>
+      <c r="FW1" s="3"/>
+      <c r="FX1" s="3"/>
+      <c r="FY1" s="3"/>
+      <c r="FZ1" s="3"/>
+      <c r="GA1" s="3"/>
+      <c r="GB1" s="3"/>
+      <c r="GC1" s="3"/>
+      <c r="GD1" s="3"/>
+      <c r="GE1" s="3"/>
+      <c r="GF1" s="3"/>
+      <c r="GG1" s="3"/>
+      <c r="GH1" s="3"/>
+      <c r="GI1" s="3"/>
+      <c r="GJ1" s="3"/>
+      <c r="GK1" s="3"/>
+      <c r="GL1" s="3"/>
+      <c r="GM1" s="3"/>
+      <c r="GN1" s="3"/>
+      <c r="GO1" s="3"/>
+      <c r="GP1" s="3"/>
+      <c r="GQ1" s="3"/>
+      <c r="GR1" s="3"/>
+      <c r="GS1" s="3"/>
+      <c r="GT1" s="3"/>
+      <c r="GU1" s="3"/>
+      <c r="GV1" s="3"/>
+      <c r="GW1" s="3"/>
+      <c r="GX1" s="3"/>
+      <c r="GY1" s="3"/>
+      <c r="GZ1" s="3"/>
+      <c r="HA1" s="3"/>
+      <c r="HB1" s="3"/>
+      <c r="HC1" s="3"/>
+      <c r="HD1" s="3"/>
+      <c r="HE1" s="3"/>
+      <c r="HF1" s="3"/>
+      <c r="HG1" s="3"/>
+      <c r="HH1" s="3"/>
+      <c r="HI1" s="3"/>
+      <c r="HJ1" s="3"/>
+      <c r="HK1" s="3"/>
+      <c r="HL1" s="3"/>
+      <c r="HM1" s="3"/>
+      <c r="HN1" s="3"/>
+      <c r="HO1" s="3"/>
+      <c r="HP1" s="3"/>
+      <c r="HQ1" s="3"/>
+      <c r="HR1" s="3"/>
+      <c r="HS1" s="3"/>
+      <c r="HT1" s="3"/>
+      <c r="HU1" s="3"/>
+      <c r="HV1" s="3"/>
+      <c r="HW1" s="3"/>
+      <c r="HX1" s="3"/>
+      <c r="HY1" s="3"/>
+      <c r="HZ1" s="3"/>
+      <c r="IA1" s="3"/>
+      <c r="IB1" s="3"/>
+      <c r="IC1" s="3"/>
+      <c r="ID1" s="3"/>
+      <c r="IE1" s="3"/>
+      <c r="IF1" s="3"/>
+      <c r="IG1" s="3"/>
+      <c r="IH1" s="3"/>
+      <c r="II1" s="3"/>
+      <c r="IJ1" s="3"/>
+      <c r="IK1" s="3"/>
+      <c r="IL1" s="3"/>
+      <c r="IM1" s="3"/>
+      <c r="IN1" s="3"/>
+      <c r="IO1" s="3"/>
+      <c r="IP1" s="3"/>
+      <c r="IQ1" s="3"/>
+      <c r="IR1" s="3"/>
+      <c r="IS1" s="3"/>
+      <c r="IT1" s="3"/>
+      <c r="IU1" s="3"/>
+      <c r="IV1" s="3"/>
+      <c r="IW1" s="3"/>
+      <c r="IX1" s="3"/>
+      <c r="IY1" s="3"/>
+      <c r="IZ1" s="3"/>
+      <c r="JA1" s="3"/>
+      <c r="JB1" s="3"/>
+      <c r="JC1" s="3"/>
+      <c r="JD1" s="3"/>
+      <c r="JE1" s="3"/>
+      <c r="JF1" s="3"/>
+      <c r="JG1" s="3"/>
+      <c r="JH1" s="3"/>
+      <c r="JI1" s="3"/>
+      <c r="JJ1" s="3"/>
+      <c r="JK1" s="3"/>
+      <c r="JL1" s="3"/>
+      <c r="JM1" s="3"/>
+      <c r="JN1" s="3"/>
+      <c r="JO1" s="3"/>
+      <c r="JP1" s="3"/>
+      <c r="JQ1" s="3"/>
+      <c r="JR1" s="3"/>
+      <c r="JS1" s="3"/>
+      <c r="JT1" s="3"/>
+      <c r="JU1" s="3"/>
+      <c r="JV1" s="3"/>
+      <c r="JW1" s="3"/>
+      <c r="JX1" s="3"/>
+      <c r="JY1" s="3"/>
+      <c r="JZ1" s="3"/>
+      <c r="KA1" s="3"/>
+      <c r="KB1" s="3"/>
+      <c r="KC1" s="3"/>
+      <c r="KD1" s="3"/>
+      <c r="KE1" s="3"/>
+      <c r="KF1" s="3"/>
+      <c r="KG1" s="3"/>
+      <c r="KH1" s="3"/>
+      <c r="KI1" s="3"/>
+      <c r="KJ1" s="3"/>
+      <c r="KK1" s="3"/>
+      <c r="KL1" s="3"/>
+      <c r="KM1" s="3"/>
+      <c r="KN1" s="3"/>
+      <c r="KO1" s="3"/>
+      <c r="KP1" s="3"/>
+      <c r="KQ1" s="3"/>
+      <c r="KR1" s="3"/>
+      <c r="KS1" s="3"/>
+      <c r="KT1" s="3"/>
+      <c r="KU1" s="3"/>
+      <c r="KV1" s="3"/>
+      <c r="KW1" s="3"/>
+      <c r="KX1" s="3"/>
+      <c r="KY1" s="3"/>
+      <c r="KZ1" s="3"/>
+      <c r="LA1" s="3"/>
+      <c r="LB1" s="3"/>
+      <c r="LC1" s="3"/>
+      <c r="LD1" s="3"/>
+      <c r="LE1" s="3"/>
+      <c r="LF1" s="3"/>
+      <c r="LG1" s="3"/>
+      <c r="LH1" s="3"/>
+      <c r="LI1" s="3"/>
+      <c r="LJ1" s="3"/>
+      <c r="LK1" s="3"/>
+      <c r="LL1" s="3"/>
+      <c r="LM1" s="3"/>
+      <c r="LN1" s="3"/>
+      <c r="LO1" s="3"/>
+      <c r="LP1" s="3"/>
+      <c r="LQ1" s="3"/>
+      <c r="LR1" s="3"/>
+      <c r="LS1" s="3"/>
+      <c r="LT1" s="3"/>
+      <c r="LU1" s="3"/>
+      <c r="LV1" s="3"/>
+      <c r="LW1" s="3"/>
+      <c r="LX1" s="3"/>
+      <c r="LY1" s="3"/>
+      <c r="LZ1" s="3"/>
+      <c r="MA1" s="3"/>
+      <c r="MB1" s="3"/>
+      <c r="MC1" s="3"/>
+      <c r="MD1" s="3"/>
+      <c r="ME1" s="3"/>
+      <c r="MF1" s="3"/>
+      <c r="MG1" s="3"/>
+      <c r="MH1" s="3"/>
+      <c r="MI1" s="3"/>
+      <c r="MJ1" s="3"/>
+      <c r="MK1" s="3"/>
+      <c r="ML1" s="3"/>
+      <c r="MM1" s="3"/>
+      <c r="MN1" s="3"/>
+      <c r="MO1" s="3"/>
+      <c r="MP1" s="3"/>
+      <c r="MQ1" s="3"/>
+      <c r="MR1" s="3"/>
+      <c r="MS1" s="3"/>
+      <c r="MT1" s="3"/>
+      <c r="MU1" s="3"/>
+      <c r="MV1" s="3"/>
+      <c r="MW1" s="3"/>
+      <c r="MX1" s="3"/>
+      <c r="MY1" s="3"/>
+      <c r="MZ1" s="3"/>
+      <c r="NA1" s="3"/>
+      <c r="NB1" s="3"/>
+      <c r="NC1" s="3"/>
+      <c r="ND1" s="3"/>
+      <c r="NE1" s="3"/>
+      <c r="NF1" s="3"/>
+      <c r="NG1" s="3"/>
+      <c r="NH1" s="3"/>
+      <c r="NI1" s="3"/>
+      <c r="NJ1" s="3"/>
+      <c r="NK1" s="3"/>
+      <c r="NL1" s="3"/>
+      <c r="NM1" s="3"/>
+      <c r="NN1" s="3"/>
+      <c r="NO1" s="3"/>
+      <c r="NP1" s="3"/>
+      <c r="NQ1" s="3"/>
+      <c r="NR1" s="3"/>
+      <c r="NS1" s="3"/>
+      <c r="NT1" s="3"/>
+      <c r="NU1" s="3"/>
+      <c r="NV1" s="3"/>
+      <c r="NW1" s="3"/>
+      <c r="NX1" s="3"/>
+      <c r="NY1" s="3"/>
+      <c r="NZ1" s="3"/>
+      <c r="OA1" s="3"/>
+      <c r="OB1" s="3"/>
+      <c r="OC1" s="3"/>
+      <c r="OD1" s="3"/>
+      <c r="OE1" s="3"/>
+      <c r="OF1" s="3"/>
+      <c r="OG1" s="3"/>
+      <c r="OH1" s="3"/>
+      <c r="OI1" s="3"/>
+      <c r="OJ1" s="3"/>
+      <c r="OK1" s="3"/>
+      <c r="OL1" s="3"/>
+      <c r="OM1" s="3"/>
+      <c r="ON1" s="3"/>
+      <c r="OO1" s="3"/>
+      <c r="OP1" s="3"/>
+      <c r="OQ1" s="3"/>
+      <c r="OR1" s="3"/>
+      <c r="OS1" s="3"/>
+      <c r="OT1" s="3"/>
+      <c r="OU1" s="3"/>
+      <c r="OV1" s="3"/>
+      <c r="OW1" s="3"/>
+      <c r="OX1" s="3"/>
+      <c r="OY1" s="3"/>
+      <c r="OZ1" s="3"/>
+      <c r="PA1" s="3"/>
+      <c r="PB1" s="3"/>
+      <c r="PC1" s="3"/>
+      <c r="PD1" s="3"/>
+      <c r="PE1" s="3"/>
+      <c r="PF1" s="3"/>
+      <c r="PG1" s="3"/>
+      <c r="PH1" s="3"/>
+      <c r="PI1" s="3"/>
+      <c r="PJ1" s="3"/>
+      <c r="PK1" s="3"/>
+      <c r="PL1" s="3"/>
+      <c r="PM1" s="3"/>
+      <c r="PN1" s="3"/>
+      <c r="PO1" s="3"/>
+      <c r="PP1" s="3"/>
+      <c r="PQ1" s="3"/>
+      <c r="PR1" s="3"/>
+      <c r="PS1" s="3"/>
+      <c r="PT1" s="3"/>
+      <c r="PU1" s="3"/>
+      <c r="PV1" s="3"/>
+      <c r="PW1" s="3"/>
+      <c r="PX1" s="3"/>
+      <c r="PY1" s="3"/>
+      <c r="PZ1" s="3"/>
+      <c r="QA1" s="3"/>
+      <c r="QB1" s="3"/>
+      <c r="QC1" s="3"/>
+      <c r="QD1" s="3"/>
+      <c r="QE1" s="3"/>
+      <c r="QF1" s="3"/>
+      <c r="QG1" s="3"/>
+      <c r="QH1" s="3"/>
+      <c r="QI1" s="3"/>
+      <c r="QJ1" s="3"/>
+      <c r="QK1" s="3"/>
+      <c r="QL1" s="3"/>
+      <c r="QM1" s="3"/>
+      <c r="QN1" s="3"/>
+      <c r="QO1" s="3"/>
+      <c r="QP1" s="3"/>
+      <c r="QQ1" s="3"/>
+      <c r="QR1" s="3"/>
+      <c r="QS1" s="3"/>
+      <c r="QT1" s="3"/>
+      <c r="QU1" s="3"/>
+      <c r="QV1" s="3"/>
+      <c r="QW1" s="3"/>
+      <c r="QX1" s="3"/>
+      <c r="QY1" s="3"/>
+      <c r="QZ1" s="3"/>
+      <c r="RA1" s="3"/>
+      <c r="RB1" s="3"/>
+      <c r="RC1" s="3"/>
+      <c r="RD1" s="3"/>
+      <c r="RE1" s="3"/>
+      <c r="RF1" s="3"/>
+      <c r="RG1" s="3"/>
+      <c r="RH1" s="3"/>
+      <c r="RI1" s="3"/>
+      <c r="RJ1" s="3"/>
+      <c r="RK1" s="3"/>
+      <c r="RL1" s="3"/>
+      <c r="RM1" s="3"/>
+      <c r="RN1" s="3"/>
+      <c r="RO1" s="3"/>
+      <c r="RP1" s="3"/>
+      <c r="RQ1" s="3"/>
+      <c r="RR1" s="3"/>
+      <c r="RS1" s="3"/>
+      <c r="RT1" s="3"/>
+      <c r="RU1" s="3"/>
+      <c r="RV1" s="3"/>
+      <c r="RW1" s="3"/>
+      <c r="RX1" s="3"/>
+      <c r="RY1" s="3"/>
+      <c r="RZ1" s="3"/>
+      <c r="SA1" s="3"/>
+      <c r="SB1" s="3"/>
+      <c r="SC1" s="3"/>
+      <c r="SD1" s="3"/>
+      <c r="SE1" s="3"/>
+      <c r="SF1" s="3"/>
+      <c r="SG1" s="3"/>
+      <c r="SH1" s="3"/>
+      <c r="SI1" s="3"/>
+      <c r="SJ1" s="3"/>
+      <c r="SK1" s="3"/>
+      <c r="SL1" s="3"/>
+      <c r="SM1" s="3"/>
+      <c r="SN1" s="3"/>
+      <c r="SO1" s="3"/>
+      <c r="SP1" s="3"/>
+      <c r="SQ1" s="3"/>
+      <c r="SR1" s="3"/>
+      <c r="SS1" s="3"/>
+      <c r="ST1" s="3"/>
+      <c r="SU1" s="3"/>
+      <c r="SV1" s="3"/>
+      <c r="SW1" s="3"/>
+      <c r="SX1" s="3"/>
+      <c r="SY1" s="3"/>
+      <c r="SZ1" s="3"/>
+      <c r="TA1" s="3"/>
+      <c r="TB1" s="3"/>
+      <c r="TC1" s="3"/>
+      <c r="TD1" s="3"/>
+      <c r="TE1" s="3"/>
+      <c r="TF1" s="3"/>
+      <c r="TG1" s="3"/>
+      <c r="TH1" s="3"/>
+      <c r="TI1" s="3"/>
+      <c r="TJ1" s="3"/>
+      <c r="TK1" s="3"/>
+      <c r="TL1" s="3"/>
+      <c r="TM1" s="3"/>
+      <c r="TN1" s="3"/>
+      <c r="TO1" s="3"/>
+      <c r="TP1" s="3"/>
+      <c r="TQ1" s="3"/>
+      <c r="TR1" s="3"/>
+      <c r="TS1" s="3"/>
+      <c r="TT1" s="3"/>
+      <c r="TU1" s="3"/>
+      <c r="TV1" s="3"/>
+      <c r="TW1" s="3"/>
+      <c r="TX1" s="3"/>
+      <c r="TY1" s="3"/>
+      <c r="TZ1" s="3"/>
+      <c r="UA1" s="3"/>
+      <c r="UB1" s="3"/>
+      <c r="UC1" s="3"/>
+      <c r="UD1" s="3"/>
+      <c r="UE1" s="3"/>
+      <c r="UF1" s="3"/>
+      <c r="UG1" s="3"/>
+      <c r="UH1" s="3"/>
+      <c r="UI1" s="3"/>
+      <c r="UJ1" s="3"/>
+      <c r="UK1" s="3"/>
+      <c r="UL1" s="3"/>
+      <c r="UM1" s="3"/>
+      <c r="UN1" s="3"/>
+      <c r="UO1" s="3"/>
+      <c r="UP1" s="3"/>
+      <c r="UQ1" s="3"/>
+      <c r="UR1" s="3"/>
+      <c r="US1" s="3"/>
+      <c r="UT1" s="3"/>
+      <c r="UU1" s="3"/>
+      <c r="UV1" s="3"/>
+      <c r="UW1" s="3"/>
+      <c r="UX1" s="3"/>
+      <c r="UY1" s="3"/>
+      <c r="UZ1" s="3"/>
+      <c r="VA1" s="3"/>
+      <c r="VB1" s="3"/>
+      <c r="VC1" s="3"/>
+      <c r="VD1" s="3"/>
+      <c r="VE1" s="3"/>
+      <c r="VF1" s="3"/>
+      <c r="VG1" s="3"/>
+      <c r="VH1" s="3"/>
+      <c r="VI1" s="3"/>
+      <c r="VJ1" s="3"/>
+      <c r="VK1" s="3"/>
+      <c r="VL1" s="3"/>
+      <c r="VM1" s="3"/>
+      <c r="VN1" s="3"/>
+      <c r="VO1" s="3"/>
+      <c r="VP1" s="3"/>
+      <c r="VQ1" s="3"/>
+      <c r="VR1" s="3"/>
+      <c r="VS1" s="3"/>
+      <c r="VT1" s="3"/>
+      <c r="VU1" s="3"/>
+      <c r="VV1" s="3"/>
+      <c r="VW1" s="3"/>
+      <c r="VX1" s="3"/>
+      <c r="VY1" s="3"/>
+      <c r="VZ1" s="3"/>
+      <c r="WA1" s="3"/>
+      <c r="WB1" s="3"/>
+      <c r="WC1" s="3"/>
+      <c r="WD1" s="3"/>
+      <c r="WE1" s="3"/>
+      <c r="WF1" s="3"/>
+      <c r="WG1" s="3"/>
+      <c r="WH1" s="3"/>
+      <c r="WI1" s="3"/>
+      <c r="WJ1" s="3"/>
+      <c r="WK1" s="3"/>
+      <c r="WL1" s="3"/>
+      <c r="WM1" s="3"/>
+      <c r="WN1" s="3"/>
+      <c r="WO1" s="3"/>
+      <c r="WP1" s="3"/>
+      <c r="WQ1" s="3"/>
+      <c r="WR1" s="3"/>
+      <c r="WS1" s="3"/>
+      <c r="WT1" s="3"/>
+      <c r="WU1" s="3"/>
+      <c r="WV1" s="3"/>
+      <c r="WW1" s="3"/>
+      <c r="WX1" s="3"/>
+      <c r="WY1" s="3"/>
+      <c r="WZ1" s="3"/>
+      <c r="XA1" s="3"/>
+      <c r="XB1" s="3"/>
+      <c r="XC1" s="3"/>
+      <c r="XD1" s="3"/>
+      <c r="XE1" s="3"/>
+      <c r="XF1" s="3"/>
+      <c r="XG1" s="3"/>
+      <c r="XH1" s="3"/>
+      <c r="XI1" s="3"/>
+      <c r="XJ1" s="3"/>
+      <c r="XK1" s="3"/>
+      <c r="XL1" s="3"/>
+      <c r="XM1" s="3"/>
+      <c r="XN1" s="3"/>
+      <c r="XO1" s="3"/>
+      <c r="XP1" s="3"/>
+      <c r="XQ1" s="3"/>
+      <c r="XR1" s="3"/>
+      <c r="XS1" s="3"/>
+      <c r="XT1" s="3"/>
+      <c r="XU1" s="3"/>
+      <c r="XV1" s="3"/>
+      <c r="XW1" s="3"/>
+      <c r="XX1" s="3"/>
+      <c r="XY1" s="3"/>
+      <c r="XZ1" s="3"/>
+      <c r="YA1" s="3"/>
+      <c r="YB1" s="3"/>
+      <c r="YC1" s="3"/>
+      <c r="YD1" s="3"/>
+      <c r="YE1" s="3"/>
+      <c r="YF1" s="3"/>
+      <c r="YG1" s="3"/>
+      <c r="YH1" s="3"/>
+      <c r="YI1" s="3"/>
+      <c r="YJ1" s="3"/>
+      <c r="YK1" s="3"/>
+      <c r="YL1" s="3"/>
+      <c r="YM1" s="3"/>
+      <c r="YN1" s="3"/>
+      <c r="YO1" s="3"/>
+      <c r="YP1" s="3"/>
+      <c r="YQ1" s="3"/>
+      <c r="YR1" s="3"/>
+      <c r="YS1" s="3"/>
+      <c r="YT1" s="3"/>
+      <c r="YU1" s="3"/>
+      <c r="YV1" s="3"/>
+      <c r="YW1" s="3"/>
+      <c r="YX1" s="3"/>
+      <c r="YY1" s="3"/>
+      <c r="YZ1" s="3"/>
+      <c r="ZA1" s="3"/>
+      <c r="ZB1" s="3"/>
+      <c r="ZC1" s="3"/>
+      <c r="ZD1" s="3"/>
+      <c r="ZE1" s="3"/>
+      <c r="ZF1" s="3"/>
+      <c r="ZG1" s="3"/>
+      <c r="ZH1" s="3"/>
+      <c r="ZI1" s="3"/>
+      <c r="ZJ1" s="3"/>
+      <c r="ZK1" s="3"/>
+      <c r="ZL1" s="3"/>
+      <c r="ZM1" s="3"/>
+      <c r="ZN1" s="3"/>
+      <c r="ZO1" s="3"/>
+      <c r="ZP1" s="3"/>
+      <c r="ZQ1" s="3"/>
+      <c r="ZR1" s="3"/>
+      <c r="ZS1" s="3"/>
+      <c r="ZT1" s="3"/>
+      <c r="ZU1" s="3"/>
+      <c r="ZV1" s="3"/>
+      <c r="ZW1" s="3"/>
+      <c r="ZX1" s="3"/>
+      <c r="ZY1" s="3"/>
+      <c r="ZZ1" s="3"/>
+      <c r="AAA1" s="3"/>
+      <c r="AAB1" s="3"/>
+      <c r="AAC1" s="3"/>
+      <c r="AAD1" s="3"/>
+      <c r="AAE1" s="3"/>
+      <c r="AAF1" s="3"/>
+      <c r="AAG1" s="3"/>
+      <c r="AAH1" s="3"/>
+      <c r="AAI1" s="3"/>
+      <c r="AAJ1" s="3"/>
+      <c r="AAK1" s="3"/>
+      <c r="AAL1" s="3"/>
+      <c r="AAM1" s="3"/>
+      <c r="AAN1" s="3"/>
+      <c r="AAO1" s="3"/>
+      <c r="AAP1" s="3"/>
+      <c r="AAQ1" s="3"/>
+      <c r="AAR1" s="3"/>
+      <c r="AAS1" s="3"/>
+      <c r="AAT1" s="3"/>
+      <c r="AAU1" s="3"/>
+      <c r="AAV1" s="3"/>
+      <c r="AAW1" s="3"/>
+      <c r="AAX1" s="3"/>
+      <c r="AAY1" s="3"/>
+      <c r="AAZ1" s="3"/>
+      <c r="ABA1" s="3"/>
+      <c r="ABB1" s="3"/>
+      <c r="ABC1" s="3"/>
+      <c r="ABD1" s="3"/>
+      <c r="ABE1" s="3"/>
+      <c r="ABF1" s="3"/>
+      <c r="ABG1" s="3"/>
+      <c r="ABH1" s="3"/>
+      <c r="ABI1" s="3"/>
+      <c r="ABJ1" s="3"/>
+      <c r="ABK1" s="3"/>
+      <c r="ABL1" s="3"/>
+      <c r="ABM1" s="3"/>
+      <c r="ABN1" s="3"/>
+      <c r="ABO1" s="3"/>
+      <c r="ABP1" s="3"/>
+      <c r="ABQ1" s="3"/>
+      <c r="ABR1" s="3"/>
+      <c r="ABS1" s="3"/>
+      <c r="ABT1" s="3"/>
+      <c r="ABU1" s="3"/>
+      <c r="ABV1" s="3"/>
+      <c r="ABW1" s="3"/>
+      <c r="ABX1" s="3"/>
+      <c r="ABY1" s="3"/>
+      <c r="ABZ1" s="3"/>
+      <c r="ACA1" s="3"/>
+      <c r="ACB1" s="3"/>
+      <c r="ACC1" s="3"/>
+      <c r="ACD1" s="3"/>
+      <c r="ACE1" s="3"/>
+      <c r="ACF1" s="3"/>
+      <c r="ACG1" s="3"/>
+      <c r="ACH1" s="3"/>
+      <c r="ACI1" s="3"/>
+      <c r="ACJ1" s="3"/>
+      <c r="ACK1" s="3"/>
+      <c r="ACL1" s="3"/>
+      <c r="ACM1" s="3"/>
+      <c r="ACN1" s="3"/>
+      <c r="ACO1" s="3"/>
+      <c r="ACP1" s="3"/>
+      <c r="ACQ1" s="3"/>
+      <c r="ACR1" s="3"/>
+      <c r="ACS1" s="3"/>
+      <c r="ACT1" s="3"/>
+      <c r="ACU1" s="3"/>
+      <c r="ACV1" s="3"/>
+      <c r="ACW1" s="3"/>
+      <c r="ACX1" s="3"/>
+      <c r="ACY1" s="3"/>
+      <c r="ACZ1" s="3"/>
+      <c r="ADA1" s="3"/>
+      <c r="ADB1" s="3"/>
+      <c r="ADC1" s="3"/>
+      <c r="ADD1" s="3"/>
+      <c r="ADE1" s="3"/>
+      <c r="ADF1" s="3"/>
+      <c r="ADG1" s="3"/>
+      <c r="ADH1" s="3"/>
+      <c r="ADI1" s="3"/>
+      <c r="ADJ1" s="3"/>
+      <c r="ADK1" s="3"/>
+      <c r="ADL1" s="3"/>
+      <c r="ADM1" s="3"/>
+      <c r="ADN1" s="3"/>
+      <c r="ADO1" s="3"/>
+      <c r="ADP1" s="3"/>
+      <c r="ADQ1" s="3"/>
+      <c r="ADR1" s="3"/>
+      <c r="ADS1" s="3"/>
+      <c r="ADT1" s="3"/>
+      <c r="ADU1" s="3"/>
+      <c r="ADV1" s="3"/>
+      <c r="ADW1" s="3"/>
+      <c r="ADX1" s="3"/>
+      <c r="ADY1" s="3"/>
+      <c r="ADZ1" s="3"/>
+      <c r="AEA1" s="3"/>
+      <c r="AEB1" s="3"/>
+      <c r="AEC1" s="3"/>
+      <c r="AED1" s="3"/>
+      <c r="AEE1" s="3"/>
+      <c r="AEF1" s="3"/>
+      <c r="AEG1" s="3"/>
+      <c r="AEH1" s="3"/>
+      <c r="AEI1" s="3"/>
+      <c r="AEJ1" s="3"/>
+      <c r="AEK1" s="3"/>
+      <c r="AEL1" s="3"/>
+      <c r="AEM1" s="3"/>
+      <c r="AEN1" s="3"/>
+      <c r="AEO1" s="3"/>
+      <c r="AEP1" s="3"/>
+      <c r="AEQ1" s="3"/>
+      <c r="AER1" s="3"/>
+      <c r="AES1" s="3"/>
+      <c r="AET1" s="3"/>
+      <c r="AEU1" s="3"/>
+      <c r="AEV1" s="3"/>
+      <c r="AEW1" s="3"/>
+      <c r="AEX1" s="3"/>
+      <c r="AEY1" s="3"/>
+      <c r="AEZ1" s="3"/>
+      <c r="AFA1" s="3"/>
+      <c r="AFB1" s="3"/>
+      <c r="AFC1" s="3"/>
+      <c r="AFD1" s="3"/>
+      <c r="AFE1" s="3"/>
+      <c r="AFF1" s="3"/>
+      <c r="AFG1" s="3"/>
+      <c r="AFH1" s="3"/>
+      <c r="AFI1" s="3"/>
+      <c r="AFJ1" s="3"/>
+      <c r="AFK1" s="3"/>
+      <c r="AFL1" s="3"/>
+      <c r="AFM1" s="3"/>
+      <c r="AFN1" s="3"/>
+      <c r="AFO1" s="3"/>
+      <c r="AFP1" s="3"/>
+      <c r="AFQ1" s="3"/>
+      <c r="AFR1" s="3"/>
+      <c r="AFS1" s="3"/>
+      <c r="AFT1" s="3"/>
+      <c r="AFU1" s="3"/>
+      <c r="AFV1" s="3"/>
+      <c r="AFW1" s="3"/>
+      <c r="AFX1" s="3"/>
+      <c r="AFY1" s="3"/>
+      <c r="AFZ1" s="3"/>
+      <c r="AGA1" s="3"/>
+      <c r="AGB1" s="3"/>
+      <c r="AGC1" s="3"/>
+      <c r="AGD1" s="3"/>
+      <c r="AGE1" s="3"/>
+      <c r="AGF1" s="3"/>
+      <c r="AGG1" s="3"/>
+      <c r="AGH1" s="3"/>
+      <c r="AGI1" s="3"/>
+      <c r="AGJ1" s="3"/>
+      <c r="AGK1" s="3"/>
+      <c r="AGL1" s="3"/>
+      <c r="AGM1" s="3"/>
+      <c r="AGN1" s="3"/>
+      <c r="AGO1" s="3"/>
+      <c r="AGP1" s="3"/>
+      <c r="AGQ1" s="3"/>
+      <c r="AGR1" s="3"/>
+      <c r="AGS1" s="3"/>
+      <c r="AGT1" s="3"/>
+      <c r="AGU1" s="3"/>
+      <c r="AGV1" s="3"/>
+      <c r="AGW1" s="3"/>
+      <c r="AGX1" s="3"/>
+      <c r="AGY1" s="3"/>
+      <c r="AGZ1" s="3"/>
+      <c r="AHA1" s="3"/>
+      <c r="AHB1" s="3"/>
+      <c r="AHC1" s="3"/>
+      <c r="AHD1" s="3"/>
+      <c r="AHE1" s="3"/>
+      <c r="AHF1" s="3"/>
+      <c r="AHG1" s="3"/>
+      <c r="AHH1" s="3"/>
+      <c r="AHI1" s="3"/>
+      <c r="AHJ1" s="3"/>
+      <c r="AHK1" s="3"/>
+      <c r="AHL1" s="3"/>
+      <c r="AHM1" s="3"/>
+      <c r="AHN1" s="3"/>
+      <c r="AHO1" s="3"/>
+      <c r="AHP1" s="3"/>
+      <c r="AHQ1" s="3"/>
+      <c r="AHR1" s="3"/>
+      <c r="AHS1" s="3"/>
+      <c r="AHT1" s="3"/>
+      <c r="AHU1" s="3"/>
+      <c r="AHV1" s="3"/>
+      <c r="AHW1" s="3"/>
+      <c r="AHX1" s="3"/>
+      <c r="AHY1" s="3"/>
+      <c r="AHZ1" s="3"/>
+      <c r="AIA1" s="3"/>
+      <c r="AIB1" s="3"/>
+      <c r="AIC1" s="3"/>
+      <c r="AID1" s="3"/>
+      <c r="AIE1" s="3"/>
+      <c r="AIF1" s="3"/>
+      <c r="AIG1" s="3"/>
+      <c r="AIH1" s="3"/>
+      <c r="AII1" s="3"/>
+      <c r="AIJ1" s="3"/>
+      <c r="AIK1" s="3"/>
+      <c r="AIL1" s="3"/>
+      <c r="AIM1" s="3"/>
+      <c r="AIN1" s="3"/>
+      <c r="AIO1" s="3"/>
+      <c r="AIP1" s="3"/>
+      <c r="AIQ1" s="3"/>
+      <c r="AIR1" s="3"/>
+      <c r="AIS1" s="3"/>
+      <c r="AIT1" s="3"/>
+      <c r="AIU1" s="3"/>
+      <c r="AIV1" s="3"/>
+      <c r="AIW1" s="3"/>
+      <c r="AIX1" s="3"/>
+      <c r="AIY1" s="3"/>
+      <c r="AIZ1" s="3"/>
+      <c r="AJA1" s="3"/>
+      <c r="AJB1" s="3"/>
+      <c r="AJC1" s="3"/>
+      <c r="AJD1" s="3"/>
+      <c r="AJE1" s="3"/>
+      <c r="AJF1" s="3"/>
+      <c r="AJG1" s="3"/>
+      <c r="AJH1" s="3"/>
+      <c r="AJI1" s="3"/>
+      <c r="AJJ1" s="3"/>
+      <c r="AJK1" s="3"/>
+      <c r="AJL1" s="3"/>
+      <c r="AJM1" s="3"/>
+      <c r="AJN1" s="3"/>
+      <c r="AJO1" s="3"/>
+      <c r="AJP1" s="3"/>
+      <c r="AJQ1" s="3"/>
+      <c r="AJR1" s="3"/>
+      <c r="AJS1" s="3"/>
+      <c r="AJT1" s="3"/>
+      <c r="AJU1" s="3"/>
+      <c r="AJV1" s="3"/>
+      <c r="AJW1" s="3"/>
+      <c r="AJX1" s="3"/>
+      <c r="AJY1" s="3"/>
+      <c r="AJZ1" s="3"/>
+      <c r="AKA1" s="3"/>
+      <c r="AKB1" s="3"/>
+      <c r="AKC1" s="3"/>
+      <c r="AKD1" s="3"/>
+      <c r="AKE1" s="3"/>
+      <c r="AKF1" s="3"/>
+      <c r="AKG1" s="3"/>
+      <c r="AKH1" s="3"/>
+      <c r="AKI1" s="3"/>
+      <c r="AKJ1" s="3"/>
+      <c r="AKK1" s="3"/>
+      <c r="AKL1" s="3"/>
+      <c r="AKM1" s="3"/>
+      <c r="AKN1" s="3"/>
+      <c r="AKO1" s="3"/>
+      <c r="AKP1" s="3"/>
+      <c r="AKQ1" s="3"/>
+      <c r="AKR1" s="3"/>
+      <c r="AKS1" s="3"/>
+      <c r="AKT1" s="3"/>
+      <c r="AKU1" s="3"/>
+      <c r="AKV1" s="3"/>
+      <c r="AKW1" s="3"/>
+      <c r="AKX1" s="3"/>
+      <c r="AKY1" s="3"/>
+      <c r="AKZ1" s="3"/>
+      <c r="ALA1" s="3"/>
+      <c r="ALB1" s="3"/>
+      <c r="ALC1" s="3"/>
+      <c r="ALD1" s="3"/>
+      <c r="ALE1" s="3"/>
+      <c r="ALF1" s="3"/>
+      <c r="ALG1" s="3"/>
+      <c r="ALH1" s="3"/>
+      <c r="ALI1" s="3"/>
+      <c r="ALJ1" s="3"/>
+      <c r="ALK1" s="3"/>
+      <c r="ALL1" s="3"/>
+      <c r="ALM1" s="3"/>
+      <c r="ALN1" s="3"/>
+      <c r="ALO1" s="3"/>
+      <c r="ALP1" s="3"/>
+      <c r="ALQ1" s="3"/>
+      <c r="ALR1" s="3"/>
+      <c r="ALS1" s="3"/>
+      <c r="ALT1" s="3"/>
+      <c r="ALU1" s="3"/>
+      <c r="ALV1" s="3"/>
+      <c r="ALW1" s="3"/>
+      <c r="ALX1" s="3"/>
+      <c r="ALY1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
@@ -3785,14 +3802,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
       <formula1>ListExtractors!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3802,7 +3819,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
@@ -3841,18 +3858,18 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
       <formula1>Help!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1004" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1004" type="list">
       <formula1>ListDigesters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
fix(Examples/DefaultConfig): Make audio_host optional
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -628,7 +628,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
   <si>
     <t xml:space="preserve">SoundScapeExplorer
 Version 11</t>
@@ -698,26 +698,43 @@
 Examples: `audio`, `C:\path\to\audio`, `/home/user/audio`</t>
   </si>
   <si>
+    <t xml:space="preserve">expected_sample_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sample rate of your audio samples in Hertz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timeline_origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The date to start integration from.</t>
+  </si>
+  <si>
     <t xml:space="preserve">audio_host</t>
   </si>
   <si>
-    <t xml:space="preserve">http://localhost:5531</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The host name serving your audio files.
-For Docker, use `http://localhost:5531`.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expected_sample_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The sample rate of your audio samples in Hertz.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timeline_origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The date to start integration from.</t>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">The host name serving your audio files. Example: `http://localhost:5531`
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optional</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">timezone</t>
@@ -1133,16 +1150,16 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <i val="true"/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <i val="true"/>
       <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1343,15 +1360,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1701,25 +1718,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>67</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>68</v>
       </c>
       <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="40" t="n">
         <v>2</v>
@@ -1730,7 +1747,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="39" t="n">
         <v>3</v>
@@ -1786,31 +1803,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="D1" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>73</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>74</v>
       </c>
       <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="40" t="n">
         <v>50</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="40" t="n">
         <v>1</v>
@@ -1866,82 +1883,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="48" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" s="48" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>80</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="49" t="s">
         <v>84</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="49" t="s">
         <v>86</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="50" t="s">
         <v>88</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="50" t="s">
         <v>90</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="50" t="s">
         <v>92</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="50" t="s">
         <v>94</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1980,74 +1997,74 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="49" t="s">
         <v>97</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>99</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>101</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="49" t="s">
         <v>103</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="49" t="s">
         <v>105</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,27 +2105,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2146,17 +2163,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2190,22 +2207,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2280,88 +2297,1103 @@
       <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="n">
+        <v>44100</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>23</v>
       </c>
       <c r="AMJ4" s="15"/>
     </row>
     <row r="5" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="19" t="n">
+        <v>36526</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="17" t="n">
-        <v>44100</v>
-      </c>
-      <c r="C5" s="18" t="s">
+      <c r="AMJ5" s="15"/>
+    </row>
+    <row r="6" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="AMJ5" s="15"/>
-    </row>
-    <row r="6" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="20" t="n">
-        <v>36526</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="14"/>
+      <c r="AH6" s="14"/>
+      <c r="AI6" s="14"/>
+      <c r="AJ6" s="14"/>
+      <c r="AK6" s="14"/>
+      <c r="AL6" s="14"/>
+      <c r="AM6" s="14"/>
+      <c r="AN6" s="14"/>
+      <c r="AO6" s="14"/>
+      <c r="AP6" s="14"/>
+      <c r="AQ6" s="14"/>
+      <c r="AR6" s="14"/>
+      <c r="AS6" s="14"/>
+      <c r="AT6" s="14"/>
+      <c r="AU6" s="14"/>
+      <c r="AV6" s="14"/>
+      <c r="AW6" s="14"/>
+      <c r="AX6" s="14"/>
+      <c r="AY6" s="14"/>
+      <c r="AZ6" s="14"/>
+      <c r="BA6" s="14"/>
+      <c r="BB6" s="14"/>
+      <c r="BC6" s="14"/>
+      <c r="BD6" s="14"/>
+      <c r="BE6" s="14"/>
+      <c r="BF6" s="14"/>
+      <c r="BG6" s="14"/>
+      <c r="BH6" s="14"/>
+      <c r="BI6" s="14"/>
+      <c r="BJ6" s="14"/>
+      <c r="BK6" s="14"/>
+      <c r="BL6" s="14"/>
+      <c r="BM6" s="14"/>
+      <c r="BN6" s="14"/>
+      <c r="BO6" s="14"/>
+      <c r="BP6" s="14"/>
+      <c r="BQ6" s="14"/>
+      <c r="BR6" s="14"/>
+      <c r="BS6" s="14"/>
+      <c r="BT6" s="14"/>
+      <c r="BU6" s="14"/>
+      <c r="BV6" s="14"/>
+      <c r="BW6" s="14"/>
+      <c r="BX6" s="14"/>
+      <c r="BY6" s="14"/>
+      <c r="BZ6" s="14"/>
+      <c r="CA6" s="14"/>
+      <c r="CB6" s="14"/>
+      <c r="CC6" s="14"/>
+      <c r="CD6" s="14"/>
+      <c r="CE6" s="14"/>
+      <c r="CF6" s="14"/>
+      <c r="CG6" s="14"/>
+      <c r="CH6" s="14"/>
+      <c r="CI6" s="14"/>
+      <c r="CJ6" s="14"/>
+      <c r="CK6" s="14"/>
+      <c r="CL6" s="14"/>
+      <c r="CM6" s="14"/>
+      <c r="CN6" s="14"/>
+      <c r="CO6" s="14"/>
+      <c r="CP6" s="14"/>
+      <c r="CQ6" s="14"/>
+      <c r="CR6" s="14"/>
+      <c r="CS6" s="14"/>
+      <c r="CT6" s="14"/>
+      <c r="CU6" s="14"/>
+      <c r="CV6" s="14"/>
+      <c r="CW6" s="14"/>
+      <c r="CX6" s="14"/>
+      <c r="CY6" s="14"/>
+      <c r="CZ6" s="14"/>
+      <c r="DA6" s="14"/>
+      <c r="DB6" s="14"/>
+      <c r="DC6" s="14"/>
+      <c r="DD6" s="14"/>
+      <c r="DE6" s="14"/>
+      <c r="DF6" s="14"/>
+      <c r="DG6" s="14"/>
+      <c r="DH6" s="14"/>
+      <c r="DI6" s="14"/>
+      <c r="DJ6" s="14"/>
+      <c r="DK6" s="14"/>
+      <c r="DL6" s="14"/>
+      <c r="DM6" s="14"/>
+      <c r="DN6" s="14"/>
+      <c r="DO6" s="14"/>
+      <c r="DP6" s="14"/>
+      <c r="DQ6" s="14"/>
+      <c r="DR6" s="14"/>
+      <c r="DS6" s="14"/>
+      <c r="DT6" s="14"/>
+      <c r="DU6" s="14"/>
+      <c r="DV6" s="14"/>
+      <c r="DW6" s="14"/>
+      <c r="DX6" s="14"/>
+      <c r="DY6" s="14"/>
+      <c r="DZ6" s="14"/>
+      <c r="EA6" s="14"/>
+      <c r="EB6" s="14"/>
+      <c r="EC6" s="14"/>
+      <c r="ED6" s="14"/>
+      <c r="EE6" s="14"/>
+      <c r="EF6" s="14"/>
+      <c r="EG6" s="14"/>
+      <c r="EH6" s="14"/>
+      <c r="EI6" s="14"/>
+      <c r="EJ6" s="14"/>
+      <c r="EK6" s="14"/>
+      <c r="EL6" s="14"/>
+      <c r="EM6" s="14"/>
+      <c r="EN6" s="14"/>
+      <c r="EO6" s="14"/>
+      <c r="EP6" s="14"/>
+      <c r="EQ6" s="14"/>
+      <c r="ER6" s="14"/>
+      <c r="ES6" s="14"/>
+      <c r="ET6" s="14"/>
+      <c r="EU6" s="14"/>
+      <c r="EV6" s="14"/>
+      <c r="EW6" s="14"/>
+      <c r="EX6" s="14"/>
+      <c r="EY6" s="14"/>
+      <c r="EZ6" s="14"/>
+      <c r="FA6" s="14"/>
+      <c r="FB6" s="14"/>
+      <c r="FC6" s="14"/>
+      <c r="FD6" s="14"/>
+      <c r="FE6" s="14"/>
+      <c r="FF6" s="14"/>
+      <c r="FG6" s="14"/>
+      <c r="FH6" s="14"/>
+      <c r="FI6" s="14"/>
+      <c r="FJ6" s="14"/>
+      <c r="FK6" s="14"/>
+      <c r="FL6" s="14"/>
+      <c r="FM6" s="14"/>
+      <c r="FN6" s="14"/>
+      <c r="FO6" s="14"/>
+      <c r="FP6" s="14"/>
+      <c r="FQ6" s="14"/>
+      <c r="FR6" s="14"/>
+      <c r="FS6" s="14"/>
+      <c r="FT6" s="14"/>
+      <c r="FU6" s="14"/>
+      <c r="FV6" s="14"/>
+      <c r="FW6" s="14"/>
+      <c r="FX6" s="14"/>
+      <c r="FY6" s="14"/>
+      <c r="FZ6" s="14"/>
+      <c r="GA6" s="14"/>
+      <c r="GB6" s="14"/>
+      <c r="GC6" s="14"/>
+      <c r="GD6" s="14"/>
+      <c r="GE6" s="14"/>
+      <c r="GF6" s="14"/>
+      <c r="GG6" s="14"/>
+      <c r="GH6" s="14"/>
+      <c r="GI6" s="14"/>
+      <c r="GJ6" s="14"/>
+      <c r="GK6" s="14"/>
+      <c r="GL6" s="14"/>
+      <c r="GM6" s="14"/>
+      <c r="GN6" s="14"/>
+      <c r="GO6" s="14"/>
+      <c r="GP6" s="14"/>
+      <c r="GQ6" s="14"/>
+      <c r="GR6" s="14"/>
+      <c r="GS6" s="14"/>
+      <c r="GT6" s="14"/>
+      <c r="GU6" s="14"/>
+      <c r="GV6" s="14"/>
+      <c r="GW6" s="14"/>
+      <c r="GX6" s="14"/>
+      <c r="GY6" s="14"/>
+      <c r="GZ6" s="14"/>
+      <c r="HA6" s="14"/>
+      <c r="HB6" s="14"/>
+      <c r="HC6" s="14"/>
+      <c r="HD6" s="14"/>
+      <c r="HE6" s="14"/>
+      <c r="HF6" s="14"/>
+      <c r="HG6" s="14"/>
+      <c r="HH6" s="14"/>
+      <c r="HI6" s="14"/>
+      <c r="HJ6" s="14"/>
+      <c r="HK6" s="14"/>
+      <c r="HL6" s="14"/>
+      <c r="HM6" s="14"/>
+      <c r="HN6" s="14"/>
+      <c r="HO6" s="14"/>
+      <c r="HP6" s="14"/>
+      <c r="HQ6" s="14"/>
+      <c r="HR6" s="14"/>
+      <c r="HS6" s="14"/>
+      <c r="HT6" s="14"/>
+      <c r="HU6" s="14"/>
+      <c r="HV6" s="14"/>
+      <c r="HW6" s="14"/>
+      <c r="HX6" s="14"/>
+      <c r="HY6" s="14"/>
+      <c r="HZ6" s="14"/>
+      <c r="IA6" s="14"/>
+      <c r="IB6" s="14"/>
+      <c r="IC6" s="14"/>
+      <c r="ID6" s="14"/>
+      <c r="IE6" s="14"/>
+      <c r="IF6" s="14"/>
+      <c r="IG6" s="14"/>
+      <c r="IH6" s="14"/>
+      <c r="II6" s="14"/>
+      <c r="IJ6" s="14"/>
+      <c r="IK6" s="14"/>
+      <c r="IL6" s="14"/>
+      <c r="IM6" s="14"/>
+      <c r="IN6" s="14"/>
+      <c r="IO6" s="14"/>
+      <c r="IP6" s="14"/>
+      <c r="IQ6" s="14"/>
+      <c r="IR6" s="14"/>
+      <c r="IS6" s="14"/>
+      <c r="IT6" s="14"/>
+      <c r="IU6" s="14"/>
+      <c r="IV6" s="14"/>
+      <c r="IW6" s="14"/>
+      <c r="IX6" s="14"/>
+      <c r="IY6" s="14"/>
+      <c r="IZ6" s="14"/>
+      <c r="JA6" s="14"/>
+      <c r="JB6" s="14"/>
+      <c r="JC6" s="14"/>
+      <c r="JD6" s="14"/>
+      <c r="JE6" s="14"/>
+      <c r="JF6" s="14"/>
+      <c r="JG6" s="14"/>
+      <c r="JH6" s="14"/>
+      <c r="JI6" s="14"/>
+      <c r="JJ6" s="14"/>
+      <c r="JK6" s="14"/>
+      <c r="JL6" s="14"/>
+      <c r="JM6" s="14"/>
+      <c r="JN6" s="14"/>
+      <c r="JO6" s="14"/>
+      <c r="JP6" s="14"/>
+      <c r="JQ6" s="14"/>
+      <c r="JR6" s="14"/>
+      <c r="JS6" s="14"/>
+      <c r="JT6" s="14"/>
+      <c r="JU6" s="14"/>
+      <c r="JV6" s="14"/>
+      <c r="JW6" s="14"/>
+      <c r="JX6" s="14"/>
+      <c r="JY6" s="14"/>
+      <c r="JZ6" s="14"/>
+      <c r="KA6" s="14"/>
+      <c r="KB6" s="14"/>
+      <c r="KC6" s="14"/>
+      <c r="KD6" s="14"/>
+      <c r="KE6" s="14"/>
+      <c r="KF6" s="14"/>
+      <c r="KG6" s="14"/>
+      <c r="KH6" s="14"/>
+      <c r="KI6" s="14"/>
+      <c r="KJ6" s="14"/>
+      <c r="KK6" s="14"/>
+      <c r="KL6" s="14"/>
+      <c r="KM6" s="14"/>
+      <c r="KN6" s="14"/>
+      <c r="KO6" s="14"/>
+      <c r="KP6" s="14"/>
+      <c r="KQ6" s="14"/>
+      <c r="KR6" s="14"/>
+      <c r="KS6" s="14"/>
+      <c r="KT6" s="14"/>
+      <c r="KU6" s="14"/>
+      <c r="KV6" s="14"/>
+      <c r="KW6" s="14"/>
+      <c r="KX6" s="14"/>
+      <c r="KY6" s="14"/>
+      <c r="KZ6" s="14"/>
+      <c r="LA6" s="14"/>
+      <c r="LB6" s="14"/>
+      <c r="LC6" s="14"/>
+      <c r="LD6" s="14"/>
+      <c r="LE6" s="14"/>
+      <c r="LF6" s="14"/>
+      <c r="LG6" s="14"/>
+      <c r="LH6" s="14"/>
+      <c r="LI6" s="14"/>
+      <c r="LJ6" s="14"/>
+      <c r="LK6" s="14"/>
+      <c r="LL6" s="14"/>
+      <c r="LM6" s="14"/>
+      <c r="LN6" s="14"/>
+      <c r="LO6" s="14"/>
+      <c r="LP6" s="14"/>
+      <c r="LQ6" s="14"/>
+      <c r="LR6" s="14"/>
+      <c r="LS6" s="14"/>
+      <c r="LT6" s="14"/>
+      <c r="LU6" s="14"/>
+      <c r="LV6" s="14"/>
+      <c r="LW6" s="14"/>
+      <c r="LX6" s="14"/>
+      <c r="LY6" s="14"/>
+      <c r="LZ6" s="14"/>
+      <c r="MA6" s="14"/>
+      <c r="MB6" s="14"/>
+      <c r="MC6" s="14"/>
+      <c r="MD6" s="14"/>
+      <c r="ME6" s="14"/>
+      <c r="MF6" s="14"/>
+      <c r="MG6" s="14"/>
+      <c r="MH6" s="14"/>
+      <c r="MI6" s="14"/>
+      <c r="MJ6" s="14"/>
+      <c r="MK6" s="14"/>
+      <c r="ML6" s="14"/>
+      <c r="MM6" s="14"/>
+      <c r="MN6" s="14"/>
+      <c r="MO6" s="14"/>
+      <c r="MP6" s="14"/>
+      <c r="MQ6" s="14"/>
+      <c r="MR6" s="14"/>
+      <c r="MS6" s="14"/>
+      <c r="MT6" s="14"/>
+      <c r="MU6" s="14"/>
+      <c r="MV6" s="14"/>
+      <c r="MW6" s="14"/>
+      <c r="MX6" s="14"/>
+      <c r="MY6" s="14"/>
+      <c r="MZ6" s="14"/>
+      <c r="NA6" s="14"/>
+      <c r="NB6" s="14"/>
+      <c r="NC6" s="14"/>
+      <c r="ND6" s="14"/>
+      <c r="NE6" s="14"/>
+      <c r="NF6" s="14"/>
+      <c r="NG6" s="14"/>
+      <c r="NH6" s="14"/>
+      <c r="NI6" s="14"/>
+      <c r="NJ6" s="14"/>
+      <c r="NK6" s="14"/>
+      <c r="NL6" s="14"/>
+      <c r="NM6" s="14"/>
+      <c r="NN6" s="14"/>
+      <c r="NO6" s="14"/>
+      <c r="NP6" s="14"/>
+      <c r="NQ6" s="14"/>
+      <c r="NR6" s="14"/>
+      <c r="NS6" s="14"/>
+      <c r="NT6" s="14"/>
+      <c r="NU6" s="14"/>
+      <c r="NV6" s="14"/>
+      <c r="NW6" s="14"/>
+      <c r="NX6" s="14"/>
+      <c r="NY6" s="14"/>
+      <c r="NZ6" s="14"/>
+      <c r="OA6" s="14"/>
+      <c r="OB6" s="14"/>
+      <c r="OC6" s="14"/>
+      <c r="OD6" s="14"/>
+      <c r="OE6" s="14"/>
+      <c r="OF6" s="14"/>
+      <c r="OG6" s="14"/>
+      <c r="OH6" s="14"/>
+      <c r="OI6" s="14"/>
+      <c r="OJ6" s="14"/>
+      <c r="OK6" s="14"/>
+      <c r="OL6" s="14"/>
+      <c r="OM6" s="14"/>
+      <c r="ON6" s="14"/>
+      <c r="OO6" s="14"/>
+      <c r="OP6" s="14"/>
+      <c r="OQ6" s="14"/>
+      <c r="OR6" s="14"/>
+      <c r="OS6" s="14"/>
+      <c r="OT6" s="14"/>
+      <c r="OU6" s="14"/>
+      <c r="OV6" s="14"/>
+      <c r="OW6" s="14"/>
+      <c r="OX6" s="14"/>
+      <c r="OY6" s="14"/>
+      <c r="OZ6" s="14"/>
+      <c r="PA6" s="14"/>
+      <c r="PB6" s="14"/>
+      <c r="PC6" s="14"/>
+      <c r="PD6" s="14"/>
+      <c r="PE6" s="14"/>
+      <c r="PF6" s="14"/>
+      <c r="PG6" s="14"/>
+      <c r="PH6" s="14"/>
+      <c r="PI6" s="14"/>
+      <c r="PJ6" s="14"/>
+      <c r="PK6" s="14"/>
+      <c r="PL6" s="14"/>
+      <c r="PM6" s="14"/>
+      <c r="PN6" s="14"/>
+      <c r="PO6" s="14"/>
+      <c r="PP6" s="14"/>
+      <c r="PQ6" s="14"/>
+      <c r="PR6" s="14"/>
+      <c r="PS6" s="14"/>
+      <c r="PT6" s="14"/>
+      <c r="PU6" s="14"/>
+      <c r="PV6" s="14"/>
+      <c r="PW6" s="14"/>
+      <c r="PX6" s="14"/>
+      <c r="PY6" s="14"/>
+      <c r="PZ6" s="14"/>
+      <c r="QA6" s="14"/>
+      <c r="QB6" s="14"/>
+      <c r="QC6" s="14"/>
+      <c r="QD6" s="14"/>
+      <c r="QE6" s="14"/>
+      <c r="QF6" s="14"/>
+      <c r="QG6" s="14"/>
+      <c r="QH6" s="14"/>
+      <c r="QI6" s="14"/>
+      <c r="QJ6" s="14"/>
+      <c r="QK6" s="14"/>
+      <c r="QL6" s="14"/>
+      <c r="QM6" s="14"/>
+      <c r="QN6" s="14"/>
+      <c r="QO6" s="14"/>
+      <c r="QP6" s="14"/>
+      <c r="QQ6" s="14"/>
+      <c r="QR6" s="14"/>
+      <c r="QS6" s="14"/>
+      <c r="QT6" s="14"/>
+      <c r="QU6" s="14"/>
+      <c r="QV6" s="14"/>
+      <c r="QW6" s="14"/>
+      <c r="QX6" s="14"/>
+      <c r="QY6" s="14"/>
+      <c r="QZ6" s="14"/>
+      <c r="RA6" s="14"/>
+      <c r="RB6" s="14"/>
+      <c r="RC6" s="14"/>
+      <c r="RD6" s="14"/>
+      <c r="RE6" s="14"/>
+      <c r="RF6" s="14"/>
+      <c r="RG6" s="14"/>
+      <c r="RH6" s="14"/>
+      <c r="RI6" s="14"/>
+      <c r="RJ6" s="14"/>
+      <c r="RK6" s="14"/>
+      <c r="RL6" s="14"/>
+      <c r="RM6" s="14"/>
+      <c r="RN6" s="14"/>
+      <c r="RO6" s="14"/>
+      <c r="RP6" s="14"/>
+      <c r="RQ6" s="14"/>
+      <c r="RR6" s="14"/>
+      <c r="RS6" s="14"/>
+      <c r="RT6" s="14"/>
+      <c r="RU6" s="14"/>
+      <c r="RV6" s="14"/>
+      <c r="RW6" s="14"/>
+      <c r="RX6" s="14"/>
+      <c r="RY6" s="14"/>
+      <c r="RZ6" s="14"/>
+      <c r="SA6" s="14"/>
+      <c r="SB6" s="14"/>
+      <c r="SC6" s="14"/>
+      <c r="SD6" s="14"/>
+      <c r="SE6" s="14"/>
+      <c r="SF6" s="14"/>
+      <c r="SG6" s="14"/>
+      <c r="SH6" s="14"/>
+      <c r="SI6" s="14"/>
+      <c r="SJ6" s="14"/>
+      <c r="SK6" s="14"/>
+      <c r="SL6" s="14"/>
+      <c r="SM6" s="14"/>
+      <c r="SN6" s="14"/>
+      <c r="SO6" s="14"/>
+      <c r="SP6" s="14"/>
+      <c r="SQ6" s="14"/>
+      <c r="SR6" s="14"/>
+      <c r="SS6" s="14"/>
+      <c r="ST6" s="14"/>
+      <c r="SU6" s="14"/>
+      <c r="SV6" s="14"/>
+      <c r="SW6" s="14"/>
+      <c r="SX6" s="14"/>
+      <c r="SY6" s="14"/>
+      <c r="SZ6" s="14"/>
+      <c r="TA6" s="14"/>
+      <c r="TB6" s="14"/>
+      <c r="TC6" s="14"/>
+      <c r="TD6" s="14"/>
+      <c r="TE6" s="14"/>
+      <c r="TF6" s="14"/>
+      <c r="TG6" s="14"/>
+      <c r="TH6" s="14"/>
+      <c r="TI6" s="14"/>
+      <c r="TJ6" s="14"/>
+      <c r="TK6" s="14"/>
+      <c r="TL6" s="14"/>
+      <c r="TM6" s="14"/>
+      <c r="TN6" s="14"/>
+      <c r="TO6" s="14"/>
+      <c r="TP6" s="14"/>
+      <c r="TQ6" s="14"/>
+      <c r="TR6" s="14"/>
+      <c r="TS6" s="14"/>
+      <c r="TT6" s="14"/>
+      <c r="TU6" s="14"/>
+      <c r="TV6" s="14"/>
+      <c r="TW6" s="14"/>
+      <c r="TX6" s="14"/>
+      <c r="TY6" s="14"/>
+      <c r="TZ6" s="14"/>
+      <c r="UA6" s="14"/>
+      <c r="UB6" s="14"/>
+      <c r="UC6" s="14"/>
+      <c r="UD6" s="14"/>
+      <c r="UE6" s="14"/>
+      <c r="UF6" s="14"/>
+      <c r="UG6" s="14"/>
+      <c r="UH6" s="14"/>
+      <c r="UI6" s="14"/>
+      <c r="UJ6" s="14"/>
+      <c r="UK6" s="14"/>
+      <c r="UL6" s="14"/>
+      <c r="UM6" s="14"/>
+      <c r="UN6" s="14"/>
+      <c r="UO6" s="14"/>
+      <c r="UP6" s="14"/>
+      <c r="UQ6" s="14"/>
+      <c r="UR6" s="14"/>
+      <c r="US6" s="14"/>
+      <c r="UT6" s="14"/>
+      <c r="UU6" s="14"/>
+      <c r="UV6" s="14"/>
+      <c r="UW6" s="14"/>
+      <c r="UX6" s="14"/>
+      <c r="UY6" s="14"/>
+      <c r="UZ6" s="14"/>
+      <c r="VA6" s="14"/>
+      <c r="VB6" s="14"/>
+      <c r="VC6" s="14"/>
+      <c r="VD6" s="14"/>
+      <c r="VE6" s="14"/>
+      <c r="VF6" s="14"/>
+      <c r="VG6" s="14"/>
+      <c r="VH6" s="14"/>
+      <c r="VI6" s="14"/>
+      <c r="VJ6" s="14"/>
+      <c r="VK6" s="14"/>
+      <c r="VL6" s="14"/>
+      <c r="VM6" s="14"/>
+      <c r="VN6" s="14"/>
+      <c r="VO6" s="14"/>
+      <c r="VP6" s="14"/>
+      <c r="VQ6" s="14"/>
+      <c r="VR6" s="14"/>
+      <c r="VS6" s="14"/>
+      <c r="VT6" s="14"/>
+      <c r="VU6" s="14"/>
+      <c r="VV6" s="14"/>
+      <c r="VW6" s="14"/>
+      <c r="VX6" s="14"/>
+      <c r="VY6" s="14"/>
+      <c r="VZ6" s="14"/>
+      <c r="WA6" s="14"/>
+      <c r="WB6" s="14"/>
+      <c r="WC6" s="14"/>
+      <c r="WD6" s="14"/>
+      <c r="WE6" s="14"/>
+      <c r="WF6" s="14"/>
+      <c r="WG6" s="14"/>
+      <c r="WH6" s="14"/>
+      <c r="WI6" s="14"/>
+      <c r="WJ6" s="14"/>
+      <c r="WK6" s="14"/>
+      <c r="WL6" s="14"/>
+      <c r="WM6" s="14"/>
+      <c r="WN6" s="14"/>
+      <c r="WO6" s="14"/>
+      <c r="WP6" s="14"/>
+      <c r="WQ6" s="14"/>
+      <c r="WR6" s="14"/>
+      <c r="WS6" s="14"/>
+      <c r="WT6" s="14"/>
+      <c r="WU6" s="14"/>
+      <c r="WV6" s="14"/>
+      <c r="WW6" s="14"/>
+      <c r="WX6" s="14"/>
+      <c r="WY6" s="14"/>
+      <c r="WZ6" s="14"/>
+      <c r="XA6" s="14"/>
+      <c r="XB6" s="14"/>
+      <c r="XC6" s="14"/>
+      <c r="XD6" s="14"/>
+      <c r="XE6" s="14"/>
+      <c r="XF6" s="14"/>
+      <c r="XG6" s="14"/>
+      <c r="XH6" s="14"/>
+      <c r="XI6" s="14"/>
+      <c r="XJ6" s="14"/>
+      <c r="XK6" s="14"/>
+      <c r="XL6" s="14"/>
+      <c r="XM6" s="14"/>
+      <c r="XN6" s="14"/>
+      <c r="XO6" s="14"/>
+      <c r="XP6" s="14"/>
+      <c r="XQ6" s="14"/>
+      <c r="XR6" s="14"/>
+      <c r="XS6" s="14"/>
+      <c r="XT6" s="14"/>
+      <c r="XU6" s="14"/>
+      <c r="XV6" s="14"/>
+      <c r="XW6" s="14"/>
+      <c r="XX6" s="14"/>
+      <c r="XY6" s="14"/>
+      <c r="XZ6" s="14"/>
+      <c r="YA6" s="14"/>
+      <c r="YB6" s="14"/>
+      <c r="YC6" s="14"/>
+      <c r="YD6" s="14"/>
+      <c r="YE6" s="14"/>
+      <c r="YF6" s="14"/>
+      <c r="YG6" s="14"/>
+      <c r="YH6" s="14"/>
+      <c r="YI6" s="14"/>
+      <c r="YJ6" s="14"/>
+      <c r="YK6" s="14"/>
+      <c r="YL6" s="14"/>
+      <c r="YM6" s="14"/>
+      <c r="YN6" s="14"/>
+      <c r="YO6" s="14"/>
+      <c r="YP6" s="14"/>
+      <c r="YQ6" s="14"/>
+      <c r="YR6" s="14"/>
+      <c r="YS6" s="14"/>
+      <c r="YT6" s="14"/>
+      <c r="YU6" s="14"/>
+      <c r="YV6" s="14"/>
+      <c r="YW6" s="14"/>
+      <c r="YX6" s="14"/>
+      <c r="YY6" s="14"/>
+      <c r="YZ6" s="14"/>
+      <c r="ZA6" s="14"/>
+      <c r="ZB6" s="14"/>
+      <c r="ZC6" s="14"/>
+      <c r="ZD6" s="14"/>
+      <c r="ZE6" s="14"/>
+      <c r="ZF6" s="14"/>
+      <c r="ZG6" s="14"/>
+      <c r="ZH6" s="14"/>
+      <c r="ZI6" s="14"/>
+      <c r="ZJ6" s="14"/>
+      <c r="ZK6" s="14"/>
+      <c r="ZL6" s="14"/>
+      <c r="ZM6" s="14"/>
+      <c r="ZN6" s="14"/>
+      <c r="ZO6" s="14"/>
+      <c r="ZP6" s="14"/>
+      <c r="ZQ6" s="14"/>
+      <c r="ZR6" s="14"/>
+      <c r="ZS6" s="14"/>
+      <c r="ZT6" s="14"/>
+      <c r="ZU6" s="14"/>
+      <c r="ZV6" s="14"/>
+      <c r="ZW6" s="14"/>
+      <c r="ZX6" s="14"/>
+      <c r="ZY6" s="14"/>
+      <c r="ZZ6" s="14"/>
+      <c r="AAA6" s="14"/>
+      <c r="AAB6" s="14"/>
+      <c r="AAC6" s="14"/>
+      <c r="AAD6" s="14"/>
+      <c r="AAE6" s="14"/>
+      <c r="AAF6" s="14"/>
+      <c r="AAG6" s="14"/>
+      <c r="AAH6" s="14"/>
+      <c r="AAI6" s="14"/>
+      <c r="AAJ6" s="14"/>
+      <c r="AAK6" s="14"/>
+      <c r="AAL6" s="14"/>
+      <c r="AAM6" s="14"/>
+      <c r="AAN6" s="14"/>
+      <c r="AAO6" s="14"/>
+      <c r="AAP6" s="14"/>
+      <c r="AAQ6" s="14"/>
+      <c r="AAR6" s="14"/>
+      <c r="AAS6" s="14"/>
+      <c r="AAT6" s="14"/>
+      <c r="AAU6" s="14"/>
+      <c r="AAV6" s="14"/>
+      <c r="AAW6" s="14"/>
+      <c r="AAX6" s="14"/>
+      <c r="AAY6" s="14"/>
+      <c r="AAZ6" s="14"/>
+      <c r="ABA6" s="14"/>
+      <c r="ABB6" s="14"/>
+      <c r="ABC6" s="14"/>
+      <c r="ABD6" s="14"/>
+      <c r="ABE6" s="14"/>
+      <c r="ABF6" s="14"/>
+      <c r="ABG6" s="14"/>
+      <c r="ABH6" s="14"/>
+      <c r="ABI6" s="14"/>
+      <c r="ABJ6" s="14"/>
+      <c r="ABK6" s="14"/>
+      <c r="ABL6" s="14"/>
+      <c r="ABM6" s="14"/>
+      <c r="ABN6" s="14"/>
+      <c r="ABO6" s="14"/>
+      <c r="ABP6" s="14"/>
+      <c r="ABQ6" s="14"/>
+      <c r="ABR6" s="14"/>
+      <c r="ABS6" s="14"/>
+      <c r="ABT6" s="14"/>
+      <c r="ABU6" s="14"/>
+      <c r="ABV6" s="14"/>
+      <c r="ABW6" s="14"/>
+      <c r="ABX6" s="14"/>
+      <c r="ABY6" s="14"/>
+      <c r="ABZ6" s="14"/>
+      <c r="ACA6" s="14"/>
+      <c r="ACB6" s="14"/>
+      <c r="ACC6" s="14"/>
+      <c r="ACD6" s="14"/>
+      <c r="ACE6" s="14"/>
+      <c r="ACF6" s="14"/>
+      <c r="ACG6" s="14"/>
+      <c r="ACH6" s="14"/>
+      <c r="ACI6" s="14"/>
+      <c r="ACJ6" s="14"/>
+      <c r="ACK6" s="14"/>
+      <c r="ACL6" s="14"/>
+      <c r="ACM6" s="14"/>
+      <c r="ACN6" s="14"/>
+      <c r="ACO6" s="14"/>
+      <c r="ACP6" s="14"/>
+      <c r="ACQ6" s="14"/>
+      <c r="ACR6" s="14"/>
+      <c r="ACS6" s="14"/>
+      <c r="ACT6" s="14"/>
+      <c r="ACU6" s="14"/>
+      <c r="ACV6" s="14"/>
+      <c r="ACW6" s="14"/>
+      <c r="ACX6" s="14"/>
+      <c r="ACY6" s="14"/>
+      <c r="ACZ6" s="14"/>
+      <c r="ADA6" s="14"/>
+      <c r="ADB6" s="14"/>
+      <c r="ADC6" s="14"/>
+      <c r="ADD6" s="14"/>
+      <c r="ADE6" s="14"/>
+      <c r="ADF6" s="14"/>
+      <c r="ADG6" s="14"/>
+      <c r="ADH6" s="14"/>
+      <c r="ADI6" s="14"/>
+      <c r="ADJ6" s="14"/>
+      <c r="ADK6" s="14"/>
+      <c r="ADL6" s="14"/>
+      <c r="ADM6" s="14"/>
+      <c r="ADN6" s="14"/>
+      <c r="ADO6" s="14"/>
+      <c r="ADP6" s="14"/>
+      <c r="ADQ6" s="14"/>
+      <c r="ADR6" s="14"/>
+      <c r="ADS6" s="14"/>
+      <c r="ADT6" s="14"/>
+      <c r="ADU6" s="14"/>
+      <c r="ADV6" s="14"/>
+      <c r="ADW6" s="14"/>
+      <c r="ADX6" s="14"/>
+      <c r="ADY6" s="14"/>
+      <c r="ADZ6" s="14"/>
+      <c r="AEA6" s="14"/>
+      <c r="AEB6" s="14"/>
+      <c r="AEC6" s="14"/>
+      <c r="AED6" s="14"/>
+      <c r="AEE6" s="14"/>
+      <c r="AEF6" s="14"/>
+      <c r="AEG6" s="14"/>
+      <c r="AEH6" s="14"/>
+      <c r="AEI6" s="14"/>
+      <c r="AEJ6" s="14"/>
+      <c r="AEK6" s="14"/>
+      <c r="AEL6" s="14"/>
+      <c r="AEM6" s="14"/>
+      <c r="AEN6" s="14"/>
+      <c r="AEO6" s="14"/>
+      <c r="AEP6" s="14"/>
+      <c r="AEQ6" s="14"/>
+      <c r="AER6" s="14"/>
+      <c r="AES6" s="14"/>
+      <c r="AET6" s="14"/>
+      <c r="AEU6" s="14"/>
+      <c r="AEV6" s="14"/>
+      <c r="AEW6" s="14"/>
+      <c r="AEX6" s="14"/>
+      <c r="AEY6" s="14"/>
+      <c r="AEZ6" s="14"/>
+      <c r="AFA6" s="14"/>
+      <c r="AFB6" s="14"/>
+      <c r="AFC6" s="14"/>
+      <c r="AFD6" s="14"/>
+      <c r="AFE6" s="14"/>
+      <c r="AFF6" s="14"/>
+      <c r="AFG6" s="14"/>
+      <c r="AFH6" s="14"/>
+      <c r="AFI6" s="14"/>
+      <c r="AFJ6" s="14"/>
+      <c r="AFK6" s="14"/>
+      <c r="AFL6" s="14"/>
+      <c r="AFM6" s="14"/>
+      <c r="AFN6" s="14"/>
+      <c r="AFO6" s="14"/>
+      <c r="AFP6" s="14"/>
+      <c r="AFQ6" s="14"/>
+      <c r="AFR6" s="14"/>
+      <c r="AFS6" s="14"/>
+      <c r="AFT6" s="14"/>
+      <c r="AFU6" s="14"/>
+      <c r="AFV6" s="14"/>
+      <c r="AFW6" s="14"/>
+      <c r="AFX6" s="14"/>
+      <c r="AFY6" s="14"/>
+      <c r="AFZ6" s="14"/>
+      <c r="AGA6" s="14"/>
+      <c r="AGB6" s="14"/>
+      <c r="AGC6" s="14"/>
+      <c r="AGD6" s="14"/>
+      <c r="AGE6" s="14"/>
+      <c r="AGF6" s="14"/>
+      <c r="AGG6" s="14"/>
+      <c r="AGH6" s="14"/>
+      <c r="AGI6" s="14"/>
+      <c r="AGJ6" s="14"/>
+      <c r="AGK6" s="14"/>
+      <c r="AGL6" s="14"/>
+      <c r="AGM6" s="14"/>
+      <c r="AGN6" s="14"/>
+      <c r="AGO6" s="14"/>
+      <c r="AGP6" s="14"/>
+      <c r="AGQ6" s="14"/>
+      <c r="AGR6" s="14"/>
+      <c r="AGS6" s="14"/>
+      <c r="AGT6" s="14"/>
+      <c r="AGU6" s="14"/>
+      <c r="AGV6" s="14"/>
+      <c r="AGW6" s="14"/>
+      <c r="AGX6" s="14"/>
+      <c r="AGY6" s="14"/>
+      <c r="AGZ6" s="14"/>
+      <c r="AHA6" s="14"/>
+      <c r="AHB6" s="14"/>
+      <c r="AHC6" s="14"/>
+      <c r="AHD6" s="14"/>
+      <c r="AHE6" s="14"/>
+      <c r="AHF6" s="14"/>
+      <c r="AHG6" s="14"/>
+      <c r="AHH6" s="14"/>
+      <c r="AHI6" s="14"/>
+      <c r="AHJ6" s="14"/>
+      <c r="AHK6" s="14"/>
+      <c r="AHL6" s="14"/>
+      <c r="AHM6" s="14"/>
+      <c r="AHN6" s="14"/>
+      <c r="AHO6" s="14"/>
+      <c r="AHP6" s="14"/>
+      <c r="AHQ6" s="14"/>
+      <c r="AHR6" s="14"/>
+      <c r="AHS6" s="14"/>
+      <c r="AHT6" s="14"/>
+      <c r="AHU6" s="14"/>
+      <c r="AHV6" s="14"/>
+      <c r="AHW6" s="14"/>
+      <c r="AHX6" s="14"/>
+      <c r="AHY6" s="14"/>
+      <c r="AHZ6" s="14"/>
+      <c r="AIA6" s="14"/>
+      <c r="AIB6" s="14"/>
+      <c r="AIC6" s="14"/>
+      <c r="AID6" s="14"/>
+      <c r="AIE6" s="14"/>
+      <c r="AIF6" s="14"/>
+      <c r="AIG6" s="14"/>
+      <c r="AIH6" s="14"/>
+      <c r="AII6" s="14"/>
+      <c r="AIJ6" s="14"/>
+      <c r="AIK6" s="14"/>
+      <c r="AIL6" s="14"/>
+      <c r="AIM6" s="14"/>
+      <c r="AIN6" s="14"/>
+      <c r="AIO6" s="14"/>
+      <c r="AIP6" s="14"/>
+      <c r="AIQ6" s="14"/>
+      <c r="AIR6" s="14"/>
+      <c r="AIS6" s="14"/>
+      <c r="AIT6" s="14"/>
+      <c r="AIU6" s="14"/>
+      <c r="AIV6" s="14"/>
+      <c r="AIW6" s="14"/>
+      <c r="AIX6" s="14"/>
+      <c r="AIY6" s="14"/>
+      <c r="AIZ6" s="14"/>
+      <c r="AJA6" s="14"/>
+      <c r="AJB6" s="14"/>
+      <c r="AJC6" s="14"/>
+      <c r="AJD6" s="14"/>
+      <c r="AJE6" s="14"/>
+      <c r="AJF6" s="14"/>
+      <c r="AJG6" s="14"/>
+      <c r="AJH6" s="14"/>
+      <c r="AJI6" s="14"/>
+      <c r="AJJ6" s="14"/>
+      <c r="AJK6" s="14"/>
+      <c r="AJL6" s="14"/>
+      <c r="AJM6" s="14"/>
+      <c r="AJN6" s="14"/>
+      <c r="AJO6" s="14"/>
+      <c r="AJP6" s="14"/>
+      <c r="AJQ6" s="14"/>
+      <c r="AJR6" s="14"/>
+      <c r="AJS6" s="14"/>
+      <c r="AJT6" s="14"/>
+      <c r="AJU6" s="14"/>
+      <c r="AJV6" s="14"/>
+      <c r="AJW6" s="14"/>
+      <c r="AJX6" s="14"/>
+      <c r="AJY6" s="14"/>
+      <c r="AJZ6" s="14"/>
+      <c r="AKA6" s="14"/>
+      <c r="AKB6" s="14"/>
+      <c r="AKC6" s="14"/>
+      <c r="AKD6" s="14"/>
+      <c r="AKE6" s="14"/>
+      <c r="AKF6" s="14"/>
+      <c r="AKG6" s="14"/>
+      <c r="AKH6" s="14"/>
+      <c r="AKI6" s="14"/>
+      <c r="AKJ6" s="14"/>
+      <c r="AKK6" s="14"/>
+      <c r="AKL6" s="14"/>
+      <c r="AKM6" s="14"/>
+      <c r="AKN6" s="14"/>
+      <c r="AKO6" s="14"/>
+      <c r="AKP6" s="14"/>
+      <c r="AKQ6" s="14"/>
+      <c r="AKR6" s="14"/>
+      <c r="AKS6" s="14"/>
+      <c r="AKT6" s="14"/>
+      <c r="AKU6" s="14"/>
+      <c r="AKV6" s="14"/>
+      <c r="AKW6" s="14"/>
+      <c r="AKX6" s="14"/>
+      <c r="AKY6" s="14"/>
+      <c r="AKZ6" s="14"/>
+      <c r="ALA6" s="14"/>
+      <c r="ALB6" s="14"/>
+      <c r="ALC6" s="14"/>
+      <c r="ALD6" s="14"/>
+      <c r="ALE6" s="14"/>
+      <c r="ALF6" s="14"/>
+      <c r="ALG6" s="14"/>
+      <c r="ALH6" s="14"/>
+      <c r="ALI6" s="14"/>
+      <c r="ALJ6" s="14"/>
+      <c r="ALK6" s="14"/>
+      <c r="ALL6" s="14"/>
+      <c r="ALM6" s="14"/>
+      <c r="ALN6" s="14"/>
+      <c r="ALO6" s="14"/>
+      <c r="ALP6" s="14"/>
+      <c r="ALQ6" s="14"/>
+      <c r="ALR6" s="14"/>
+      <c r="ALS6" s="14"/>
+      <c r="ALT6" s="14"/>
+      <c r="ALU6" s="14"/>
+      <c r="ALV6" s="14"/>
+      <c r="ALW6" s="14"/>
+      <c r="ALX6" s="14"/>
+      <c r="ALY6" s="14"/>
+      <c r="ALZ6" s="14"/>
+      <c r="AMA6" s="14"/>
+      <c r="AMB6" s="14"/>
+      <c r="AMC6" s="14"/>
+      <c r="AMD6" s="14"/>
+      <c r="AME6" s="14"/>
+      <c r="AMF6" s="14"/>
+      <c r="AMG6" s="14"/>
+      <c r="AMH6" s="14"/>
+      <c r="AMI6" s="14"/>
+      <c r="AMJ6" s="15"/>
+    </row>
+    <row r="7" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="s">
         <v>27</v>
-      </c>
-      <c r="AMJ6" s="15"/>
-    </row>
-    <row r="7" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
-        <v>28</v>
       </c>
       <c r="B7" s="22"/>
       <c r="C7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AMJ7" s="15"/>
+    </row>
+    <row r="8" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
         <v>29</v>
-      </c>
-      <c r="AMJ7" s="15"/>
-    </row>
-    <row r="8" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
-        <v>30</v>
       </c>
       <c r="B8" s="22" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="AMJ8" s="15"/>
+    </row>
+    <row r="9" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="AMJ8" s="15"/>
-    </row>
-    <row r="9" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="s">
-        <v>32</v>
       </c>
       <c r="B9" s="22" t="n">
         <v>10</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AMJ9" s="15"/>
+    </row>
+    <row r="10" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="AMJ9" s="15"/>
-    </row>
-    <row r="10" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
-        <v>34</v>
       </c>
       <c r="B10" s="22" t="n">
         <v>42000</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AMJ10" s="15"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="http://localhost:5531"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2400,16 +3432,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="D1" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,7 +3450,7 @@
         <v>/path/from/audio/folder</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="32" t="n">
         <v>45089.8854166667</v>
@@ -2487,18 +3519,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="29" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="34" t="n">
         <v>20</v>
@@ -2556,15 +3588,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="34" t="n">
         <v>15</v>
@@ -2616,18 +3648,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="35" t="n">
         <v>44927</v>
@@ -2677,22 +3709,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>53</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2765,16 +3797,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="41" t="s">
         <v>56</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>57</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -3788,7 +4820,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="39" t="n">
         <v>0</v>
@@ -3797,7 +4829,7 @@
         <v>1000</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3838,22 +4870,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(Examples/DefaultConfig): Center file headers
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -1283,7 +1283,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1394,10 +1394,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1708,48 +1704,48 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="39" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="39" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="39" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="38" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="38" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="38" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="42" t="s">
         <v>67</v>
       </c>
       <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="40" t="n">
+      <c r="B2" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="39" t="n">
+      <c r="B3" s="38" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1793,46 +1789,46 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="39" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="39" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="39" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="40" t="s">
         <v>73</v>
       </c>
       <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="40" t="n">
+      <c r="B2" s="39" t="n">
         <v>50</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="40" t="n">
+      <c r="D2" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="40" t="n">
+      <c r="E2" s="39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1876,88 +1872,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="49" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="49" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="49" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1990,85 +1986,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="48" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="48" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="50"/>
+      <c r="B10" s="49"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2099,32 +2095,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2157,22 +2153,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2201,27 +2197,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3440,19 +3436,19 @@
       <c r="C1" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="str">
+      <c r="A2" s="29" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="32" t="n">
+      <c r="C2" s="31" t="n">
         <v>45089.8854166667</v>
       </c>
       <c r="D2" s="26" t="s">
@@ -3460,27 +3456,27 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="31"/>
+      <c r="C7" s="30"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3512,30 +3508,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="34" t="n">
+      <c r="B2" s="33" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="34" t="n">
+      <c r="C2" s="33" t="n">
         <v>20000</v>
       </c>
     </row>
@@ -3581,24 +3577,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="34" t="n">
+      <c r="B2" s="33" t="n">
         <v>15</v>
       </c>
     </row>
@@ -3641,30 +3637,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="20.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="35" t="n">
+      <c r="B2" s="34" t="n">
         <v>44927</v>
       </c>
-      <c r="C2" s="35" t="n">
+      <c r="C2" s="34" t="n">
         <v>45292</v>
       </c>
     </row>
@@ -3701,60 +3697,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="34" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="33" width="18.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3788,24 +3784,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="10.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="39" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="39" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="15.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="5" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>56</v>
       </c>
       <c r="E1" s="3"/>
@@ -4819,16 +4815,16 @@
       <c r="ALY1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="39" t="n">
+      <c r="B2" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="40" t="n">
+      <c r="C2" s="39" t="n">
         <v>1000</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4864,27 +4860,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="42" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="41" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(Examples/DefaultConfig): Update audio host example
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -721,7 +721,28 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">The host name serving your audio files. Example: `http://localhost:5531`
+      <t xml:space="preserve">The host name serving your audio files. Example: `</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://localhost:5531/</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">`
 </t>
     </r>
     <r>
@@ -1097,7 +1118,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1158,6 +1179,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -1452,7 +1481,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3390,6 +3419,9 @@
       <c r="AMJ10" s="15"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" display="http://localhost:5531/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3572,7 +3604,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat(Examples/Config): Add VLOOKUP descriptors
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -713,49 +713,8 @@
     <t xml:space="preserve">audio_host</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The host name serving your audio files. Example: `</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://localhost:5531/</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">`
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional</t>
-    </r>
+    <t xml:space="preserve">The host name serving your audio files. Example: `http://localhost:5531/`
+Optional</t>
   </si>
   <si>
     <t xml:space="preserve">timezone</t>
@@ -1118,7 +1077,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1192,6 +1151,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1312,7 +1277,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1401,6 +1366,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1449,6 +1418,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1473,6 +1446,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1481,7 +1458,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1725,56 +1706,57 @@
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="38" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="38" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="38" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="39" t="n">
+      <c r="B2" s="41" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="38" t="n">
+      <c r="B3" s="40" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1806,58 +1788,55 @@
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="39" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="39" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="41" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="41" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="41" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="39" t="n">
+      <c r="B2" s="41" t="n">
         <v>50</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="39" t="n">
+      <c r="D2" s="41" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="39" t="n">
+      <c r="E2" s="41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1901,88 +1880,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="51" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="52" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="52" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="52" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="52" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="52" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="53" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="53" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="53" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="53" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2015,85 +1994,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="51" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="52" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="52" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="52" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="52" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="52" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="52" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="52" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="52" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="49"/>
+      <c r="B10" s="53"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2124,32 +2103,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="48" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="48" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2182,22 +2161,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2226,27 +2205,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="16.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="48" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="48" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2270,11 +2249,9 @@
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2347,7 +2324,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="14"/>
@@ -3376,7 +3353,7 @@
       <c r="A7" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
@@ -3386,7 +3363,7 @@
       <c r="A8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="22" t="n">
+      <c r="B8" s="23" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="18" t="s">
@@ -3398,7 +3375,7 @@
       <c r="A9" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="22" t="n">
+      <c r="B9" s="23" t="n">
         <v>10</v>
       </c>
       <c r="C9" s="18" t="s">
@@ -3410,7 +3387,7 @@
       <c r="A10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="22" t="n">
+      <c r="B10" s="23" t="n">
         <v>42000</v>
       </c>
       <c r="C10" s="18" t="s">
@@ -3420,7 +3397,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" display="http://localhost:5531/"/>
+    <hyperlink ref="C6" r:id="rId1" display="The host name serving your audio files. Example: `http://localhost:5531/`&#10;Optional"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3441,74 +3418,72 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="5" style="27" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="5" style="28" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1003" min="29" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="29" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="str">
+      <c r="A2" s="30" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="31" t="n">
+      <c r="C2" s="32" t="n">
         <v>45089.8854166667</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="27" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="30"/>
+      <c r="C7" s="31"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3531,53 +3506,51 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="33" t="n">
+      <c r="B2" s="34" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="33" t="n">
+      <c r="C2" s="34" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3600,44 +3573,42 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="33" t="n">
+      <c r="B2" s="34" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="26"/>
+      <c r="B4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="26"/>
+      <c r="B5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="26"/>
+      <c r="B6" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3660,48 +3631,47 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="20.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1018" style="35" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="34" t="n">
+      <c r="B2" s="36" t="n">
         <v>44927</v>
       </c>
-      <c r="C2" s="34" t="n">
+      <c r="C2" s="36" t="n">
         <v>45292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="26"/>
+      <c r="C4" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3724,65 +3694,67 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="33" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="34" width="18.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="29" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3808,1056 +3780,55 @@
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:ALY2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="10.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="39" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="15.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="41" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="41" width="15.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="42" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1014" style="35" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
-      <c r="AZ1" s="3"/>
-      <c r="BA1" s="3"/>
-      <c r="BB1" s="3"/>
-      <c r="BC1" s="3"/>
-      <c r="BD1" s="3"/>
-      <c r="BE1" s="3"/>
-      <c r="BF1" s="3"/>
-      <c r="BG1" s="3"/>
-      <c r="BH1" s="3"/>
-      <c r="BI1" s="3"/>
-      <c r="BJ1" s="3"/>
-      <c r="BK1" s="3"/>
-      <c r="BL1" s="3"/>
-      <c r="BM1" s="3"/>
-      <c r="BN1" s="3"/>
-      <c r="BO1" s="3"/>
-      <c r="BP1" s="3"/>
-      <c r="BQ1" s="3"/>
-      <c r="BR1" s="3"/>
-      <c r="BS1" s="3"/>
-      <c r="BT1" s="3"/>
-      <c r="BU1" s="3"/>
-      <c r="BV1" s="3"/>
-      <c r="BW1" s="3"/>
-      <c r="BX1" s="3"/>
-      <c r="BY1" s="3"/>
-      <c r="BZ1" s="3"/>
-      <c r="CA1" s="3"/>
-      <c r="CB1" s="3"/>
-      <c r="CC1" s="3"/>
-      <c r="CD1" s="3"/>
-      <c r="CE1" s="3"/>
-      <c r="CF1" s="3"/>
-      <c r="CG1" s="3"/>
-      <c r="CH1" s="3"/>
-      <c r="CI1" s="3"/>
-      <c r="CJ1" s="3"/>
-      <c r="CK1" s="3"/>
-      <c r="CL1" s="3"/>
-      <c r="CM1" s="3"/>
-      <c r="CN1" s="3"/>
-      <c r="CO1" s="3"/>
-      <c r="CP1" s="3"/>
-      <c r="CQ1" s="3"/>
-      <c r="CR1" s="3"/>
-      <c r="CS1" s="3"/>
-      <c r="CT1" s="3"/>
-      <c r="CU1" s="3"/>
-      <c r="CV1" s="3"/>
-      <c r="CW1" s="3"/>
-      <c r="CX1" s="3"/>
-      <c r="CY1" s="3"/>
-      <c r="CZ1" s="3"/>
-      <c r="DA1" s="3"/>
-      <c r="DB1" s="3"/>
-      <c r="DC1" s="3"/>
-      <c r="DD1" s="3"/>
-      <c r="DE1" s="3"/>
-      <c r="DF1" s="3"/>
-      <c r="DG1" s="3"/>
-      <c r="DH1" s="3"/>
-      <c r="DI1" s="3"/>
-      <c r="DJ1" s="3"/>
-      <c r="DK1" s="3"/>
-      <c r="DL1" s="3"/>
-      <c r="DM1" s="3"/>
-      <c r="DN1" s="3"/>
-      <c r="DO1" s="3"/>
-      <c r="DP1" s="3"/>
-      <c r="DQ1" s="3"/>
-      <c r="DR1" s="3"/>
-      <c r="DS1" s="3"/>
-      <c r="DT1" s="3"/>
-      <c r="DU1" s="3"/>
-      <c r="DV1" s="3"/>
-      <c r="DW1" s="3"/>
-      <c r="DX1" s="3"/>
-      <c r="DY1" s="3"/>
-      <c r="DZ1" s="3"/>
-      <c r="EA1" s="3"/>
-      <c r="EB1" s="3"/>
-      <c r="EC1" s="3"/>
-      <c r="ED1" s="3"/>
-      <c r="EE1" s="3"/>
-      <c r="EF1" s="3"/>
-      <c r="EG1" s="3"/>
-      <c r="EH1" s="3"/>
-      <c r="EI1" s="3"/>
-      <c r="EJ1" s="3"/>
-      <c r="EK1" s="3"/>
-      <c r="EL1" s="3"/>
-      <c r="EM1" s="3"/>
-      <c r="EN1" s="3"/>
-      <c r="EO1" s="3"/>
-      <c r="EP1" s="3"/>
-      <c r="EQ1" s="3"/>
-      <c r="ER1" s="3"/>
-      <c r="ES1" s="3"/>
-      <c r="ET1" s="3"/>
-      <c r="EU1" s="3"/>
-      <c r="EV1" s="3"/>
-      <c r="EW1" s="3"/>
-      <c r="EX1" s="3"/>
-      <c r="EY1" s="3"/>
-      <c r="EZ1" s="3"/>
-      <c r="FA1" s="3"/>
-      <c r="FB1" s="3"/>
-      <c r="FC1" s="3"/>
-      <c r="FD1" s="3"/>
-      <c r="FE1" s="3"/>
-      <c r="FF1" s="3"/>
-      <c r="FG1" s="3"/>
-      <c r="FH1" s="3"/>
-      <c r="FI1" s="3"/>
-      <c r="FJ1" s="3"/>
-      <c r="FK1" s="3"/>
-      <c r="FL1" s="3"/>
-      <c r="FM1" s="3"/>
-      <c r="FN1" s="3"/>
-      <c r="FO1" s="3"/>
-      <c r="FP1" s="3"/>
-      <c r="FQ1" s="3"/>
-      <c r="FR1" s="3"/>
-      <c r="FS1" s="3"/>
-      <c r="FT1" s="3"/>
-      <c r="FU1" s="3"/>
-      <c r="FV1" s="3"/>
-      <c r="FW1" s="3"/>
-      <c r="FX1" s="3"/>
-      <c r="FY1" s="3"/>
-      <c r="FZ1" s="3"/>
-      <c r="GA1" s="3"/>
-      <c r="GB1" s="3"/>
-      <c r="GC1" s="3"/>
-      <c r="GD1" s="3"/>
-      <c r="GE1" s="3"/>
-      <c r="GF1" s="3"/>
-      <c r="GG1" s="3"/>
-      <c r="GH1" s="3"/>
-      <c r="GI1" s="3"/>
-      <c r="GJ1" s="3"/>
-      <c r="GK1" s="3"/>
-      <c r="GL1" s="3"/>
-      <c r="GM1" s="3"/>
-      <c r="GN1" s="3"/>
-      <c r="GO1" s="3"/>
-      <c r="GP1" s="3"/>
-      <c r="GQ1" s="3"/>
-      <c r="GR1" s="3"/>
-      <c r="GS1" s="3"/>
-      <c r="GT1" s="3"/>
-      <c r="GU1" s="3"/>
-      <c r="GV1" s="3"/>
-      <c r="GW1" s="3"/>
-      <c r="GX1" s="3"/>
-      <c r="GY1" s="3"/>
-      <c r="GZ1" s="3"/>
-      <c r="HA1" s="3"/>
-      <c r="HB1" s="3"/>
-      <c r="HC1" s="3"/>
-      <c r="HD1" s="3"/>
-      <c r="HE1" s="3"/>
-      <c r="HF1" s="3"/>
-      <c r="HG1" s="3"/>
-      <c r="HH1" s="3"/>
-      <c r="HI1" s="3"/>
-      <c r="HJ1" s="3"/>
-      <c r="HK1" s="3"/>
-      <c r="HL1" s="3"/>
-      <c r="HM1" s="3"/>
-      <c r="HN1" s="3"/>
-      <c r="HO1" s="3"/>
-      <c r="HP1" s="3"/>
-      <c r="HQ1" s="3"/>
-      <c r="HR1" s="3"/>
-      <c r="HS1" s="3"/>
-      <c r="HT1" s="3"/>
-      <c r="HU1" s="3"/>
-      <c r="HV1" s="3"/>
-      <c r="HW1" s="3"/>
-      <c r="HX1" s="3"/>
-      <c r="HY1" s="3"/>
-      <c r="HZ1" s="3"/>
-      <c r="IA1" s="3"/>
-      <c r="IB1" s="3"/>
-      <c r="IC1" s="3"/>
-      <c r="ID1" s="3"/>
-      <c r="IE1" s="3"/>
-      <c r="IF1" s="3"/>
-      <c r="IG1" s="3"/>
-      <c r="IH1" s="3"/>
-      <c r="II1" s="3"/>
-      <c r="IJ1" s="3"/>
-      <c r="IK1" s="3"/>
-      <c r="IL1" s="3"/>
-      <c r="IM1" s="3"/>
-      <c r="IN1" s="3"/>
-      <c r="IO1" s="3"/>
-      <c r="IP1" s="3"/>
-      <c r="IQ1" s="3"/>
-      <c r="IR1" s="3"/>
-      <c r="IS1" s="3"/>
-      <c r="IT1" s="3"/>
-      <c r="IU1" s="3"/>
-      <c r="IV1" s="3"/>
-      <c r="IW1" s="3"/>
-      <c r="IX1" s="3"/>
-      <c r="IY1" s="3"/>
-      <c r="IZ1" s="3"/>
-      <c r="JA1" s="3"/>
-      <c r="JB1" s="3"/>
-      <c r="JC1" s="3"/>
-      <c r="JD1" s="3"/>
-      <c r="JE1" s="3"/>
-      <c r="JF1" s="3"/>
-      <c r="JG1" s="3"/>
-      <c r="JH1" s="3"/>
-      <c r="JI1" s="3"/>
-      <c r="JJ1" s="3"/>
-      <c r="JK1" s="3"/>
-      <c r="JL1" s="3"/>
-      <c r="JM1" s="3"/>
-      <c r="JN1" s="3"/>
-      <c r="JO1" s="3"/>
-      <c r="JP1" s="3"/>
-      <c r="JQ1" s="3"/>
-      <c r="JR1" s="3"/>
-      <c r="JS1" s="3"/>
-      <c r="JT1" s="3"/>
-      <c r="JU1" s="3"/>
-      <c r="JV1" s="3"/>
-      <c r="JW1" s="3"/>
-      <c r="JX1" s="3"/>
-      <c r="JY1" s="3"/>
-      <c r="JZ1" s="3"/>
-      <c r="KA1" s="3"/>
-      <c r="KB1" s="3"/>
-      <c r="KC1" s="3"/>
-      <c r="KD1" s="3"/>
-      <c r="KE1" s="3"/>
-      <c r="KF1" s="3"/>
-      <c r="KG1" s="3"/>
-      <c r="KH1" s="3"/>
-      <c r="KI1" s="3"/>
-      <c r="KJ1" s="3"/>
-      <c r="KK1" s="3"/>
-      <c r="KL1" s="3"/>
-      <c r="KM1" s="3"/>
-      <c r="KN1" s="3"/>
-      <c r="KO1" s="3"/>
-      <c r="KP1" s="3"/>
-      <c r="KQ1" s="3"/>
-      <c r="KR1" s="3"/>
-      <c r="KS1" s="3"/>
-      <c r="KT1" s="3"/>
-      <c r="KU1" s="3"/>
-      <c r="KV1" s="3"/>
-      <c r="KW1" s="3"/>
-      <c r="KX1" s="3"/>
-      <c r="KY1" s="3"/>
-      <c r="KZ1" s="3"/>
-      <c r="LA1" s="3"/>
-      <c r="LB1" s="3"/>
-      <c r="LC1" s="3"/>
-      <c r="LD1" s="3"/>
-      <c r="LE1" s="3"/>
-      <c r="LF1" s="3"/>
-      <c r="LG1" s="3"/>
-      <c r="LH1" s="3"/>
-      <c r="LI1" s="3"/>
-      <c r="LJ1" s="3"/>
-      <c r="LK1" s="3"/>
-      <c r="LL1" s="3"/>
-      <c r="LM1" s="3"/>
-      <c r="LN1" s="3"/>
-      <c r="LO1" s="3"/>
-      <c r="LP1" s="3"/>
-      <c r="LQ1" s="3"/>
-      <c r="LR1" s="3"/>
-      <c r="LS1" s="3"/>
-      <c r="LT1" s="3"/>
-      <c r="LU1" s="3"/>
-      <c r="LV1" s="3"/>
-      <c r="LW1" s="3"/>
-      <c r="LX1" s="3"/>
-      <c r="LY1" s="3"/>
-      <c r="LZ1" s="3"/>
-      <c r="MA1" s="3"/>
-      <c r="MB1" s="3"/>
-      <c r="MC1" s="3"/>
-      <c r="MD1" s="3"/>
-      <c r="ME1" s="3"/>
-      <c r="MF1" s="3"/>
-      <c r="MG1" s="3"/>
-      <c r="MH1" s="3"/>
-      <c r="MI1" s="3"/>
-      <c r="MJ1" s="3"/>
-      <c r="MK1" s="3"/>
-      <c r="ML1" s="3"/>
-      <c r="MM1" s="3"/>
-      <c r="MN1" s="3"/>
-      <c r="MO1" s="3"/>
-      <c r="MP1" s="3"/>
-      <c r="MQ1" s="3"/>
-      <c r="MR1" s="3"/>
-      <c r="MS1" s="3"/>
-      <c r="MT1" s="3"/>
-      <c r="MU1" s="3"/>
-      <c r="MV1" s="3"/>
-      <c r="MW1" s="3"/>
-      <c r="MX1" s="3"/>
-      <c r="MY1" s="3"/>
-      <c r="MZ1" s="3"/>
-      <c r="NA1" s="3"/>
-      <c r="NB1" s="3"/>
-      <c r="NC1" s="3"/>
-      <c r="ND1" s="3"/>
-      <c r="NE1" s="3"/>
-      <c r="NF1" s="3"/>
-      <c r="NG1" s="3"/>
-      <c r="NH1" s="3"/>
-      <c r="NI1" s="3"/>
-      <c r="NJ1" s="3"/>
-      <c r="NK1" s="3"/>
-      <c r="NL1" s="3"/>
-      <c r="NM1" s="3"/>
-      <c r="NN1" s="3"/>
-      <c r="NO1" s="3"/>
-      <c r="NP1" s="3"/>
-      <c r="NQ1" s="3"/>
-      <c r="NR1" s="3"/>
-      <c r="NS1" s="3"/>
-      <c r="NT1" s="3"/>
-      <c r="NU1" s="3"/>
-      <c r="NV1" s="3"/>
-      <c r="NW1" s="3"/>
-      <c r="NX1" s="3"/>
-      <c r="NY1" s="3"/>
-      <c r="NZ1" s="3"/>
-      <c r="OA1" s="3"/>
-      <c r="OB1" s="3"/>
-      <c r="OC1" s="3"/>
-      <c r="OD1" s="3"/>
-      <c r="OE1" s="3"/>
-      <c r="OF1" s="3"/>
-      <c r="OG1" s="3"/>
-      <c r="OH1" s="3"/>
-      <c r="OI1" s="3"/>
-      <c r="OJ1" s="3"/>
-      <c r="OK1" s="3"/>
-      <c r="OL1" s="3"/>
-      <c r="OM1" s="3"/>
-      <c r="ON1" s="3"/>
-      <c r="OO1" s="3"/>
-      <c r="OP1" s="3"/>
-      <c r="OQ1" s="3"/>
-      <c r="OR1" s="3"/>
-      <c r="OS1" s="3"/>
-      <c r="OT1" s="3"/>
-      <c r="OU1" s="3"/>
-      <c r="OV1" s="3"/>
-      <c r="OW1" s="3"/>
-      <c r="OX1" s="3"/>
-      <c r="OY1" s="3"/>
-      <c r="OZ1" s="3"/>
-      <c r="PA1" s="3"/>
-      <c r="PB1" s="3"/>
-      <c r="PC1" s="3"/>
-      <c r="PD1" s="3"/>
-      <c r="PE1" s="3"/>
-      <c r="PF1" s="3"/>
-      <c r="PG1" s="3"/>
-      <c r="PH1" s="3"/>
-      <c r="PI1" s="3"/>
-      <c r="PJ1" s="3"/>
-      <c r="PK1" s="3"/>
-      <c r="PL1" s="3"/>
-      <c r="PM1" s="3"/>
-      <c r="PN1" s="3"/>
-      <c r="PO1" s="3"/>
-      <c r="PP1" s="3"/>
-      <c r="PQ1" s="3"/>
-      <c r="PR1" s="3"/>
-      <c r="PS1" s="3"/>
-      <c r="PT1" s="3"/>
-      <c r="PU1" s="3"/>
-      <c r="PV1" s="3"/>
-      <c r="PW1" s="3"/>
-      <c r="PX1" s="3"/>
-      <c r="PY1" s="3"/>
-      <c r="PZ1" s="3"/>
-      <c r="QA1" s="3"/>
-      <c r="QB1" s="3"/>
-      <c r="QC1" s="3"/>
-      <c r="QD1" s="3"/>
-      <c r="QE1" s="3"/>
-      <c r="QF1" s="3"/>
-      <c r="QG1" s="3"/>
-      <c r="QH1" s="3"/>
-      <c r="QI1" s="3"/>
-      <c r="QJ1" s="3"/>
-      <c r="QK1" s="3"/>
-      <c r="QL1" s="3"/>
-      <c r="QM1" s="3"/>
-      <c r="QN1" s="3"/>
-      <c r="QO1" s="3"/>
-      <c r="QP1" s="3"/>
-      <c r="QQ1" s="3"/>
-      <c r="QR1" s="3"/>
-      <c r="QS1" s="3"/>
-      <c r="QT1" s="3"/>
-      <c r="QU1" s="3"/>
-      <c r="QV1" s="3"/>
-      <c r="QW1" s="3"/>
-      <c r="QX1" s="3"/>
-      <c r="QY1" s="3"/>
-      <c r="QZ1" s="3"/>
-      <c r="RA1" s="3"/>
-      <c r="RB1" s="3"/>
-      <c r="RC1" s="3"/>
-      <c r="RD1" s="3"/>
-      <c r="RE1" s="3"/>
-      <c r="RF1" s="3"/>
-      <c r="RG1" s="3"/>
-      <c r="RH1" s="3"/>
-      <c r="RI1" s="3"/>
-      <c r="RJ1" s="3"/>
-      <c r="RK1" s="3"/>
-      <c r="RL1" s="3"/>
-      <c r="RM1" s="3"/>
-      <c r="RN1" s="3"/>
-      <c r="RO1" s="3"/>
-      <c r="RP1" s="3"/>
-      <c r="RQ1" s="3"/>
-      <c r="RR1" s="3"/>
-      <c r="RS1" s="3"/>
-      <c r="RT1" s="3"/>
-      <c r="RU1" s="3"/>
-      <c r="RV1" s="3"/>
-      <c r="RW1" s="3"/>
-      <c r="RX1" s="3"/>
-      <c r="RY1" s="3"/>
-      <c r="RZ1" s="3"/>
-      <c r="SA1" s="3"/>
-      <c r="SB1" s="3"/>
-      <c r="SC1" s="3"/>
-      <c r="SD1" s="3"/>
-      <c r="SE1" s="3"/>
-      <c r="SF1" s="3"/>
-      <c r="SG1" s="3"/>
-      <c r="SH1" s="3"/>
-      <c r="SI1" s="3"/>
-      <c r="SJ1" s="3"/>
-      <c r="SK1" s="3"/>
-      <c r="SL1" s="3"/>
-      <c r="SM1" s="3"/>
-      <c r="SN1" s="3"/>
-      <c r="SO1" s="3"/>
-      <c r="SP1" s="3"/>
-      <c r="SQ1" s="3"/>
-      <c r="SR1" s="3"/>
-      <c r="SS1" s="3"/>
-      <c r="ST1" s="3"/>
-      <c r="SU1" s="3"/>
-      <c r="SV1" s="3"/>
-      <c r="SW1" s="3"/>
-      <c r="SX1" s="3"/>
-      <c r="SY1" s="3"/>
-      <c r="SZ1" s="3"/>
-      <c r="TA1" s="3"/>
-      <c r="TB1" s="3"/>
-      <c r="TC1" s="3"/>
-      <c r="TD1" s="3"/>
-      <c r="TE1" s="3"/>
-      <c r="TF1" s="3"/>
-      <c r="TG1" s="3"/>
-      <c r="TH1" s="3"/>
-      <c r="TI1" s="3"/>
-      <c r="TJ1" s="3"/>
-      <c r="TK1" s="3"/>
-      <c r="TL1" s="3"/>
-      <c r="TM1" s="3"/>
-      <c r="TN1" s="3"/>
-      <c r="TO1" s="3"/>
-      <c r="TP1" s="3"/>
-      <c r="TQ1" s="3"/>
-      <c r="TR1" s="3"/>
-      <c r="TS1" s="3"/>
-      <c r="TT1" s="3"/>
-      <c r="TU1" s="3"/>
-      <c r="TV1" s="3"/>
-      <c r="TW1" s="3"/>
-      <c r="TX1" s="3"/>
-      <c r="TY1" s="3"/>
-      <c r="TZ1" s="3"/>
-      <c r="UA1" s="3"/>
-      <c r="UB1" s="3"/>
-      <c r="UC1" s="3"/>
-      <c r="UD1" s="3"/>
-      <c r="UE1" s="3"/>
-      <c r="UF1" s="3"/>
-      <c r="UG1" s="3"/>
-      <c r="UH1" s="3"/>
-      <c r="UI1" s="3"/>
-      <c r="UJ1" s="3"/>
-      <c r="UK1" s="3"/>
-      <c r="UL1" s="3"/>
-      <c r="UM1" s="3"/>
-      <c r="UN1" s="3"/>
-      <c r="UO1" s="3"/>
-      <c r="UP1" s="3"/>
-      <c r="UQ1" s="3"/>
-      <c r="UR1" s="3"/>
-      <c r="US1" s="3"/>
-      <c r="UT1" s="3"/>
-      <c r="UU1" s="3"/>
-      <c r="UV1" s="3"/>
-      <c r="UW1" s="3"/>
-      <c r="UX1" s="3"/>
-      <c r="UY1" s="3"/>
-      <c r="UZ1" s="3"/>
-      <c r="VA1" s="3"/>
-      <c r="VB1" s="3"/>
-      <c r="VC1" s="3"/>
-      <c r="VD1" s="3"/>
-      <c r="VE1" s="3"/>
-      <c r="VF1" s="3"/>
-      <c r="VG1" s="3"/>
-      <c r="VH1" s="3"/>
-      <c r="VI1" s="3"/>
-      <c r="VJ1" s="3"/>
-      <c r="VK1" s="3"/>
-      <c r="VL1" s="3"/>
-      <c r="VM1" s="3"/>
-      <c r="VN1" s="3"/>
-      <c r="VO1" s="3"/>
-      <c r="VP1" s="3"/>
-      <c r="VQ1" s="3"/>
-      <c r="VR1" s="3"/>
-      <c r="VS1" s="3"/>
-      <c r="VT1" s="3"/>
-      <c r="VU1" s="3"/>
-      <c r="VV1" s="3"/>
-      <c r="VW1" s="3"/>
-      <c r="VX1" s="3"/>
-      <c r="VY1" s="3"/>
-      <c r="VZ1" s="3"/>
-      <c r="WA1" s="3"/>
-      <c r="WB1" s="3"/>
-      <c r="WC1" s="3"/>
-      <c r="WD1" s="3"/>
-      <c r="WE1" s="3"/>
-      <c r="WF1" s="3"/>
-      <c r="WG1" s="3"/>
-      <c r="WH1" s="3"/>
-      <c r="WI1" s="3"/>
-      <c r="WJ1" s="3"/>
-      <c r="WK1" s="3"/>
-      <c r="WL1" s="3"/>
-      <c r="WM1" s="3"/>
-      <c r="WN1" s="3"/>
-      <c r="WO1" s="3"/>
-      <c r="WP1" s="3"/>
-      <c r="WQ1" s="3"/>
-      <c r="WR1" s="3"/>
-      <c r="WS1" s="3"/>
-      <c r="WT1" s="3"/>
-      <c r="WU1" s="3"/>
-      <c r="WV1" s="3"/>
-      <c r="WW1" s="3"/>
-      <c r="WX1" s="3"/>
-      <c r="WY1" s="3"/>
-      <c r="WZ1" s="3"/>
-      <c r="XA1" s="3"/>
-      <c r="XB1" s="3"/>
-      <c r="XC1" s="3"/>
-      <c r="XD1" s="3"/>
-      <c r="XE1" s="3"/>
-      <c r="XF1" s="3"/>
-      <c r="XG1" s="3"/>
-      <c r="XH1" s="3"/>
-      <c r="XI1" s="3"/>
-      <c r="XJ1" s="3"/>
-      <c r="XK1" s="3"/>
-      <c r="XL1" s="3"/>
-      <c r="XM1" s="3"/>
-      <c r="XN1" s="3"/>
-      <c r="XO1" s="3"/>
-      <c r="XP1" s="3"/>
-      <c r="XQ1" s="3"/>
-      <c r="XR1" s="3"/>
-      <c r="XS1" s="3"/>
-      <c r="XT1" s="3"/>
-      <c r="XU1" s="3"/>
-      <c r="XV1" s="3"/>
-      <c r="XW1" s="3"/>
-      <c r="XX1" s="3"/>
-      <c r="XY1" s="3"/>
-      <c r="XZ1" s="3"/>
-      <c r="YA1" s="3"/>
-      <c r="YB1" s="3"/>
-      <c r="YC1" s="3"/>
-      <c r="YD1" s="3"/>
-      <c r="YE1" s="3"/>
-      <c r="YF1" s="3"/>
-      <c r="YG1" s="3"/>
-      <c r="YH1" s="3"/>
-      <c r="YI1" s="3"/>
-      <c r="YJ1" s="3"/>
-      <c r="YK1" s="3"/>
-      <c r="YL1" s="3"/>
-      <c r="YM1" s="3"/>
-      <c r="YN1" s="3"/>
-      <c r="YO1" s="3"/>
-      <c r="YP1" s="3"/>
-      <c r="YQ1" s="3"/>
-      <c r="YR1" s="3"/>
-      <c r="YS1" s="3"/>
-      <c r="YT1" s="3"/>
-      <c r="YU1" s="3"/>
-      <c r="YV1" s="3"/>
-      <c r="YW1" s="3"/>
-      <c r="YX1" s="3"/>
-      <c r="YY1" s="3"/>
-      <c r="YZ1" s="3"/>
-      <c r="ZA1" s="3"/>
-      <c r="ZB1" s="3"/>
-      <c r="ZC1" s="3"/>
-      <c r="ZD1" s="3"/>
-      <c r="ZE1" s="3"/>
-      <c r="ZF1" s="3"/>
-      <c r="ZG1" s="3"/>
-      <c r="ZH1" s="3"/>
-      <c r="ZI1" s="3"/>
-      <c r="ZJ1" s="3"/>
-      <c r="ZK1" s="3"/>
-      <c r="ZL1" s="3"/>
-      <c r="ZM1" s="3"/>
-      <c r="ZN1" s="3"/>
-      <c r="ZO1" s="3"/>
-      <c r="ZP1" s="3"/>
-      <c r="ZQ1" s="3"/>
-      <c r="ZR1" s="3"/>
-      <c r="ZS1" s="3"/>
-      <c r="ZT1" s="3"/>
-      <c r="ZU1" s="3"/>
-      <c r="ZV1" s="3"/>
-      <c r="ZW1" s="3"/>
-      <c r="ZX1" s="3"/>
-      <c r="ZY1" s="3"/>
-      <c r="ZZ1" s="3"/>
-      <c r="AAA1" s="3"/>
-      <c r="AAB1" s="3"/>
-      <c r="AAC1" s="3"/>
-      <c r="AAD1" s="3"/>
-      <c r="AAE1" s="3"/>
-      <c r="AAF1" s="3"/>
-      <c r="AAG1" s="3"/>
-      <c r="AAH1" s="3"/>
-      <c r="AAI1" s="3"/>
-      <c r="AAJ1" s="3"/>
-      <c r="AAK1" s="3"/>
-      <c r="AAL1" s="3"/>
-      <c r="AAM1" s="3"/>
-      <c r="AAN1" s="3"/>
-      <c r="AAO1" s="3"/>
-      <c r="AAP1" s="3"/>
-      <c r="AAQ1" s="3"/>
-      <c r="AAR1" s="3"/>
-      <c r="AAS1" s="3"/>
-      <c r="AAT1" s="3"/>
-      <c r="AAU1" s="3"/>
-      <c r="AAV1" s="3"/>
-      <c r="AAW1" s="3"/>
-      <c r="AAX1" s="3"/>
-      <c r="AAY1" s="3"/>
-      <c r="AAZ1" s="3"/>
-      <c r="ABA1" s="3"/>
-      <c r="ABB1" s="3"/>
-      <c r="ABC1" s="3"/>
-      <c r="ABD1" s="3"/>
-      <c r="ABE1" s="3"/>
-      <c r="ABF1" s="3"/>
-      <c r="ABG1" s="3"/>
-      <c r="ABH1" s="3"/>
-      <c r="ABI1" s="3"/>
-      <c r="ABJ1" s="3"/>
-      <c r="ABK1" s="3"/>
-      <c r="ABL1" s="3"/>
-      <c r="ABM1" s="3"/>
-      <c r="ABN1" s="3"/>
-      <c r="ABO1" s="3"/>
-      <c r="ABP1" s="3"/>
-      <c r="ABQ1" s="3"/>
-      <c r="ABR1" s="3"/>
-      <c r="ABS1" s="3"/>
-      <c r="ABT1" s="3"/>
-      <c r="ABU1" s="3"/>
-      <c r="ABV1" s="3"/>
-      <c r="ABW1" s="3"/>
-      <c r="ABX1" s="3"/>
-      <c r="ABY1" s="3"/>
-      <c r="ABZ1" s="3"/>
-      <c r="ACA1" s="3"/>
-      <c r="ACB1" s="3"/>
-      <c r="ACC1" s="3"/>
-      <c r="ACD1" s="3"/>
-      <c r="ACE1" s="3"/>
-      <c r="ACF1" s="3"/>
-      <c r="ACG1" s="3"/>
-      <c r="ACH1" s="3"/>
-      <c r="ACI1" s="3"/>
-      <c r="ACJ1" s="3"/>
-      <c r="ACK1" s="3"/>
-      <c r="ACL1" s="3"/>
-      <c r="ACM1" s="3"/>
-      <c r="ACN1" s="3"/>
-      <c r="ACO1" s="3"/>
-      <c r="ACP1" s="3"/>
-      <c r="ACQ1" s="3"/>
-      <c r="ACR1" s="3"/>
-      <c r="ACS1" s="3"/>
-      <c r="ACT1" s="3"/>
-      <c r="ACU1" s="3"/>
-      <c r="ACV1" s="3"/>
-      <c r="ACW1" s="3"/>
-      <c r="ACX1" s="3"/>
-      <c r="ACY1" s="3"/>
-      <c r="ACZ1" s="3"/>
-      <c r="ADA1" s="3"/>
-      <c r="ADB1" s="3"/>
-      <c r="ADC1" s="3"/>
-      <c r="ADD1" s="3"/>
-      <c r="ADE1" s="3"/>
-      <c r="ADF1" s="3"/>
-      <c r="ADG1" s="3"/>
-      <c r="ADH1" s="3"/>
-      <c r="ADI1" s="3"/>
-      <c r="ADJ1" s="3"/>
-      <c r="ADK1" s="3"/>
-      <c r="ADL1" s="3"/>
-      <c r="ADM1" s="3"/>
-      <c r="ADN1" s="3"/>
-      <c r="ADO1" s="3"/>
-      <c r="ADP1" s="3"/>
-      <c r="ADQ1" s="3"/>
-      <c r="ADR1" s="3"/>
-      <c r="ADS1" s="3"/>
-      <c r="ADT1" s="3"/>
-      <c r="ADU1" s="3"/>
-      <c r="ADV1" s="3"/>
-      <c r="ADW1" s="3"/>
-      <c r="ADX1" s="3"/>
-      <c r="ADY1" s="3"/>
-      <c r="ADZ1" s="3"/>
-      <c r="AEA1" s="3"/>
-      <c r="AEB1" s="3"/>
-      <c r="AEC1" s="3"/>
-      <c r="AED1" s="3"/>
-      <c r="AEE1" s="3"/>
-      <c r="AEF1" s="3"/>
-      <c r="AEG1" s="3"/>
-      <c r="AEH1" s="3"/>
-      <c r="AEI1" s="3"/>
-      <c r="AEJ1" s="3"/>
-      <c r="AEK1" s="3"/>
-      <c r="AEL1" s="3"/>
-      <c r="AEM1" s="3"/>
-      <c r="AEN1" s="3"/>
-      <c r="AEO1" s="3"/>
-      <c r="AEP1" s="3"/>
-      <c r="AEQ1" s="3"/>
-      <c r="AER1" s="3"/>
-      <c r="AES1" s="3"/>
-      <c r="AET1" s="3"/>
-      <c r="AEU1" s="3"/>
-      <c r="AEV1" s="3"/>
-      <c r="AEW1" s="3"/>
-      <c r="AEX1" s="3"/>
-      <c r="AEY1" s="3"/>
-      <c r="AEZ1" s="3"/>
-      <c r="AFA1" s="3"/>
-      <c r="AFB1" s="3"/>
-      <c r="AFC1" s="3"/>
-      <c r="AFD1" s="3"/>
-      <c r="AFE1" s="3"/>
-      <c r="AFF1" s="3"/>
-      <c r="AFG1" s="3"/>
-      <c r="AFH1" s="3"/>
-      <c r="AFI1" s="3"/>
-      <c r="AFJ1" s="3"/>
-      <c r="AFK1" s="3"/>
-      <c r="AFL1" s="3"/>
-      <c r="AFM1" s="3"/>
-      <c r="AFN1" s="3"/>
-      <c r="AFO1" s="3"/>
-      <c r="AFP1" s="3"/>
-      <c r="AFQ1" s="3"/>
-      <c r="AFR1" s="3"/>
-      <c r="AFS1" s="3"/>
-      <c r="AFT1" s="3"/>
-      <c r="AFU1" s="3"/>
-      <c r="AFV1" s="3"/>
-      <c r="AFW1" s="3"/>
-      <c r="AFX1" s="3"/>
-      <c r="AFY1" s="3"/>
-      <c r="AFZ1" s="3"/>
-      <c r="AGA1" s="3"/>
-      <c r="AGB1" s="3"/>
-      <c r="AGC1" s="3"/>
-      <c r="AGD1" s="3"/>
-      <c r="AGE1" s="3"/>
-      <c r="AGF1" s="3"/>
-      <c r="AGG1" s="3"/>
-      <c r="AGH1" s="3"/>
-      <c r="AGI1" s="3"/>
-      <c r="AGJ1" s="3"/>
-      <c r="AGK1" s="3"/>
-      <c r="AGL1" s="3"/>
-      <c r="AGM1" s="3"/>
-      <c r="AGN1" s="3"/>
-      <c r="AGO1" s="3"/>
-      <c r="AGP1" s="3"/>
-      <c r="AGQ1" s="3"/>
-      <c r="AGR1" s="3"/>
-      <c r="AGS1" s="3"/>
-      <c r="AGT1" s="3"/>
-      <c r="AGU1" s="3"/>
-      <c r="AGV1" s="3"/>
-      <c r="AGW1" s="3"/>
-      <c r="AGX1" s="3"/>
-      <c r="AGY1" s="3"/>
-      <c r="AGZ1" s="3"/>
-      <c r="AHA1" s="3"/>
-      <c r="AHB1" s="3"/>
-      <c r="AHC1" s="3"/>
-      <c r="AHD1" s="3"/>
-      <c r="AHE1" s="3"/>
-      <c r="AHF1" s="3"/>
-      <c r="AHG1" s="3"/>
-      <c r="AHH1" s="3"/>
-      <c r="AHI1" s="3"/>
-      <c r="AHJ1" s="3"/>
-      <c r="AHK1" s="3"/>
-      <c r="AHL1" s="3"/>
-      <c r="AHM1" s="3"/>
-      <c r="AHN1" s="3"/>
-      <c r="AHO1" s="3"/>
-      <c r="AHP1" s="3"/>
-      <c r="AHQ1" s="3"/>
-      <c r="AHR1" s="3"/>
-      <c r="AHS1" s="3"/>
-      <c r="AHT1" s="3"/>
-      <c r="AHU1" s="3"/>
-      <c r="AHV1" s="3"/>
-      <c r="AHW1" s="3"/>
-      <c r="AHX1" s="3"/>
-      <c r="AHY1" s="3"/>
-      <c r="AHZ1" s="3"/>
-      <c r="AIA1" s="3"/>
-      <c r="AIB1" s="3"/>
-      <c r="AIC1" s="3"/>
-      <c r="AID1" s="3"/>
-      <c r="AIE1" s="3"/>
-      <c r="AIF1" s="3"/>
-      <c r="AIG1" s="3"/>
-      <c r="AIH1" s="3"/>
-      <c r="AII1" s="3"/>
-      <c r="AIJ1" s="3"/>
-      <c r="AIK1" s="3"/>
-      <c r="AIL1" s="3"/>
-      <c r="AIM1" s="3"/>
-      <c r="AIN1" s="3"/>
-      <c r="AIO1" s="3"/>
-      <c r="AIP1" s="3"/>
-      <c r="AIQ1" s="3"/>
-      <c r="AIR1" s="3"/>
-      <c r="AIS1" s="3"/>
-      <c r="AIT1" s="3"/>
-      <c r="AIU1" s="3"/>
-      <c r="AIV1" s="3"/>
-      <c r="AIW1" s="3"/>
-      <c r="AIX1" s="3"/>
-      <c r="AIY1" s="3"/>
-      <c r="AIZ1" s="3"/>
-      <c r="AJA1" s="3"/>
-      <c r="AJB1" s="3"/>
-      <c r="AJC1" s="3"/>
-      <c r="AJD1" s="3"/>
-      <c r="AJE1" s="3"/>
-      <c r="AJF1" s="3"/>
-      <c r="AJG1" s="3"/>
-      <c r="AJH1" s="3"/>
-      <c r="AJI1" s="3"/>
-      <c r="AJJ1" s="3"/>
-      <c r="AJK1" s="3"/>
-      <c r="AJL1" s="3"/>
-      <c r="AJM1" s="3"/>
-      <c r="AJN1" s="3"/>
-      <c r="AJO1" s="3"/>
-      <c r="AJP1" s="3"/>
-      <c r="AJQ1" s="3"/>
-      <c r="AJR1" s="3"/>
-      <c r="AJS1" s="3"/>
-      <c r="AJT1" s="3"/>
-      <c r="AJU1" s="3"/>
-      <c r="AJV1" s="3"/>
-      <c r="AJW1" s="3"/>
-      <c r="AJX1" s="3"/>
-      <c r="AJY1" s="3"/>
-      <c r="AJZ1" s="3"/>
-      <c r="AKA1" s="3"/>
-      <c r="AKB1" s="3"/>
-      <c r="AKC1" s="3"/>
-      <c r="AKD1" s="3"/>
-      <c r="AKE1" s="3"/>
-      <c r="AKF1" s="3"/>
-      <c r="AKG1" s="3"/>
-      <c r="AKH1" s="3"/>
-      <c r="AKI1" s="3"/>
-      <c r="AKJ1" s="3"/>
-      <c r="AKK1" s="3"/>
-      <c r="AKL1" s="3"/>
-      <c r="AKM1" s="3"/>
-      <c r="AKN1" s="3"/>
-      <c r="AKO1" s="3"/>
-      <c r="AKP1" s="3"/>
-      <c r="AKQ1" s="3"/>
-      <c r="AKR1" s="3"/>
-      <c r="AKS1" s="3"/>
-      <c r="AKT1" s="3"/>
-      <c r="AKU1" s="3"/>
-      <c r="AKV1" s="3"/>
-      <c r="AKW1" s="3"/>
-      <c r="AKX1" s="3"/>
-      <c r="AKY1" s="3"/>
-      <c r="AKZ1" s="3"/>
-      <c r="ALA1" s="3"/>
-      <c r="ALB1" s="3"/>
-      <c r="ALC1" s="3"/>
-      <c r="ALD1" s="3"/>
-      <c r="ALE1" s="3"/>
-      <c r="ALF1" s="3"/>
-      <c r="ALG1" s="3"/>
-      <c r="ALH1" s="3"/>
-      <c r="ALI1" s="3"/>
-      <c r="ALJ1" s="3"/>
-      <c r="ALK1" s="3"/>
-      <c r="ALL1" s="3"/>
-      <c r="ALM1" s="3"/>
-      <c r="ALN1" s="3"/>
-      <c r="ALO1" s="3"/>
-      <c r="ALP1" s="3"/>
-      <c r="ALQ1" s="3"/>
-      <c r="ALR1" s="3"/>
-      <c r="ALS1" s="3"/>
-      <c r="ALT1" s="3"/>
-      <c r="ALU1" s="3"/>
-      <c r="ALV1" s="3"/>
-      <c r="ALW1" s="3"/>
-      <c r="ALX1" s="3"/>
-      <c r="ALY1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="38" t="n">
+      <c r="B2" s="40" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="39" t="n">
+      <c r="C2" s="41" t="n">
         <v>1000</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="41" t="s">
         <v>58</v>
+      </c>
+      <c r="E2" s="42" t="str">
+        <f aca="false">VLOOKUP(A2,ListExtractors!$A$2:$B$1048576,2,0)</f>
+        <v>The VGGish neural network.</v>
       </c>
     </row>
   </sheetData>
@@ -4884,36 +3855,50 @@
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="44" t="s">
         <v>60</v>
       </c>
+      <c r="B2" s="45" t="str">
+        <f aca="false">VLOOKUP(A2,ListDigesters!$A$2:$B$1048576,2,0)</f>
+        <v>The silhouette between subtypes of a given cluster.</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="44" t="s">
         <v>61</v>
       </c>
+      <c r="B3" s="45" t="str">
+        <f aca="false">VLOOKUP(A3,ListDigesters!$A$2:$B$1048576,2,0)</f>
+        <v>The overlap between subtypes of a given cluster.</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="44" t="s">
         <v>62</v>
+      </c>
+      <c r="B4" s="45" t="str">
+        <f aca="false">VLOOKUP(A4,ListDigesters!$A$2:$B$1048576,2,0)</f>
+        <v>Contingency between two clusters.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(Examples/Campaigns): Update configuration files to version 12
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -628,10 +628,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
   <si>
     <t xml:space="preserve">SoundScapeExplorer
-Version 11</t>
+Version 12</t>
   </si>
   <si>
     <t xml:space="preserve">Instructions</t>
@@ -647,29 +647,10 @@
 Find more information in grey tabs</t>
   </si>
   <si>
-    <t xml:space="preserve">Wiki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/sound-scape-explorer/sound-scape-explorer/wiki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Found a bug?
-Want to suggest a new feature?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/sound-scape-explorer/sound-scape-explorer/issues/new/choose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need help?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/sound-scape-explorer/sound-scape-explorer/discussions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Online version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://sound-scape-explorer.github.io/sound-scape-explorer</t>
+    <t xml:space="preserve">Documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sound-scape-explorer.github.io/</t>
   </si>
   <si>
     <t xml:space="preserve">setting</t>
@@ -1077,7 +1058,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1151,12 +1132,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1277,7 +1252,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1326,10 +1301,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1418,10 +1389,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1458,11 +1425,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1572,7 +1535,7 @@
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMI17"/>
+  <dimension ref="A1:AMI12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1647,48 +1610,13 @@
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B5"/>
     <mergeCell ref="A7:A9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" display="https://github.com/sound-scape-explorer/sound-scape-explorer/wiki"/>
-    <hyperlink ref="B13" r:id="rId2" display="https://github.com/sound-scape-explorer/sound-scape-explorer/issues/new/choose"/>
-    <hyperlink ref="B15" r:id="rId3" display="https://github.com/sound-scape-explorer/sound-scape-explorer/discussions"/>
-    <hyperlink ref="B17" r:id="rId4" display="https://sound-scape-explorer.github.io/sound-scape-explorer"/>
+    <hyperlink ref="B11" r:id="rId1" display="https://sound-scape-explorer.github.io/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1716,47 +1644,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="38" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="38" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="38" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>67</v>
+      <c r="A1" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="41" t="n">
+      <c r="A2" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="40" t="n">
+      <c r="A3" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="38" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1798,45 +1726,45 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="41" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="41" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="41" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="39" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="39" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="39" t="n">
+        <v>50</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="41" t="n">
-        <v>50</v>
-      </c>
-      <c r="C2" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="41" t="n">
+      <c r="D2" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="41" t="n">
+      <c r="E2" s="39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1880,89 +1808,89 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="51" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="45" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="52" t="s">
+      <c r="B5" s="49" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B6" s="49" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="48" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B7" s="50" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B8" s="50" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B9" s="50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B10" s="50" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="53" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="53" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1994,85 +1922,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="51" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B5" s="49" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B6" s="49" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="48" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="52" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="52" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="52" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="53"/>
+      <c r="B10" s="50"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2103,33 +2031,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="50" t="s">
-        <v>63</v>
+      <c r="A1" s="47" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
-        <v>68</v>
+      <c r="A2" s="45" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
-        <v>109</v>
+      <c r="A3" s="45" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="48" t="s">
-        <v>110</v>
+      <c r="A4" s="45" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="s">
-        <v>111</v>
+      <c r="A5" s="45" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2161,23 +2089,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="50" t="s">
-        <v>69</v>
+      <c r="A1" s="47" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
-        <v>74</v>
+      <c r="A2" s="45" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
-        <v>112</v>
+      <c r="A3" s="45" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2205,28 +2133,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="16.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="50" t="s">
-        <v>53</v>
+      <c r="A1" s="47" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
-        <v>113</v>
+      <c r="A2" s="45" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
-        <v>114</v>
+      <c r="A3" s="45" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="48" t="s">
-        <v>115</v>
+      <c r="A4" s="45" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2262,1138 +2190,1138 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+    <row r="1" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="AMJ1" s="14"/>
+    </row>
+    <row r="2" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="AMJ2" s="14"/>
+    </row>
+    <row r="3" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="AMJ1" s="15"/>
-    </row>
-    <row r="2" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="AMJ3" s="14"/>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B4" s="16" t="n">
+        <v>44100</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="AMJ4" s="14"/>
+    </row>
+    <row r="5" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AMJ2" s="15"/>
-    </row>
-    <row r="3" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="B5" s="18" t="n">
+        <v>36526</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="AMJ5" s="14"/>
+    </row>
+    <row r="6" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AMJ3" s="15"/>
-    </row>
-    <row r="4" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+      <c r="AX6" s="13"/>
+      <c r="AY6" s="13"/>
+      <c r="AZ6" s="13"/>
+      <c r="BA6" s="13"/>
+      <c r="BB6" s="13"/>
+      <c r="BC6" s="13"/>
+      <c r="BD6" s="13"/>
+      <c r="BE6" s="13"/>
+      <c r="BF6" s="13"/>
+      <c r="BG6" s="13"/>
+      <c r="BH6" s="13"/>
+      <c r="BI6" s="13"/>
+      <c r="BJ6" s="13"/>
+      <c r="BK6" s="13"/>
+      <c r="BL6" s="13"/>
+      <c r="BM6" s="13"/>
+      <c r="BN6" s="13"/>
+      <c r="BO6" s="13"/>
+      <c r="BP6" s="13"/>
+      <c r="BQ6" s="13"/>
+      <c r="BR6" s="13"/>
+      <c r="BS6" s="13"/>
+      <c r="BT6" s="13"/>
+      <c r="BU6" s="13"/>
+      <c r="BV6" s="13"/>
+      <c r="BW6" s="13"/>
+      <c r="BX6" s="13"/>
+      <c r="BY6" s="13"/>
+      <c r="BZ6" s="13"/>
+      <c r="CA6" s="13"/>
+      <c r="CB6" s="13"/>
+      <c r="CC6" s="13"/>
+      <c r="CD6" s="13"/>
+      <c r="CE6" s="13"/>
+      <c r="CF6" s="13"/>
+      <c r="CG6" s="13"/>
+      <c r="CH6" s="13"/>
+      <c r="CI6" s="13"/>
+      <c r="CJ6" s="13"/>
+      <c r="CK6" s="13"/>
+      <c r="CL6" s="13"/>
+      <c r="CM6" s="13"/>
+      <c r="CN6" s="13"/>
+      <c r="CO6" s="13"/>
+      <c r="CP6" s="13"/>
+      <c r="CQ6" s="13"/>
+      <c r="CR6" s="13"/>
+      <c r="CS6" s="13"/>
+      <c r="CT6" s="13"/>
+      <c r="CU6" s="13"/>
+      <c r="CV6" s="13"/>
+      <c r="CW6" s="13"/>
+      <c r="CX6" s="13"/>
+      <c r="CY6" s="13"/>
+      <c r="CZ6" s="13"/>
+      <c r="DA6" s="13"/>
+      <c r="DB6" s="13"/>
+      <c r="DC6" s="13"/>
+      <c r="DD6" s="13"/>
+      <c r="DE6" s="13"/>
+      <c r="DF6" s="13"/>
+      <c r="DG6" s="13"/>
+      <c r="DH6" s="13"/>
+      <c r="DI6" s="13"/>
+      <c r="DJ6" s="13"/>
+      <c r="DK6" s="13"/>
+      <c r="DL6" s="13"/>
+      <c r="DM6" s="13"/>
+      <c r="DN6" s="13"/>
+      <c r="DO6" s="13"/>
+      <c r="DP6" s="13"/>
+      <c r="DQ6" s="13"/>
+      <c r="DR6" s="13"/>
+      <c r="DS6" s="13"/>
+      <c r="DT6" s="13"/>
+      <c r="DU6" s="13"/>
+      <c r="DV6" s="13"/>
+      <c r="DW6" s="13"/>
+      <c r="DX6" s="13"/>
+      <c r="DY6" s="13"/>
+      <c r="DZ6" s="13"/>
+      <c r="EA6" s="13"/>
+      <c r="EB6" s="13"/>
+      <c r="EC6" s="13"/>
+      <c r="ED6" s="13"/>
+      <c r="EE6" s="13"/>
+      <c r="EF6" s="13"/>
+      <c r="EG6" s="13"/>
+      <c r="EH6" s="13"/>
+      <c r="EI6" s="13"/>
+      <c r="EJ6" s="13"/>
+      <c r="EK6" s="13"/>
+      <c r="EL6" s="13"/>
+      <c r="EM6" s="13"/>
+      <c r="EN6" s="13"/>
+      <c r="EO6" s="13"/>
+      <c r="EP6" s="13"/>
+      <c r="EQ6" s="13"/>
+      <c r="ER6" s="13"/>
+      <c r="ES6" s="13"/>
+      <c r="ET6" s="13"/>
+      <c r="EU6" s="13"/>
+      <c r="EV6" s="13"/>
+      <c r="EW6" s="13"/>
+      <c r="EX6" s="13"/>
+      <c r="EY6" s="13"/>
+      <c r="EZ6" s="13"/>
+      <c r="FA6" s="13"/>
+      <c r="FB6" s="13"/>
+      <c r="FC6" s="13"/>
+      <c r="FD6" s="13"/>
+      <c r="FE6" s="13"/>
+      <c r="FF6" s="13"/>
+      <c r="FG6" s="13"/>
+      <c r="FH6" s="13"/>
+      <c r="FI6" s="13"/>
+      <c r="FJ6" s="13"/>
+      <c r="FK6" s="13"/>
+      <c r="FL6" s="13"/>
+      <c r="FM6" s="13"/>
+      <c r="FN6" s="13"/>
+      <c r="FO6" s="13"/>
+      <c r="FP6" s="13"/>
+      <c r="FQ6" s="13"/>
+      <c r="FR6" s="13"/>
+      <c r="FS6" s="13"/>
+      <c r="FT6" s="13"/>
+      <c r="FU6" s="13"/>
+      <c r="FV6" s="13"/>
+      <c r="FW6" s="13"/>
+      <c r="FX6" s="13"/>
+      <c r="FY6" s="13"/>
+      <c r="FZ6" s="13"/>
+      <c r="GA6" s="13"/>
+      <c r="GB6" s="13"/>
+      <c r="GC6" s="13"/>
+      <c r="GD6" s="13"/>
+      <c r="GE6" s="13"/>
+      <c r="GF6" s="13"/>
+      <c r="GG6" s="13"/>
+      <c r="GH6" s="13"/>
+      <c r="GI6" s="13"/>
+      <c r="GJ6" s="13"/>
+      <c r="GK6" s="13"/>
+      <c r="GL6" s="13"/>
+      <c r="GM6" s="13"/>
+      <c r="GN6" s="13"/>
+      <c r="GO6" s="13"/>
+      <c r="GP6" s="13"/>
+      <c r="GQ6" s="13"/>
+      <c r="GR6" s="13"/>
+      <c r="GS6" s="13"/>
+      <c r="GT6" s="13"/>
+      <c r="GU6" s="13"/>
+      <c r="GV6" s="13"/>
+      <c r="GW6" s="13"/>
+      <c r="GX6" s="13"/>
+      <c r="GY6" s="13"/>
+      <c r="GZ6" s="13"/>
+      <c r="HA6" s="13"/>
+      <c r="HB6" s="13"/>
+      <c r="HC6" s="13"/>
+      <c r="HD6" s="13"/>
+      <c r="HE6" s="13"/>
+      <c r="HF6" s="13"/>
+      <c r="HG6" s="13"/>
+      <c r="HH6" s="13"/>
+      <c r="HI6" s="13"/>
+      <c r="HJ6" s="13"/>
+      <c r="HK6" s="13"/>
+      <c r="HL6" s="13"/>
+      <c r="HM6" s="13"/>
+      <c r="HN6" s="13"/>
+      <c r="HO6" s="13"/>
+      <c r="HP6" s="13"/>
+      <c r="HQ6" s="13"/>
+      <c r="HR6" s="13"/>
+      <c r="HS6" s="13"/>
+      <c r="HT6" s="13"/>
+      <c r="HU6" s="13"/>
+      <c r="HV6" s="13"/>
+      <c r="HW6" s="13"/>
+      <c r="HX6" s="13"/>
+      <c r="HY6" s="13"/>
+      <c r="HZ6" s="13"/>
+      <c r="IA6" s="13"/>
+      <c r="IB6" s="13"/>
+      <c r="IC6" s="13"/>
+      <c r="ID6" s="13"/>
+      <c r="IE6" s="13"/>
+      <c r="IF6" s="13"/>
+      <c r="IG6" s="13"/>
+      <c r="IH6" s="13"/>
+      <c r="II6" s="13"/>
+      <c r="IJ6" s="13"/>
+      <c r="IK6" s="13"/>
+      <c r="IL6" s="13"/>
+      <c r="IM6" s="13"/>
+      <c r="IN6" s="13"/>
+      <c r="IO6" s="13"/>
+      <c r="IP6" s="13"/>
+      <c r="IQ6" s="13"/>
+      <c r="IR6" s="13"/>
+      <c r="IS6" s="13"/>
+      <c r="IT6" s="13"/>
+      <c r="IU6" s="13"/>
+      <c r="IV6" s="13"/>
+      <c r="IW6" s="13"/>
+      <c r="IX6" s="13"/>
+      <c r="IY6" s="13"/>
+      <c r="IZ6" s="13"/>
+      <c r="JA6" s="13"/>
+      <c r="JB6" s="13"/>
+      <c r="JC6" s="13"/>
+      <c r="JD6" s="13"/>
+      <c r="JE6" s="13"/>
+      <c r="JF6" s="13"/>
+      <c r="JG6" s="13"/>
+      <c r="JH6" s="13"/>
+      <c r="JI6" s="13"/>
+      <c r="JJ6" s="13"/>
+      <c r="JK6" s="13"/>
+      <c r="JL6" s="13"/>
+      <c r="JM6" s="13"/>
+      <c r="JN6" s="13"/>
+      <c r="JO6" s="13"/>
+      <c r="JP6" s="13"/>
+      <c r="JQ6" s="13"/>
+      <c r="JR6" s="13"/>
+      <c r="JS6" s="13"/>
+      <c r="JT6" s="13"/>
+      <c r="JU6" s="13"/>
+      <c r="JV6" s="13"/>
+      <c r="JW6" s="13"/>
+      <c r="JX6" s="13"/>
+      <c r="JY6" s="13"/>
+      <c r="JZ6" s="13"/>
+      <c r="KA6" s="13"/>
+      <c r="KB6" s="13"/>
+      <c r="KC6" s="13"/>
+      <c r="KD6" s="13"/>
+      <c r="KE6" s="13"/>
+      <c r="KF6" s="13"/>
+      <c r="KG6" s="13"/>
+      <c r="KH6" s="13"/>
+      <c r="KI6" s="13"/>
+      <c r="KJ6" s="13"/>
+      <c r="KK6" s="13"/>
+      <c r="KL6" s="13"/>
+      <c r="KM6" s="13"/>
+      <c r="KN6" s="13"/>
+      <c r="KO6" s="13"/>
+      <c r="KP6" s="13"/>
+      <c r="KQ6" s="13"/>
+      <c r="KR6" s="13"/>
+      <c r="KS6" s="13"/>
+      <c r="KT6" s="13"/>
+      <c r="KU6" s="13"/>
+      <c r="KV6" s="13"/>
+      <c r="KW6" s="13"/>
+      <c r="KX6" s="13"/>
+      <c r="KY6" s="13"/>
+      <c r="KZ6" s="13"/>
+      <c r="LA6" s="13"/>
+      <c r="LB6" s="13"/>
+      <c r="LC6" s="13"/>
+      <c r="LD6" s="13"/>
+      <c r="LE6" s="13"/>
+      <c r="LF6" s="13"/>
+      <c r="LG6" s="13"/>
+      <c r="LH6" s="13"/>
+      <c r="LI6" s="13"/>
+      <c r="LJ6" s="13"/>
+      <c r="LK6" s="13"/>
+      <c r="LL6" s="13"/>
+      <c r="LM6" s="13"/>
+      <c r="LN6" s="13"/>
+      <c r="LO6" s="13"/>
+      <c r="LP6" s="13"/>
+      <c r="LQ6" s="13"/>
+      <c r="LR6" s="13"/>
+      <c r="LS6" s="13"/>
+      <c r="LT6" s="13"/>
+      <c r="LU6" s="13"/>
+      <c r="LV6" s="13"/>
+      <c r="LW6" s="13"/>
+      <c r="LX6" s="13"/>
+      <c r="LY6" s="13"/>
+      <c r="LZ6" s="13"/>
+      <c r="MA6" s="13"/>
+      <c r="MB6" s="13"/>
+      <c r="MC6" s="13"/>
+      <c r="MD6" s="13"/>
+      <c r="ME6" s="13"/>
+      <c r="MF6" s="13"/>
+      <c r="MG6" s="13"/>
+      <c r="MH6" s="13"/>
+      <c r="MI6" s="13"/>
+      <c r="MJ6" s="13"/>
+      <c r="MK6" s="13"/>
+      <c r="ML6" s="13"/>
+      <c r="MM6" s="13"/>
+      <c r="MN6" s="13"/>
+      <c r="MO6" s="13"/>
+      <c r="MP6" s="13"/>
+      <c r="MQ6" s="13"/>
+      <c r="MR6" s="13"/>
+      <c r="MS6" s="13"/>
+      <c r="MT6" s="13"/>
+      <c r="MU6" s="13"/>
+      <c r="MV6" s="13"/>
+      <c r="MW6" s="13"/>
+      <c r="MX6" s="13"/>
+      <c r="MY6" s="13"/>
+      <c r="MZ6" s="13"/>
+      <c r="NA6" s="13"/>
+      <c r="NB6" s="13"/>
+      <c r="NC6" s="13"/>
+      <c r="ND6" s="13"/>
+      <c r="NE6" s="13"/>
+      <c r="NF6" s="13"/>
+      <c r="NG6" s="13"/>
+      <c r="NH6" s="13"/>
+      <c r="NI6" s="13"/>
+      <c r="NJ6" s="13"/>
+      <c r="NK6" s="13"/>
+      <c r="NL6" s="13"/>
+      <c r="NM6" s="13"/>
+      <c r="NN6" s="13"/>
+      <c r="NO6" s="13"/>
+      <c r="NP6" s="13"/>
+      <c r="NQ6" s="13"/>
+      <c r="NR6" s="13"/>
+      <c r="NS6" s="13"/>
+      <c r="NT6" s="13"/>
+      <c r="NU6" s="13"/>
+      <c r="NV6" s="13"/>
+      <c r="NW6" s="13"/>
+      <c r="NX6" s="13"/>
+      <c r="NY6" s="13"/>
+      <c r="NZ6" s="13"/>
+      <c r="OA6" s="13"/>
+      <c r="OB6" s="13"/>
+      <c r="OC6" s="13"/>
+      <c r="OD6" s="13"/>
+      <c r="OE6" s="13"/>
+      <c r="OF6" s="13"/>
+      <c r="OG6" s="13"/>
+      <c r="OH6" s="13"/>
+      <c r="OI6" s="13"/>
+      <c r="OJ6" s="13"/>
+      <c r="OK6" s="13"/>
+      <c r="OL6" s="13"/>
+      <c r="OM6" s="13"/>
+      <c r="ON6" s="13"/>
+      <c r="OO6" s="13"/>
+      <c r="OP6" s="13"/>
+      <c r="OQ6" s="13"/>
+      <c r="OR6" s="13"/>
+      <c r="OS6" s="13"/>
+      <c r="OT6" s="13"/>
+      <c r="OU6" s="13"/>
+      <c r="OV6" s="13"/>
+      <c r="OW6" s="13"/>
+      <c r="OX6" s="13"/>
+      <c r="OY6" s="13"/>
+      <c r="OZ6" s="13"/>
+      <c r="PA6" s="13"/>
+      <c r="PB6" s="13"/>
+      <c r="PC6" s="13"/>
+      <c r="PD6" s="13"/>
+      <c r="PE6" s="13"/>
+      <c r="PF6" s="13"/>
+      <c r="PG6" s="13"/>
+      <c r="PH6" s="13"/>
+      <c r="PI6" s="13"/>
+      <c r="PJ6" s="13"/>
+      <c r="PK6" s="13"/>
+      <c r="PL6" s="13"/>
+      <c r="PM6" s="13"/>
+      <c r="PN6" s="13"/>
+      <c r="PO6" s="13"/>
+      <c r="PP6" s="13"/>
+      <c r="PQ6" s="13"/>
+      <c r="PR6" s="13"/>
+      <c r="PS6" s="13"/>
+      <c r="PT6" s="13"/>
+      <c r="PU6" s="13"/>
+      <c r="PV6" s="13"/>
+      <c r="PW6" s="13"/>
+      <c r="PX6" s="13"/>
+      <c r="PY6" s="13"/>
+      <c r="PZ6" s="13"/>
+      <c r="QA6" s="13"/>
+      <c r="QB6" s="13"/>
+      <c r="QC6" s="13"/>
+      <c r="QD6" s="13"/>
+      <c r="QE6" s="13"/>
+      <c r="QF6" s="13"/>
+      <c r="QG6" s="13"/>
+      <c r="QH6" s="13"/>
+      <c r="QI6" s="13"/>
+      <c r="QJ6" s="13"/>
+      <c r="QK6" s="13"/>
+      <c r="QL6" s="13"/>
+      <c r="QM6" s="13"/>
+      <c r="QN6" s="13"/>
+      <c r="QO6" s="13"/>
+      <c r="QP6" s="13"/>
+      <c r="QQ6" s="13"/>
+      <c r="QR6" s="13"/>
+      <c r="QS6" s="13"/>
+      <c r="QT6" s="13"/>
+      <c r="QU6" s="13"/>
+      <c r="QV6" s="13"/>
+      <c r="QW6" s="13"/>
+      <c r="QX6" s="13"/>
+      <c r="QY6" s="13"/>
+      <c r="QZ6" s="13"/>
+      <c r="RA6" s="13"/>
+      <c r="RB6" s="13"/>
+      <c r="RC6" s="13"/>
+      <c r="RD6" s="13"/>
+      <c r="RE6" s="13"/>
+      <c r="RF6" s="13"/>
+      <c r="RG6" s="13"/>
+      <c r="RH6" s="13"/>
+      <c r="RI6" s="13"/>
+      <c r="RJ6" s="13"/>
+      <c r="RK6" s="13"/>
+      <c r="RL6" s="13"/>
+      <c r="RM6" s="13"/>
+      <c r="RN6" s="13"/>
+      <c r="RO6" s="13"/>
+      <c r="RP6" s="13"/>
+      <c r="RQ6" s="13"/>
+      <c r="RR6" s="13"/>
+      <c r="RS6" s="13"/>
+      <c r="RT6" s="13"/>
+      <c r="RU6" s="13"/>
+      <c r="RV6" s="13"/>
+      <c r="RW6" s="13"/>
+      <c r="RX6" s="13"/>
+      <c r="RY6" s="13"/>
+      <c r="RZ6" s="13"/>
+      <c r="SA6" s="13"/>
+      <c r="SB6" s="13"/>
+      <c r="SC6" s="13"/>
+      <c r="SD6" s="13"/>
+      <c r="SE6" s="13"/>
+      <c r="SF6" s="13"/>
+      <c r="SG6" s="13"/>
+      <c r="SH6" s="13"/>
+      <c r="SI6" s="13"/>
+      <c r="SJ6" s="13"/>
+      <c r="SK6" s="13"/>
+      <c r="SL6" s="13"/>
+      <c r="SM6" s="13"/>
+      <c r="SN6" s="13"/>
+      <c r="SO6" s="13"/>
+      <c r="SP6" s="13"/>
+      <c r="SQ6" s="13"/>
+      <c r="SR6" s="13"/>
+      <c r="SS6" s="13"/>
+      <c r="ST6" s="13"/>
+      <c r="SU6" s="13"/>
+      <c r="SV6" s="13"/>
+      <c r="SW6" s="13"/>
+      <c r="SX6" s="13"/>
+      <c r="SY6" s="13"/>
+      <c r="SZ6" s="13"/>
+      <c r="TA6" s="13"/>
+      <c r="TB6" s="13"/>
+      <c r="TC6" s="13"/>
+      <c r="TD6" s="13"/>
+      <c r="TE6" s="13"/>
+      <c r="TF6" s="13"/>
+      <c r="TG6" s="13"/>
+      <c r="TH6" s="13"/>
+      <c r="TI6" s="13"/>
+      <c r="TJ6" s="13"/>
+      <c r="TK6" s="13"/>
+      <c r="TL6" s="13"/>
+      <c r="TM6" s="13"/>
+      <c r="TN6" s="13"/>
+      <c r="TO6" s="13"/>
+      <c r="TP6" s="13"/>
+      <c r="TQ6" s="13"/>
+      <c r="TR6" s="13"/>
+      <c r="TS6" s="13"/>
+      <c r="TT6" s="13"/>
+      <c r="TU6" s="13"/>
+      <c r="TV6" s="13"/>
+      <c r="TW6" s="13"/>
+      <c r="TX6" s="13"/>
+      <c r="TY6" s="13"/>
+      <c r="TZ6" s="13"/>
+      <c r="UA6" s="13"/>
+      <c r="UB6" s="13"/>
+      <c r="UC6" s="13"/>
+      <c r="UD6" s="13"/>
+      <c r="UE6" s="13"/>
+      <c r="UF6" s="13"/>
+      <c r="UG6" s="13"/>
+      <c r="UH6" s="13"/>
+      <c r="UI6" s="13"/>
+      <c r="UJ6" s="13"/>
+      <c r="UK6" s="13"/>
+      <c r="UL6" s="13"/>
+      <c r="UM6" s="13"/>
+      <c r="UN6" s="13"/>
+      <c r="UO6" s="13"/>
+      <c r="UP6" s="13"/>
+      <c r="UQ6" s="13"/>
+      <c r="UR6" s="13"/>
+      <c r="US6" s="13"/>
+      <c r="UT6" s="13"/>
+      <c r="UU6" s="13"/>
+      <c r="UV6" s="13"/>
+      <c r="UW6" s="13"/>
+      <c r="UX6" s="13"/>
+      <c r="UY6" s="13"/>
+      <c r="UZ6" s="13"/>
+      <c r="VA6" s="13"/>
+      <c r="VB6" s="13"/>
+      <c r="VC6" s="13"/>
+      <c r="VD6" s="13"/>
+      <c r="VE6" s="13"/>
+      <c r="VF6" s="13"/>
+      <c r="VG6" s="13"/>
+      <c r="VH6" s="13"/>
+      <c r="VI6" s="13"/>
+      <c r="VJ6" s="13"/>
+      <c r="VK6" s="13"/>
+      <c r="VL6" s="13"/>
+      <c r="VM6" s="13"/>
+      <c r="VN6" s="13"/>
+      <c r="VO6" s="13"/>
+      <c r="VP6" s="13"/>
+      <c r="VQ6" s="13"/>
+      <c r="VR6" s="13"/>
+      <c r="VS6" s="13"/>
+      <c r="VT6" s="13"/>
+      <c r="VU6" s="13"/>
+      <c r="VV6" s="13"/>
+      <c r="VW6" s="13"/>
+      <c r="VX6" s="13"/>
+      <c r="VY6" s="13"/>
+      <c r="VZ6" s="13"/>
+      <c r="WA6" s="13"/>
+      <c r="WB6" s="13"/>
+      <c r="WC6" s="13"/>
+      <c r="WD6" s="13"/>
+      <c r="WE6" s="13"/>
+      <c r="WF6" s="13"/>
+      <c r="WG6" s="13"/>
+      <c r="WH6" s="13"/>
+      <c r="WI6" s="13"/>
+      <c r="WJ6" s="13"/>
+      <c r="WK6" s="13"/>
+      <c r="WL6" s="13"/>
+      <c r="WM6" s="13"/>
+      <c r="WN6" s="13"/>
+      <c r="WO6" s="13"/>
+      <c r="WP6" s="13"/>
+      <c r="WQ6" s="13"/>
+      <c r="WR6" s="13"/>
+      <c r="WS6" s="13"/>
+      <c r="WT6" s="13"/>
+      <c r="WU6" s="13"/>
+      <c r="WV6" s="13"/>
+      <c r="WW6" s="13"/>
+      <c r="WX6" s="13"/>
+      <c r="WY6" s="13"/>
+      <c r="WZ6" s="13"/>
+      <c r="XA6" s="13"/>
+      <c r="XB6" s="13"/>
+      <c r="XC6" s="13"/>
+      <c r="XD6" s="13"/>
+      <c r="XE6" s="13"/>
+      <c r="XF6" s="13"/>
+      <c r="XG6" s="13"/>
+      <c r="XH6" s="13"/>
+      <c r="XI6" s="13"/>
+      <c r="XJ6" s="13"/>
+      <c r="XK6" s="13"/>
+      <c r="XL6" s="13"/>
+      <c r="XM6" s="13"/>
+      <c r="XN6" s="13"/>
+      <c r="XO6" s="13"/>
+      <c r="XP6" s="13"/>
+      <c r="XQ6" s="13"/>
+      <c r="XR6" s="13"/>
+      <c r="XS6" s="13"/>
+      <c r="XT6" s="13"/>
+      <c r="XU6" s="13"/>
+      <c r="XV6" s="13"/>
+      <c r="XW6" s="13"/>
+      <c r="XX6" s="13"/>
+      <c r="XY6" s="13"/>
+      <c r="XZ6" s="13"/>
+      <c r="YA6" s="13"/>
+      <c r="YB6" s="13"/>
+      <c r="YC6" s="13"/>
+      <c r="YD6" s="13"/>
+      <c r="YE6" s="13"/>
+      <c r="YF6" s="13"/>
+      <c r="YG6" s="13"/>
+      <c r="YH6" s="13"/>
+      <c r="YI6" s="13"/>
+      <c r="YJ6" s="13"/>
+      <c r="YK6" s="13"/>
+      <c r="YL6" s="13"/>
+      <c r="YM6" s="13"/>
+      <c r="YN6" s="13"/>
+      <c r="YO6" s="13"/>
+      <c r="YP6" s="13"/>
+      <c r="YQ6" s="13"/>
+      <c r="YR6" s="13"/>
+      <c r="YS6" s="13"/>
+      <c r="YT6" s="13"/>
+      <c r="YU6" s="13"/>
+      <c r="YV6" s="13"/>
+      <c r="YW6" s="13"/>
+      <c r="YX6" s="13"/>
+      <c r="YY6" s="13"/>
+      <c r="YZ6" s="13"/>
+      <c r="ZA6" s="13"/>
+      <c r="ZB6" s="13"/>
+      <c r="ZC6" s="13"/>
+      <c r="ZD6" s="13"/>
+      <c r="ZE6" s="13"/>
+      <c r="ZF6" s="13"/>
+      <c r="ZG6" s="13"/>
+      <c r="ZH6" s="13"/>
+      <c r="ZI6" s="13"/>
+      <c r="ZJ6" s="13"/>
+      <c r="ZK6" s="13"/>
+      <c r="ZL6" s="13"/>
+      <c r="ZM6" s="13"/>
+      <c r="ZN6" s="13"/>
+      <c r="ZO6" s="13"/>
+      <c r="ZP6" s="13"/>
+      <c r="ZQ6" s="13"/>
+      <c r="ZR6" s="13"/>
+      <c r="ZS6" s="13"/>
+      <c r="ZT6" s="13"/>
+      <c r="ZU6" s="13"/>
+      <c r="ZV6" s="13"/>
+      <c r="ZW6" s="13"/>
+      <c r="ZX6" s="13"/>
+      <c r="ZY6" s="13"/>
+      <c r="ZZ6" s="13"/>
+      <c r="AAA6" s="13"/>
+      <c r="AAB6" s="13"/>
+      <c r="AAC6" s="13"/>
+      <c r="AAD6" s="13"/>
+      <c r="AAE6" s="13"/>
+      <c r="AAF6" s="13"/>
+      <c r="AAG6" s="13"/>
+      <c r="AAH6" s="13"/>
+      <c r="AAI6" s="13"/>
+      <c r="AAJ6" s="13"/>
+      <c r="AAK6" s="13"/>
+      <c r="AAL6" s="13"/>
+      <c r="AAM6" s="13"/>
+      <c r="AAN6" s="13"/>
+      <c r="AAO6" s="13"/>
+      <c r="AAP6" s="13"/>
+      <c r="AAQ6" s="13"/>
+      <c r="AAR6" s="13"/>
+      <c r="AAS6" s="13"/>
+      <c r="AAT6" s="13"/>
+      <c r="AAU6" s="13"/>
+      <c r="AAV6" s="13"/>
+      <c r="AAW6" s="13"/>
+      <c r="AAX6" s="13"/>
+      <c r="AAY6" s="13"/>
+      <c r="AAZ6" s="13"/>
+      <c r="ABA6" s="13"/>
+      <c r="ABB6" s="13"/>
+      <c r="ABC6" s="13"/>
+      <c r="ABD6" s="13"/>
+      <c r="ABE6" s="13"/>
+      <c r="ABF6" s="13"/>
+      <c r="ABG6" s="13"/>
+      <c r="ABH6" s="13"/>
+      <c r="ABI6" s="13"/>
+      <c r="ABJ6" s="13"/>
+      <c r="ABK6" s="13"/>
+      <c r="ABL6" s="13"/>
+      <c r="ABM6" s="13"/>
+      <c r="ABN6" s="13"/>
+      <c r="ABO6" s="13"/>
+      <c r="ABP6" s="13"/>
+      <c r="ABQ6" s="13"/>
+      <c r="ABR6" s="13"/>
+      <c r="ABS6" s="13"/>
+      <c r="ABT6" s="13"/>
+      <c r="ABU6" s="13"/>
+      <c r="ABV6" s="13"/>
+      <c r="ABW6" s="13"/>
+      <c r="ABX6" s="13"/>
+      <c r="ABY6" s="13"/>
+      <c r="ABZ6" s="13"/>
+      <c r="ACA6" s="13"/>
+      <c r="ACB6" s="13"/>
+      <c r="ACC6" s="13"/>
+      <c r="ACD6" s="13"/>
+      <c r="ACE6" s="13"/>
+      <c r="ACF6" s="13"/>
+      <c r="ACG6" s="13"/>
+      <c r="ACH6" s="13"/>
+      <c r="ACI6" s="13"/>
+      <c r="ACJ6" s="13"/>
+      <c r="ACK6" s="13"/>
+      <c r="ACL6" s="13"/>
+      <c r="ACM6" s="13"/>
+      <c r="ACN6" s="13"/>
+      <c r="ACO6" s="13"/>
+      <c r="ACP6" s="13"/>
+      <c r="ACQ6" s="13"/>
+      <c r="ACR6" s="13"/>
+      <c r="ACS6" s="13"/>
+      <c r="ACT6" s="13"/>
+      <c r="ACU6" s="13"/>
+      <c r="ACV6" s="13"/>
+      <c r="ACW6" s="13"/>
+      <c r="ACX6" s="13"/>
+      <c r="ACY6" s="13"/>
+      <c r="ACZ6" s="13"/>
+      <c r="ADA6" s="13"/>
+      <c r="ADB6" s="13"/>
+      <c r="ADC6" s="13"/>
+      <c r="ADD6" s="13"/>
+      <c r="ADE6" s="13"/>
+      <c r="ADF6" s="13"/>
+      <c r="ADG6" s="13"/>
+      <c r="ADH6" s="13"/>
+      <c r="ADI6" s="13"/>
+      <c r="ADJ6" s="13"/>
+      <c r="ADK6" s="13"/>
+      <c r="ADL6" s="13"/>
+      <c r="ADM6" s="13"/>
+      <c r="ADN6" s="13"/>
+      <c r="ADO6" s="13"/>
+      <c r="ADP6" s="13"/>
+      <c r="ADQ6" s="13"/>
+      <c r="ADR6" s="13"/>
+      <c r="ADS6" s="13"/>
+      <c r="ADT6" s="13"/>
+      <c r="ADU6" s="13"/>
+      <c r="ADV6" s="13"/>
+      <c r="ADW6" s="13"/>
+      <c r="ADX6" s="13"/>
+      <c r="ADY6" s="13"/>
+      <c r="ADZ6" s="13"/>
+      <c r="AEA6" s="13"/>
+      <c r="AEB6" s="13"/>
+      <c r="AEC6" s="13"/>
+      <c r="AED6" s="13"/>
+      <c r="AEE6" s="13"/>
+      <c r="AEF6" s="13"/>
+      <c r="AEG6" s="13"/>
+      <c r="AEH6" s="13"/>
+      <c r="AEI6" s="13"/>
+      <c r="AEJ6" s="13"/>
+      <c r="AEK6" s="13"/>
+      <c r="AEL6" s="13"/>
+      <c r="AEM6" s="13"/>
+      <c r="AEN6" s="13"/>
+      <c r="AEO6" s="13"/>
+      <c r="AEP6" s="13"/>
+      <c r="AEQ6" s="13"/>
+      <c r="AER6" s="13"/>
+      <c r="AES6" s="13"/>
+      <c r="AET6" s="13"/>
+      <c r="AEU6" s="13"/>
+      <c r="AEV6" s="13"/>
+      <c r="AEW6" s="13"/>
+      <c r="AEX6" s="13"/>
+      <c r="AEY6" s="13"/>
+      <c r="AEZ6" s="13"/>
+      <c r="AFA6" s="13"/>
+      <c r="AFB6" s="13"/>
+      <c r="AFC6" s="13"/>
+      <c r="AFD6" s="13"/>
+      <c r="AFE6" s="13"/>
+      <c r="AFF6" s="13"/>
+      <c r="AFG6" s="13"/>
+      <c r="AFH6" s="13"/>
+      <c r="AFI6" s="13"/>
+      <c r="AFJ6" s="13"/>
+      <c r="AFK6" s="13"/>
+      <c r="AFL6" s="13"/>
+      <c r="AFM6" s="13"/>
+      <c r="AFN6" s="13"/>
+      <c r="AFO6" s="13"/>
+      <c r="AFP6" s="13"/>
+      <c r="AFQ6" s="13"/>
+      <c r="AFR6" s="13"/>
+      <c r="AFS6" s="13"/>
+      <c r="AFT6" s="13"/>
+      <c r="AFU6" s="13"/>
+      <c r="AFV6" s="13"/>
+      <c r="AFW6" s="13"/>
+      <c r="AFX6" s="13"/>
+      <c r="AFY6" s="13"/>
+      <c r="AFZ6" s="13"/>
+      <c r="AGA6" s="13"/>
+      <c r="AGB6" s="13"/>
+      <c r="AGC6" s="13"/>
+      <c r="AGD6" s="13"/>
+      <c r="AGE6" s="13"/>
+      <c r="AGF6" s="13"/>
+      <c r="AGG6" s="13"/>
+      <c r="AGH6" s="13"/>
+      <c r="AGI6" s="13"/>
+      <c r="AGJ6" s="13"/>
+      <c r="AGK6" s="13"/>
+      <c r="AGL6" s="13"/>
+      <c r="AGM6" s="13"/>
+      <c r="AGN6" s="13"/>
+      <c r="AGO6" s="13"/>
+      <c r="AGP6" s="13"/>
+      <c r="AGQ6" s="13"/>
+      <c r="AGR6" s="13"/>
+      <c r="AGS6" s="13"/>
+      <c r="AGT6" s="13"/>
+      <c r="AGU6" s="13"/>
+      <c r="AGV6" s="13"/>
+      <c r="AGW6" s="13"/>
+      <c r="AGX6" s="13"/>
+      <c r="AGY6" s="13"/>
+      <c r="AGZ6" s="13"/>
+      <c r="AHA6" s="13"/>
+      <c r="AHB6" s="13"/>
+      <c r="AHC6" s="13"/>
+      <c r="AHD6" s="13"/>
+      <c r="AHE6" s="13"/>
+      <c r="AHF6" s="13"/>
+      <c r="AHG6" s="13"/>
+      <c r="AHH6" s="13"/>
+      <c r="AHI6" s="13"/>
+      <c r="AHJ6" s="13"/>
+      <c r="AHK6" s="13"/>
+      <c r="AHL6" s="13"/>
+      <c r="AHM6" s="13"/>
+      <c r="AHN6" s="13"/>
+      <c r="AHO6" s="13"/>
+      <c r="AHP6" s="13"/>
+      <c r="AHQ6" s="13"/>
+      <c r="AHR6" s="13"/>
+      <c r="AHS6" s="13"/>
+      <c r="AHT6" s="13"/>
+      <c r="AHU6" s="13"/>
+      <c r="AHV6" s="13"/>
+      <c r="AHW6" s="13"/>
+      <c r="AHX6" s="13"/>
+      <c r="AHY6" s="13"/>
+      <c r="AHZ6" s="13"/>
+      <c r="AIA6" s="13"/>
+      <c r="AIB6" s="13"/>
+      <c r="AIC6" s="13"/>
+      <c r="AID6" s="13"/>
+      <c r="AIE6" s="13"/>
+      <c r="AIF6" s="13"/>
+      <c r="AIG6" s="13"/>
+      <c r="AIH6" s="13"/>
+      <c r="AII6" s="13"/>
+      <c r="AIJ6" s="13"/>
+      <c r="AIK6" s="13"/>
+      <c r="AIL6" s="13"/>
+      <c r="AIM6" s="13"/>
+      <c r="AIN6" s="13"/>
+      <c r="AIO6" s="13"/>
+      <c r="AIP6" s="13"/>
+      <c r="AIQ6" s="13"/>
+      <c r="AIR6" s="13"/>
+      <c r="AIS6" s="13"/>
+      <c r="AIT6" s="13"/>
+      <c r="AIU6" s="13"/>
+      <c r="AIV6" s="13"/>
+      <c r="AIW6" s="13"/>
+      <c r="AIX6" s="13"/>
+      <c r="AIY6" s="13"/>
+      <c r="AIZ6" s="13"/>
+      <c r="AJA6" s="13"/>
+      <c r="AJB6" s="13"/>
+      <c r="AJC6" s="13"/>
+      <c r="AJD6" s="13"/>
+      <c r="AJE6" s="13"/>
+      <c r="AJF6" s="13"/>
+      <c r="AJG6" s="13"/>
+      <c r="AJH6" s="13"/>
+      <c r="AJI6" s="13"/>
+      <c r="AJJ6" s="13"/>
+      <c r="AJK6" s="13"/>
+      <c r="AJL6" s="13"/>
+      <c r="AJM6" s="13"/>
+      <c r="AJN6" s="13"/>
+      <c r="AJO6" s="13"/>
+      <c r="AJP6" s="13"/>
+      <c r="AJQ6" s="13"/>
+      <c r="AJR6" s="13"/>
+      <c r="AJS6" s="13"/>
+      <c r="AJT6" s="13"/>
+      <c r="AJU6" s="13"/>
+      <c r="AJV6" s="13"/>
+      <c r="AJW6" s="13"/>
+      <c r="AJX6" s="13"/>
+      <c r="AJY6" s="13"/>
+      <c r="AJZ6" s="13"/>
+      <c r="AKA6" s="13"/>
+      <c r="AKB6" s="13"/>
+      <c r="AKC6" s="13"/>
+      <c r="AKD6" s="13"/>
+      <c r="AKE6" s="13"/>
+      <c r="AKF6" s="13"/>
+      <c r="AKG6" s="13"/>
+      <c r="AKH6" s="13"/>
+      <c r="AKI6" s="13"/>
+      <c r="AKJ6" s="13"/>
+      <c r="AKK6" s="13"/>
+      <c r="AKL6" s="13"/>
+      <c r="AKM6" s="13"/>
+      <c r="AKN6" s="13"/>
+      <c r="AKO6" s="13"/>
+      <c r="AKP6" s="13"/>
+      <c r="AKQ6" s="13"/>
+      <c r="AKR6" s="13"/>
+      <c r="AKS6" s="13"/>
+      <c r="AKT6" s="13"/>
+      <c r="AKU6" s="13"/>
+      <c r="AKV6" s="13"/>
+      <c r="AKW6" s="13"/>
+      <c r="AKX6" s="13"/>
+      <c r="AKY6" s="13"/>
+      <c r="AKZ6" s="13"/>
+      <c r="ALA6" s="13"/>
+      <c r="ALB6" s="13"/>
+      <c r="ALC6" s="13"/>
+      <c r="ALD6" s="13"/>
+      <c r="ALE6" s="13"/>
+      <c r="ALF6" s="13"/>
+      <c r="ALG6" s="13"/>
+      <c r="ALH6" s="13"/>
+      <c r="ALI6" s="13"/>
+      <c r="ALJ6" s="13"/>
+      <c r="ALK6" s="13"/>
+      <c r="ALL6" s="13"/>
+      <c r="ALM6" s="13"/>
+      <c r="ALN6" s="13"/>
+      <c r="ALO6" s="13"/>
+      <c r="ALP6" s="13"/>
+      <c r="ALQ6" s="13"/>
+      <c r="ALR6" s="13"/>
+      <c r="ALS6" s="13"/>
+      <c r="ALT6" s="13"/>
+      <c r="ALU6" s="13"/>
+      <c r="ALV6" s="13"/>
+      <c r="ALW6" s="13"/>
+      <c r="ALX6" s="13"/>
+      <c r="ALY6" s="13"/>
+      <c r="ALZ6" s="13"/>
+      <c r="AMA6" s="13"/>
+      <c r="AMB6" s="13"/>
+      <c r="AMC6" s="13"/>
+      <c r="AMD6" s="13"/>
+      <c r="AME6" s="13"/>
+      <c r="AMF6" s="13"/>
+      <c r="AMG6" s="13"/>
+      <c r="AMH6" s="13"/>
+      <c r="AMI6" s="13"/>
+      <c r="AMJ6" s="14"/>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="17" t="n">
-        <v>44100</v>
-      </c>
-      <c r="C4" s="18" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="AMJ4" s="15"/>
-    </row>
-    <row r="5" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="AMJ7" s="14"/>
+    </row>
+    <row r="8" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="19" t="n">
-        <v>36526</v>
-      </c>
-      <c r="C5" s="18" t="s">
+      <c r="B8" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="AMJ5" s="15"/>
-    </row>
-    <row r="6" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="s">
+      <c r="AMJ8" s="14"/>
+    </row>
+    <row r="9" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22" t="s">
+      <c r="B9" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="14"/>
-      <c r="AC6" s="14"/>
-      <c r="AD6" s="14"/>
-      <c r="AE6" s="14"/>
-      <c r="AF6" s="14"/>
-      <c r="AG6" s="14"/>
-      <c r="AH6" s="14"/>
-      <c r="AI6" s="14"/>
-      <c r="AJ6" s="14"/>
-      <c r="AK6" s="14"/>
-      <c r="AL6" s="14"/>
-      <c r="AM6" s="14"/>
-      <c r="AN6" s="14"/>
-      <c r="AO6" s="14"/>
-      <c r="AP6" s="14"/>
-      <c r="AQ6" s="14"/>
-      <c r="AR6" s="14"/>
-      <c r="AS6" s="14"/>
-      <c r="AT6" s="14"/>
-      <c r="AU6" s="14"/>
-      <c r="AV6" s="14"/>
-      <c r="AW6" s="14"/>
-      <c r="AX6" s="14"/>
-      <c r="AY6" s="14"/>
-      <c r="AZ6" s="14"/>
-      <c r="BA6" s="14"/>
-      <c r="BB6" s="14"/>
-      <c r="BC6" s="14"/>
-      <c r="BD6" s="14"/>
-      <c r="BE6" s="14"/>
-      <c r="BF6" s="14"/>
-      <c r="BG6" s="14"/>
-      <c r="BH6" s="14"/>
-      <c r="BI6" s="14"/>
-      <c r="BJ6" s="14"/>
-      <c r="BK6" s="14"/>
-      <c r="BL6" s="14"/>
-      <c r="BM6" s="14"/>
-      <c r="BN6" s="14"/>
-      <c r="BO6" s="14"/>
-      <c r="BP6" s="14"/>
-      <c r="BQ6" s="14"/>
-      <c r="BR6" s="14"/>
-      <c r="BS6" s="14"/>
-      <c r="BT6" s="14"/>
-      <c r="BU6" s="14"/>
-      <c r="BV6" s="14"/>
-      <c r="BW6" s="14"/>
-      <c r="BX6" s="14"/>
-      <c r="BY6" s="14"/>
-      <c r="BZ6" s="14"/>
-      <c r="CA6" s="14"/>
-      <c r="CB6" s="14"/>
-      <c r="CC6" s="14"/>
-      <c r="CD6" s="14"/>
-      <c r="CE6" s="14"/>
-      <c r="CF6" s="14"/>
-      <c r="CG6" s="14"/>
-      <c r="CH6" s="14"/>
-      <c r="CI6" s="14"/>
-      <c r="CJ6" s="14"/>
-      <c r="CK6" s="14"/>
-      <c r="CL6" s="14"/>
-      <c r="CM6" s="14"/>
-      <c r="CN6" s="14"/>
-      <c r="CO6" s="14"/>
-      <c r="CP6" s="14"/>
-      <c r="CQ6" s="14"/>
-      <c r="CR6" s="14"/>
-      <c r="CS6" s="14"/>
-      <c r="CT6" s="14"/>
-      <c r="CU6" s="14"/>
-      <c r="CV6" s="14"/>
-      <c r="CW6" s="14"/>
-      <c r="CX6" s="14"/>
-      <c r="CY6" s="14"/>
-      <c r="CZ6" s="14"/>
-      <c r="DA6" s="14"/>
-      <c r="DB6" s="14"/>
-      <c r="DC6" s="14"/>
-      <c r="DD6" s="14"/>
-      <c r="DE6" s="14"/>
-      <c r="DF6" s="14"/>
-      <c r="DG6" s="14"/>
-      <c r="DH6" s="14"/>
-      <c r="DI6" s="14"/>
-      <c r="DJ6" s="14"/>
-      <c r="DK6" s="14"/>
-      <c r="DL6" s="14"/>
-      <c r="DM6" s="14"/>
-      <c r="DN6" s="14"/>
-      <c r="DO6" s="14"/>
-      <c r="DP6" s="14"/>
-      <c r="DQ6" s="14"/>
-      <c r="DR6" s="14"/>
-      <c r="DS6" s="14"/>
-      <c r="DT6" s="14"/>
-      <c r="DU6" s="14"/>
-      <c r="DV6" s="14"/>
-      <c r="DW6" s="14"/>
-      <c r="DX6" s="14"/>
-      <c r="DY6" s="14"/>
-      <c r="DZ6" s="14"/>
-      <c r="EA6" s="14"/>
-      <c r="EB6" s="14"/>
-      <c r="EC6" s="14"/>
-      <c r="ED6" s="14"/>
-      <c r="EE6" s="14"/>
-      <c r="EF6" s="14"/>
-      <c r="EG6" s="14"/>
-      <c r="EH6" s="14"/>
-      <c r="EI6" s="14"/>
-      <c r="EJ6" s="14"/>
-      <c r="EK6" s="14"/>
-      <c r="EL6" s="14"/>
-      <c r="EM6" s="14"/>
-      <c r="EN6" s="14"/>
-      <c r="EO6" s="14"/>
-      <c r="EP6" s="14"/>
-      <c r="EQ6" s="14"/>
-      <c r="ER6" s="14"/>
-      <c r="ES6" s="14"/>
-      <c r="ET6" s="14"/>
-      <c r="EU6" s="14"/>
-      <c r="EV6" s="14"/>
-      <c r="EW6" s="14"/>
-      <c r="EX6" s="14"/>
-      <c r="EY6" s="14"/>
-      <c r="EZ6" s="14"/>
-      <c r="FA6" s="14"/>
-      <c r="FB6" s="14"/>
-      <c r="FC6" s="14"/>
-      <c r="FD6" s="14"/>
-      <c r="FE6" s="14"/>
-      <c r="FF6" s="14"/>
-      <c r="FG6" s="14"/>
-      <c r="FH6" s="14"/>
-      <c r="FI6" s="14"/>
-      <c r="FJ6" s="14"/>
-      <c r="FK6" s="14"/>
-      <c r="FL6" s="14"/>
-      <c r="FM6" s="14"/>
-      <c r="FN6" s="14"/>
-      <c r="FO6" s="14"/>
-      <c r="FP6" s="14"/>
-      <c r="FQ6" s="14"/>
-      <c r="FR6" s="14"/>
-      <c r="FS6" s="14"/>
-      <c r="FT6" s="14"/>
-      <c r="FU6" s="14"/>
-      <c r="FV6" s="14"/>
-      <c r="FW6" s="14"/>
-      <c r="FX6" s="14"/>
-      <c r="FY6" s="14"/>
-      <c r="FZ6" s="14"/>
-      <c r="GA6" s="14"/>
-      <c r="GB6" s="14"/>
-      <c r="GC6" s="14"/>
-      <c r="GD6" s="14"/>
-      <c r="GE6" s="14"/>
-      <c r="GF6" s="14"/>
-      <c r="GG6" s="14"/>
-      <c r="GH6" s="14"/>
-      <c r="GI6" s="14"/>
-      <c r="GJ6" s="14"/>
-      <c r="GK6" s="14"/>
-      <c r="GL6" s="14"/>
-      <c r="GM6" s="14"/>
-      <c r="GN6" s="14"/>
-      <c r="GO6" s="14"/>
-      <c r="GP6" s="14"/>
-      <c r="GQ6" s="14"/>
-      <c r="GR6" s="14"/>
-      <c r="GS6" s="14"/>
-      <c r="GT6" s="14"/>
-      <c r="GU6" s="14"/>
-      <c r="GV6" s="14"/>
-      <c r="GW6" s="14"/>
-      <c r="GX6" s="14"/>
-      <c r="GY6" s="14"/>
-      <c r="GZ6" s="14"/>
-      <c r="HA6" s="14"/>
-      <c r="HB6" s="14"/>
-      <c r="HC6" s="14"/>
-      <c r="HD6" s="14"/>
-      <c r="HE6" s="14"/>
-      <c r="HF6" s="14"/>
-      <c r="HG6" s="14"/>
-      <c r="HH6" s="14"/>
-      <c r="HI6" s="14"/>
-      <c r="HJ6" s="14"/>
-      <c r="HK6" s="14"/>
-      <c r="HL6" s="14"/>
-      <c r="HM6" s="14"/>
-      <c r="HN6" s="14"/>
-      <c r="HO6" s="14"/>
-      <c r="HP6" s="14"/>
-      <c r="HQ6" s="14"/>
-      <c r="HR6" s="14"/>
-      <c r="HS6" s="14"/>
-      <c r="HT6" s="14"/>
-      <c r="HU6" s="14"/>
-      <c r="HV6" s="14"/>
-      <c r="HW6" s="14"/>
-      <c r="HX6" s="14"/>
-      <c r="HY6" s="14"/>
-      <c r="HZ6" s="14"/>
-      <c r="IA6" s="14"/>
-      <c r="IB6" s="14"/>
-      <c r="IC6" s="14"/>
-      <c r="ID6" s="14"/>
-      <c r="IE6" s="14"/>
-      <c r="IF6" s="14"/>
-      <c r="IG6" s="14"/>
-      <c r="IH6" s="14"/>
-      <c r="II6" s="14"/>
-      <c r="IJ6" s="14"/>
-      <c r="IK6" s="14"/>
-      <c r="IL6" s="14"/>
-      <c r="IM6" s="14"/>
-      <c r="IN6" s="14"/>
-      <c r="IO6" s="14"/>
-      <c r="IP6" s="14"/>
-      <c r="IQ6" s="14"/>
-      <c r="IR6" s="14"/>
-      <c r="IS6" s="14"/>
-      <c r="IT6" s="14"/>
-      <c r="IU6" s="14"/>
-      <c r="IV6" s="14"/>
-      <c r="IW6" s="14"/>
-      <c r="IX6" s="14"/>
-      <c r="IY6" s="14"/>
-      <c r="IZ6" s="14"/>
-      <c r="JA6" s="14"/>
-      <c r="JB6" s="14"/>
-      <c r="JC6" s="14"/>
-      <c r="JD6" s="14"/>
-      <c r="JE6" s="14"/>
-      <c r="JF6" s="14"/>
-      <c r="JG6" s="14"/>
-      <c r="JH6" s="14"/>
-      <c r="JI6" s="14"/>
-      <c r="JJ6" s="14"/>
-      <c r="JK6" s="14"/>
-      <c r="JL6" s="14"/>
-      <c r="JM6" s="14"/>
-      <c r="JN6" s="14"/>
-      <c r="JO6" s="14"/>
-      <c r="JP6" s="14"/>
-      <c r="JQ6" s="14"/>
-      <c r="JR6" s="14"/>
-      <c r="JS6" s="14"/>
-      <c r="JT6" s="14"/>
-      <c r="JU6" s="14"/>
-      <c r="JV6" s="14"/>
-      <c r="JW6" s="14"/>
-      <c r="JX6" s="14"/>
-      <c r="JY6" s="14"/>
-      <c r="JZ6" s="14"/>
-      <c r="KA6" s="14"/>
-      <c r="KB6" s="14"/>
-      <c r="KC6" s="14"/>
-      <c r="KD6" s="14"/>
-      <c r="KE6" s="14"/>
-      <c r="KF6" s="14"/>
-      <c r="KG6" s="14"/>
-      <c r="KH6" s="14"/>
-      <c r="KI6" s="14"/>
-      <c r="KJ6" s="14"/>
-      <c r="KK6" s="14"/>
-      <c r="KL6" s="14"/>
-      <c r="KM6" s="14"/>
-      <c r="KN6" s="14"/>
-      <c r="KO6" s="14"/>
-      <c r="KP6" s="14"/>
-      <c r="KQ6" s="14"/>
-      <c r="KR6" s="14"/>
-      <c r="KS6" s="14"/>
-      <c r="KT6" s="14"/>
-      <c r="KU6" s="14"/>
-      <c r="KV6" s="14"/>
-      <c r="KW6" s="14"/>
-      <c r="KX6" s="14"/>
-      <c r="KY6" s="14"/>
-      <c r="KZ6" s="14"/>
-      <c r="LA6" s="14"/>
-      <c r="LB6" s="14"/>
-      <c r="LC6" s="14"/>
-      <c r="LD6" s="14"/>
-      <c r="LE6" s="14"/>
-      <c r="LF6" s="14"/>
-      <c r="LG6" s="14"/>
-      <c r="LH6" s="14"/>
-      <c r="LI6" s="14"/>
-      <c r="LJ6" s="14"/>
-      <c r="LK6" s="14"/>
-      <c r="LL6" s="14"/>
-      <c r="LM6" s="14"/>
-      <c r="LN6" s="14"/>
-      <c r="LO6" s="14"/>
-      <c r="LP6" s="14"/>
-      <c r="LQ6" s="14"/>
-      <c r="LR6" s="14"/>
-      <c r="LS6" s="14"/>
-      <c r="LT6" s="14"/>
-      <c r="LU6" s="14"/>
-      <c r="LV6" s="14"/>
-      <c r="LW6" s="14"/>
-      <c r="LX6" s="14"/>
-      <c r="LY6" s="14"/>
-      <c r="LZ6" s="14"/>
-      <c r="MA6" s="14"/>
-      <c r="MB6" s="14"/>
-      <c r="MC6" s="14"/>
-      <c r="MD6" s="14"/>
-      <c r="ME6" s="14"/>
-      <c r="MF6" s="14"/>
-      <c r="MG6" s="14"/>
-      <c r="MH6" s="14"/>
-      <c r="MI6" s="14"/>
-      <c r="MJ6" s="14"/>
-      <c r="MK6" s="14"/>
-      <c r="ML6" s="14"/>
-      <c r="MM6" s="14"/>
-      <c r="MN6" s="14"/>
-      <c r="MO6" s="14"/>
-      <c r="MP6" s="14"/>
-      <c r="MQ6" s="14"/>
-      <c r="MR6" s="14"/>
-      <c r="MS6" s="14"/>
-      <c r="MT6" s="14"/>
-      <c r="MU6" s="14"/>
-      <c r="MV6" s="14"/>
-      <c r="MW6" s="14"/>
-      <c r="MX6" s="14"/>
-      <c r="MY6" s="14"/>
-      <c r="MZ6" s="14"/>
-      <c r="NA6" s="14"/>
-      <c r="NB6" s="14"/>
-      <c r="NC6" s="14"/>
-      <c r="ND6" s="14"/>
-      <c r="NE6" s="14"/>
-      <c r="NF6" s="14"/>
-      <c r="NG6" s="14"/>
-      <c r="NH6" s="14"/>
-      <c r="NI6" s="14"/>
-      <c r="NJ6" s="14"/>
-      <c r="NK6" s="14"/>
-      <c r="NL6" s="14"/>
-      <c r="NM6" s="14"/>
-      <c r="NN6" s="14"/>
-      <c r="NO6" s="14"/>
-      <c r="NP6" s="14"/>
-      <c r="NQ6" s="14"/>
-      <c r="NR6" s="14"/>
-      <c r="NS6" s="14"/>
-      <c r="NT6" s="14"/>
-      <c r="NU6" s="14"/>
-      <c r="NV6" s="14"/>
-      <c r="NW6" s="14"/>
-      <c r="NX6" s="14"/>
-      <c r="NY6" s="14"/>
-      <c r="NZ6" s="14"/>
-      <c r="OA6" s="14"/>
-      <c r="OB6" s="14"/>
-      <c r="OC6" s="14"/>
-      <c r="OD6" s="14"/>
-      <c r="OE6" s="14"/>
-      <c r="OF6" s="14"/>
-      <c r="OG6" s="14"/>
-      <c r="OH6" s="14"/>
-      <c r="OI6" s="14"/>
-      <c r="OJ6" s="14"/>
-      <c r="OK6" s="14"/>
-      <c r="OL6" s="14"/>
-      <c r="OM6" s="14"/>
-      <c r="ON6" s="14"/>
-      <c r="OO6" s="14"/>
-      <c r="OP6" s="14"/>
-      <c r="OQ6" s="14"/>
-      <c r="OR6" s="14"/>
-      <c r="OS6" s="14"/>
-      <c r="OT6" s="14"/>
-      <c r="OU6" s="14"/>
-      <c r="OV6" s="14"/>
-      <c r="OW6" s="14"/>
-      <c r="OX6" s="14"/>
-      <c r="OY6" s="14"/>
-      <c r="OZ6" s="14"/>
-      <c r="PA6" s="14"/>
-      <c r="PB6" s="14"/>
-      <c r="PC6" s="14"/>
-      <c r="PD6" s="14"/>
-      <c r="PE6" s="14"/>
-      <c r="PF6" s="14"/>
-      <c r="PG6" s="14"/>
-      <c r="PH6" s="14"/>
-      <c r="PI6" s="14"/>
-      <c r="PJ6" s="14"/>
-      <c r="PK6" s="14"/>
-      <c r="PL6" s="14"/>
-      <c r="PM6" s="14"/>
-      <c r="PN6" s="14"/>
-      <c r="PO6" s="14"/>
-      <c r="PP6" s="14"/>
-      <c r="PQ6" s="14"/>
-      <c r="PR6" s="14"/>
-      <c r="PS6" s="14"/>
-      <c r="PT6" s="14"/>
-      <c r="PU6" s="14"/>
-      <c r="PV6" s="14"/>
-      <c r="PW6" s="14"/>
-      <c r="PX6" s="14"/>
-      <c r="PY6" s="14"/>
-      <c r="PZ6" s="14"/>
-      <c r="QA6" s="14"/>
-      <c r="QB6" s="14"/>
-      <c r="QC6" s="14"/>
-      <c r="QD6" s="14"/>
-      <c r="QE6" s="14"/>
-      <c r="QF6" s="14"/>
-      <c r="QG6" s="14"/>
-      <c r="QH6" s="14"/>
-      <c r="QI6" s="14"/>
-      <c r="QJ6" s="14"/>
-      <c r="QK6" s="14"/>
-      <c r="QL6" s="14"/>
-      <c r="QM6" s="14"/>
-      <c r="QN6" s="14"/>
-      <c r="QO6" s="14"/>
-      <c r="QP6" s="14"/>
-      <c r="QQ6" s="14"/>
-      <c r="QR6" s="14"/>
-      <c r="QS6" s="14"/>
-      <c r="QT6" s="14"/>
-      <c r="QU6" s="14"/>
-      <c r="QV6" s="14"/>
-      <c r="QW6" s="14"/>
-      <c r="QX6" s="14"/>
-      <c r="QY6" s="14"/>
-      <c r="QZ6" s="14"/>
-      <c r="RA6" s="14"/>
-      <c r="RB6" s="14"/>
-      <c r="RC6" s="14"/>
-      <c r="RD6" s="14"/>
-      <c r="RE6" s="14"/>
-      <c r="RF6" s="14"/>
-      <c r="RG6" s="14"/>
-      <c r="RH6" s="14"/>
-      <c r="RI6" s="14"/>
-      <c r="RJ6" s="14"/>
-      <c r="RK6" s="14"/>
-      <c r="RL6" s="14"/>
-      <c r="RM6" s="14"/>
-      <c r="RN6" s="14"/>
-      <c r="RO6" s="14"/>
-      <c r="RP6" s="14"/>
-      <c r="RQ6" s="14"/>
-      <c r="RR6" s="14"/>
-      <c r="RS6" s="14"/>
-      <c r="RT6" s="14"/>
-      <c r="RU6" s="14"/>
-      <c r="RV6" s="14"/>
-      <c r="RW6" s="14"/>
-      <c r="RX6" s="14"/>
-      <c r="RY6" s="14"/>
-      <c r="RZ6" s="14"/>
-      <c r="SA6" s="14"/>
-      <c r="SB6" s="14"/>
-      <c r="SC6" s="14"/>
-      <c r="SD6" s="14"/>
-      <c r="SE6" s="14"/>
-      <c r="SF6" s="14"/>
-      <c r="SG6" s="14"/>
-      <c r="SH6" s="14"/>
-      <c r="SI6" s="14"/>
-      <c r="SJ6" s="14"/>
-      <c r="SK6" s="14"/>
-      <c r="SL6" s="14"/>
-      <c r="SM6" s="14"/>
-      <c r="SN6" s="14"/>
-      <c r="SO6" s="14"/>
-      <c r="SP6" s="14"/>
-      <c r="SQ6" s="14"/>
-      <c r="SR6" s="14"/>
-      <c r="SS6" s="14"/>
-      <c r="ST6" s="14"/>
-      <c r="SU6" s="14"/>
-      <c r="SV6" s="14"/>
-      <c r="SW6" s="14"/>
-      <c r="SX6" s="14"/>
-      <c r="SY6" s="14"/>
-      <c r="SZ6" s="14"/>
-      <c r="TA6" s="14"/>
-      <c r="TB6" s="14"/>
-      <c r="TC6" s="14"/>
-      <c r="TD6" s="14"/>
-      <c r="TE6" s="14"/>
-      <c r="TF6" s="14"/>
-      <c r="TG6" s="14"/>
-      <c r="TH6" s="14"/>
-      <c r="TI6" s="14"/>
-      <c r="TJ6" s="14"/>
-      <c r="TK6" s="14"/>
-      <c r="TL6" s="14"/>
-      <c r="TM6" s="14"/>
-      <c r="TN6" s="14"/>
-      <c r="TO6" s="14"/>
-      <c r="TP6" s="14"/>
-      <c r="TQ6" s="14"/>
-      <c r="TR6" s="14"/>
-      <c r="TS6" s="14"/>
-      <c r="TT6" s="14"/>
-      <c r="TU6" s="14"/>
-      <c r="TV6" s="14"/>
-      <c r="TW6" s="14"/>
-      <c r="TX6" s="14"/>
-      <c r="TY6" s="14"/>
-      <c r="TZ6" s="14"/>
-      <c r="UA6" s="14"/>
-      <c r="UB6" s="14"/>
-      <c r="UC6" s="14"/>
-      <c r="UD6" s="14"/>
-      <c r="UE6" s="14"/>
-      <c r="UF6" s="14"/>
-      <c r="UG6" s="14"/>
-      <c r="UH6" s="14"/>
-      <c r="UI6" s="14"/>
-      <c r="UJ6" s="14"/>
-      <c r="UK6" s="14"/>
-      <c r="UL6" s="14"/>
-      <c r="UM6" s="14"/>
-      <c r="UN6" s="14"/>
-      <c r="UO6" s="14"/>
-      <c r="UP6" s="14"/>
-      <c r="UQ6" s="14"/>
-      <c r="UR6" s="14"/>
-      <c r="US6" s="14"/>
-      <c r="UT6" s="14"/>
-      <c r="UU6" s="14"/>
-      <c r="UV6" s="14"/>
-      <c r="UW6" s="14"/>
-      <c r="UX6" s="14"/>
-      <c r="UY6" s="14"/>
-      <c r="UZ6" s="14"/>
-      <c r="VA6" s="14"/>
-      <c r="VB6" s="14"/>
-      <c r="VC6" s="14"/>
-      <c r="VD6" s="14"/>
-      <c r="VE6" s="14"/>
-      <c r="VF6" s="14"/>
-      <c r="VG6" s="14"/>
-      <c r="VH6" s="14"/>
-      <c r="VI6" s="14"/>
-      <c r="VJ6" s="14"/>
-      <c r="VK6" s="14"/>
-      <c r="VL6" s="14"/>
-      <c r="VM6" s="14"/>
-      <c r="VN6" s="14"/>
-      <c r="VO6" s="14"/>
-      <c r="VP6" s="14"/>
-      <c r="VQ6" s="14"/>
-      <c r="VR6" s="14"/>
-      <c r="VS6" s="14"/>
-      <c r="VT6" s="14"/>
-      <c r="VU6" s="14"/>
-      <c r="VV6" s="14"/>
-      <c r="VW6" s="14"/>
-      <c r="VX6" s="14"/>
-      <c r="VY6" s="14"/>
-      <c r="VZ6" s="14"/>
-      <c r="WA6" s="14"/>
-      <c r="WB6" s="14"/>
-      <c r="WC6" s="14"/>
-      <c r="WD6" s="14"/>
-      <c r="WE6" s="14"/>
-      <c r="WF6" s="14"/>
-      <c r="WG6" s="14"/>
-      <c r="WH6" s="14"/>
-      <c r="WI6" s="14"/>
-      <c r="WJ6" s="14"/>
-      <c r="WK6" s="14"/>
-      <c r="WL6" s="14"/>
-      <c r="WM6" s="14"/>
-      <c r="WN6" s="14"/>
-      <c r="WO6" s="14"/>
-      <c r="WP6" s="14"/>
-      <c r="WQ6" s="14"/>
-      <c r="WR6" s="14"/>
-      <c r="WS6" s="14"/>
-      <c r="WT6" s="14"/>
-      <c r="WU6" s="14"/>
-      <c r="WV6" s="14"/>
-      <c r="WW6" s="14"/>
-      <c r="WX6" s="14"/>
-      <c r="WY6" s="14"/>
-      <c r="WZ6" s="14"/>
-      <c r="XA6" s="14"/>
-      <c r="XB6" s="14"/>
-      <c r="XC6" s="14"/>
-      <c r="XD6" s="14"/>
-      <c r="XE6" s="14"/>
-      <c r="XF6" s="14"/>
-      <c r="XG6" s="14"/>
-      <c r="XH6" s="14"/>
-      <c r="XI6" s="14"/>
-      <c r="XJ6" s="14"/>
-      <c r="XK6" s="14"/>
-      <c r="XL6" s="14"/>
-      <c r="XM6" s="14"/>
-      <c r="XN6" s="14"/>
-      <c r="XO6" s="14"/>
-      <c r="XP6" s="14"/>
-      <c r="XQ6" s="14"/>
-      <c r="XR6" s="14"/>
-      <c r="XS6" s="14"/>
-      <c r="XT6" s="14"/>
-      <c r="XU6" s="14"/>
-      <c r="XV6" s="14"/>
-      <c r="XW6" s="14"/>
-      <c r="XX6" s="14"/>
-      <c r="XY6" s="14"/>
-      <c r="XZ6" s="14"/>
-      <c r="YA6" s="14"/>
-      <c r="YB6" s="14"/>
-      <c r="YC6" s="14"/>
-      <c r="YD6" s="14"/>
-      <c r="YE6" s="14"/>
-      <c r="YF6" s="14"/>
-      <c r="YG6" s="14"/>
-      <c r="YH6" s="14"/>
-      <c r="YI6" s="14"/>
-      <c r="YJ6" s="14"/>
-      <c r="YK6" s="14"/>
-      <c r="YL6" s="14"/>
-      <c r="YM6" s="14"/>
-      <c r="YN6" s="14"/>
-      <c r="YO6" s="14"/>
-      <c r="YP6" s="14"/>
-      <c r="YQ6" s="14"/>
-      <c r="YR6" s="14"/>
-      <c r="YS6" s="14"/>
-      <c r="YT6" s="14"/>
-      <c r="YU6" s="14"/>
-      <c r="YV6" s="14"/>
-      <c r="YW6" s="14"/>
-      <c r="YX6" s="14"/>
-      <c r="YY6" s="14"/>
-      <c r="YZ6" s="14"/>
-      <c r="ZA6" s="14"/>
-      <c r="ZB6" s="14"/>
-      <c r="ZC6" s="14"/>
-      <c r="ZD6" s="14"/>
-      <c r="ZE6" s="14"/>
-      <c r="ZF6" s="14"/>
-      <c r="ZG6" s="14"/>
-      <c r="ZH6" s="14"/>
-      <c r="ZI6" s="14"/>
-      <c r="ZJ6" s="14"/>
-      <c r="ZK6" s="14"/>
-      <c r="ZL6" s="14"/>
-      <c r="ZM6" s="14"/>
-      <c r="ZN6" s="14"/>
-      <c r="ZO6" s="14"/>
-      <c r="ZP6" s="14"/>
-      <c r="ZQ6" s="14"/>
-      <c r="ZR6" s="14"/>
-      <c r="ZS6" s="14"/>
-      <c r="ZT6" s="14"/>
-      <c r="ZU6" s="14"/>
-      <c r="ZV6" s="14"/>
-      <c r="ZW6" s="14"/>
-      <c r="ZX6" s="14"/>
-      <c r="ZY6" s="14"/>
-      <c r="ZZ6" s="14"/>
-      <c r="AAA6" s="14"/>
-      <c r="AAB6" s="14"/>
-      <c r="AAC6" s="14"/>
-      <c r="AAD6" s="14"/>
-      <c r="AAE6" s="14"/>
-      <c r="AAF6" s="14"/>
-      <c r="AAG6" s="14"/>
-      <c r="AAH6" s="14"/>
-      <c r="AAI6" s="14"/>
-      <c r="AAJ6" s="14"/>
-      <c r="AAK6" s="14"/>
-      <c r="AAL6" s="14"/>
-      <c r="AAM6" s="14"/>
-      <c r="AAN6" s="14"/>
-      <c r="AAO6" s="14"/>
-      <c r="AAP6" s="14"/>
-      <c r="AAQ6" s="14"/>
-      <c r="AAR6" s="14"/>
-      <c r="AAS6" s="14"/>
-      <c r="AAT6" s="14"/>
-      <c r="AAU6" s="14"/>
-      <c r="AAV6" s="14"/>
-      <c r="AAW6" s="14"/>
-      <c r="AAX6" s="14"/>
-      <c r="AAY6" s="14"/>
-      <c r="AAZ6" s="14"/>
-      <c r="ABA6" s="14"/>
-      <c r="ABB6" s="14"/>
-      <c r="ABC6" s="14"/>
-      <c r="ABD6" s="14"/>
-      <c r="ABE6" s="14"/>
-      <c r="ABF6" s="14"/>
-      <c r="ABG6" s="14"/>
-      <c r="ABH6" s="14"/>
-      <c r="ABI6" s="14"/>
-      <c r="ABJ6" s="14"/>
-      <c r="ABK6" s="14"/>
-      <c r="ABL6" s="14"/>
-      <c r="ABM6" s="14"/>
-      <c r="ABN6" s="14"/>
-      <c r="ABO6" s="14"/>
-      <c r="ABP6" s="14"/>
-      <c r="ABQ6" s="14"/>
-      <c r="ABR6" s="14"/>
-      <c r="ABS6" s="14"/>
-      <c r="ABT6" s="14"/>
-      <c r="ABU6" s="14"/>
-      <c r="ABV6" s="14"/>
-      <c r="ABW6" s="14"/>
-      <c r="ABX6" s="14"/>
-      <c r="ABY6" s="14"/>
-      <c r="ABZ6" s="14"/>
-      <c r="ACA6" s="14"/>
-      <c r="ACB6" s="14"/>
-      <c r="ACC6" s="14"/>
-      <c r="ACD6" s="14"/>
-      <c r="ACE6" s="14"/>
-      <c r="ACF6" s="14"/>
-      <c r="ACG6" s="14"/>
-      <c r="ACH6" s="14"/>
-      <c r="ACI6" s="14"/>
-      <c r="ACJ6" s="14"/>
-      <c r="ACK6" s="14"/>
-      <c r="ACL6" s="14"/>
-      <c r="ACM6" s="14"/>
-      <c r="ACN6" s="14"/>
-      <c r="ACO6" s="14"/>
-      <c r="ACP6" s="14"/>
-      <c r="ACQ6" s="14"/>
-      <c r="ACR6" s="14"/>
-      <c r="ACS6" s="14"/>
-      <c r="ACT6" s="14"/>
-      <c r="ACU6" s="14"/>
-      <c r="ACV6" s="14"/>
-      <c r="ACW6" s="14"/>
-      <c r="ACX6" s="14"/>
-      <c r="ACY6" s="14"/>
-      <c r="ACZ6" s="14"/>
-      <c r="ADA6" s="14"/>
-      <c r="ADB6" s="14"/>
-      <c r="ADC6" s="14"/>
-      <c r="ADD6" s="14"/>
-      <c r="ADE6" s="14"/>
-      <c r="ADF6" s="14"/>
-      <c r="ADG6" s="14"/>
-      <c r="ADH6" s="14"/>
-      <c r="ADI6" s="14"/>
-      <c r="ADJ6" s="14"/>
-      <c r="ADK6" s="14"/>
-      <c r="ADL6" s="14"/>
-      <c r="ADM6" s="14"/>
-      <c r="ADN6" s="14"/>
-      <c r="ADO6" s="14"/>
-      <c r="ADP6" s="14"/>
-      <c r="ADQ6" s="14"/>
-      <c r="ADR6" s="14"/>
-      <c r="ADS6" s="14"/>
-      <c r="ADT6" s="14"/>
-      <c r="ADU6" s="14"/>
-      <c r="ADV6" s="14"/>
-      <c r="ADW6" s="14"/>
-      <c r="ADX6" s="14"/>
-      <c r="ADY6" s="14"/>
-      <c r="ADZ6" s="14"/>
-      <c r="AEA6" s="14"/>
-      <c r="AEB6" s="14"/>
-      <c r="AEC6" s="14"/>
-      <c r="AED6" s="14"/>
-      <c r="AEE6" s="14"/>
-      <c r="AEF6" s="14"/>
-      <c r="AEG6" s="14"/>
-      <c r="AEH6" s="14"/>
-      <c r="AEI6" s="14"/>
-      <c r="AEJ6" s="14"/>
-      <c r="AEK6" s="14"/>
-      <c r="AEL6" s="14"/>
-      <c r="AEM6" s="14"/>
-      <c r="AEN6" s="14"/>
-      <c r="AEO6" s="14"/>
-      <c r="AEP6" s="14"/>
-      <c r="AEQ6" s="14"/>
-      <c r="AER6" s="14"/>
-      <c r="AES6" s="14"/>
-      <c r="AET6" s="14"/>
-      <c r="AEU6" s="14"/>
-      <c r="AEV6" s="14"/>
-      <c r="AEW6" s="14"/>
-      <c r="AEX6" s="14"/>
-      <c r="AEY6" s="14"/>
-      <c r="AEZ6" s="14"/>
-      <c r="AFA6" s="14"/>
-      <c r="AFB6" s="14"/>
-      <c r="AFC6" s="14"/>
-      <c r="AFD6" s="14"/>
-      <c r="AFE6" s="14"/>
-      <c r="AFF6" s="14"/>
-      <c r="AFG6" s="14"/>
-      <c r="AFH6" s="14"/>
-      <c r="AFI6" s="14"/>
-      <c r="AFJ6" s="14"/>
-      <c r="AFK6" s="14"/>
-      <c r="AFL6" s="14"/>
-      <c r="AFM6" s="14"/>
-      <c r="AFN6" s="14"/>
-      <c r="AFO6" s="14"/>
-      <c r="AFP6" s="14"/>
-      <c r="AFQ6" s="14"/>
-      <c r="AFR6" s="14"/>
-      <c r="AFS6" s="14"/>
-      <c r="AFT6" s="14"/>
-      <c r="AFU6" s="14"/>
-      <c r="AFV6" s="14"/>
-      <c r="AFW6" s="14"/>
-      <c r="AFX6" s="14"/>
-      <c r="AFY6" s="14"/>
-      <c r="AFZ6" s="14"/>
-      <c r="AGA6" s="14"/>
-      <c r="AGB6" s="14"/>
-      <c r="AGC6" s="14"/>
-      <c r="AGD6" s="14"/>
-      <c r="AGE6" s="14"/>
-      <c r="AGF6" s="14"/>
-      <c r="AGG6" s="14"/>
-      <c r="AGH6" s="14"/>
-      <c r="AGI6" s="14"/>
-      <c r="AGJ6" s="14"/>
-      <c r="AGK6" s="14"/>
-      <c r="AGL6" s="14"/>
-      <c r="AGM6" s="14"/>
-      <c r="AGN6" s="14"/>
-      <c r="AGO6" s="14"/>
-      <c r="AGP6" s="14"/>
-      <c r="AGQ6" s="14"/>
-      <c r="AGR6" s="14"/>
-      <c r="AGS6" s="14"/>
-      <c r="AGT6" s="14"/>
-      <c r="AGU6" s="14"/>
-      <c r="AGV6" s="14"/>
-      <c r="AGW6" s="14"/>
-      <c r="AGX6" s="14"/>
-      <c r="AGY6" s="14"/>
-      <c r="AGZ6" s="14"/>
-      <c r="AHA6" s="14"/>
-      <c r="AHB6" s="14"/>
-      <c r="AHC6" s="14"/>
-      <c r="AHD6" s="14"/>
-      <c r="AHE6" s="14"/>
-      <c r="AHF6" s="14"/>
-      <c r="AHG6" s="14"/>
-      <c r="AHH6" s="14"/>
-      <c r="AHI6" s="14"/>
-      <c r="AHJ6" s="14"/>
-      <c r="AHK6" s="14"/>
-      <c r="AHL6" s="14"/>
-      <c r="AHM6" s="14"/>
-      <c r="AHN6" s="14"/>
-      <c r="AHO6" s="14"/>
-      <c r="AHP6" s="14"/>
-      <c r="AHQ6" s="14"/>
-      <c r="AHR6" s="14"/>
-      <c r="AHS6" s="14"/>
-      <c r="AHT6" s="14"/>
-      <c r="AHU6" s="14"/>
-      <c r="AHV6" s="14"/>
-      <c r="AHW6" s="14"/>
-      <c r="AHX6" s="14"/>
-      <c r="AHY6" s="14"/>
-      <c r="AHZ6" s="14"/>
-      <c r="AIA6" s="14"/>
-      <c r="AIB6" s="14"/>
-      <c r="AIC6" s="14"/>
-      <c r="AID6" s="14"/>
-      <c r="AIE6" s="14"/>
-      <c r="AIF6" s="14"/>
-      <c r="AIG6" s="14"/>
-      <c r="AIH6" s="14"/>
-      <c r="AII6" s="14"/>
-      <c r="AIJ6" s="14"/>
-      <c r="AIK6" s="14"/>
-      <c r="AIL6" s="14"/>
-      <c r="AIM6" s="14"/>
-      <c r="AIN6" s="14"/>
-      <c r="AIO6" s="14"/>
-      <c r="AIP6" s="14"/>
-      <c r="AIQ6" s="14"/>
-      <c r="AIR6" s="14"/>
-      <c r="AIS6" s="14"/>
-      <c r="AIT6" s="14"/>
-      <c r="AIU6" s="14"/>
-      <c r="AIV6" s="14"/>
-      <c r="AIW6" s="14"/>
-      <c r="AIX6" s="14"/>
-      <c r="AIY6" s="14"/>
-      <c r="AIZ6" s="14"/>
-      <c r="AJA6" s="14"/>
-      <c r="AJB6" s="14"/>
-      <c r="AJC6" s="14"/>
-      <c r="AJD6" s="14"/>
-      <c r="AJE6" s="14"/>
-      <c r="AJF6" s="14"/>
-      <c r="AJG6" s="14"/>
-      <c r="AJH6" s="14"/>
-      <c r="AJI6" s="14"/>
-      <c r="AJJ6" s="14"/>
-      <c r="AJK6" s="14"/>
-      <c r="AJL6" s="14"/>
-      <c r="AJM6" s="14"/>
-      <c r="AJN6" s="14"/>
-      <c r="AJO6" s="14"/>
-      <c r="AJP6" s="14"/>
-      <c r="AJQ6" s="14"/>
-      <c r="AJR6" s="14"/>
-      <c r="AJS6" s="14"/>
-      <c r="AJT6" s="14"/>
-      <c r="AJU6" s="14"/>
-      <c r="AJV6" s="14"/>
-      <c r="AJW6" s="14"/>
-      <c r="AJX6" s="14"/>
-      <c r="AJY6" s="14"/>
-      <c r="AJZ6" s="14"/>
-      <c r="AKA6" s="14"/>
-      <c r="AKB6" s="14"/>
-      <c r="AKC6" s="14"/>
-      <c r="AKD6" s="14"/>
-      <c r="AKE6" s="14"/>
-      <c r="AKF6" s="14"/>
-      <c r="AKG6" s="14"/>
-      <c r="AKH6" s="14"/>
-      <c r="AKI6" s="14"/>
-      <c r="AKJ6" s="14"/>
-      <c r="AKK6" s="14"/>
-      <c r="AKL6" s="14"/>
-      <c r="AKM6" s="14"/>
-      <c r="AKN6" s="14"/>
-      <c r="AKO6" s="14"/>
-      <c r="AKP6" s="14"/>
-      <c r="AKQ6" s="14"/>
-      <c r="AKR6" s="14"/>
-      <c r="AKS6" s="14"/>
-      <c r="AKT6" s="14"/>
-      <c r="AKU6" s="14"/>
-      <c r="AKV6" s="14"/>
-      <c r="AKW6" s="14"/>
-      <c r="AKX6" s="14"/>
-      <c r="AKY6" s="14"/>
-      <c r="AKZ6" s="14"/>
-      <c r="ALA6" s="14"/>
-      <c r="ALB6" s="14"/>
-      <c r="ALC6" s="14"/>
-      <c r="ALD6" s="14"/>
-      <c r="ALE6" s="14"/>
-      <c r="ALF6" s="14"/>
-      <c r="ALG6" s="14"/>
-      <c r="ALH6" s="14"/>
-      <c r="ALI6" s="14"/>
-      <c r="ALJ6" s="14"/>
-      <c r="ALK6" s="14"/>
-      <c r="ALL6" s="14"/>
-      <c r="ALM6" s="14"/>
-      <c r="ALN6" s="14"/>
-      <c r="ALO6" s="14"/>
-      <c r="ALP6" s="14"/>
-      <c r="ALQ6" s="14"/>
-      <c r="ALR6" s="14"/>
-      <c r="ALS6" s="14"/>
-      <c r="ALT6" s="14"/>
-      <c r="ALU6" s="14"/>
-      <c r="ALV6" s="14"/>
-      <c r="ALW6" s="14"/>
-      <c r="ALX6" s="14"/>
-      <c r="ALY6" s="14"/>
-      <c r="ALZ6" s="14"/>
-      <c r="AMA6" s="14"/>
-      <c r="AMB6" s="14"/>
-      <c r="AMC6" s="14"/>
-      <c r="AMD6" s="14"/>
-      <c r="AME6" s="14"/>
-      <c r="AMF6" s="14"/>
-      <c r="AMG6" s="14"/>
-      <c r="AMH6" s="14"/>
-      <c r="AMI6" s="14"/>
-      <c r="AMJ6" s="15"/>
-    </row>
-    <row r="7" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="s">
+      <c r="AMJ9" s="14"/>
+    </row>
+    <row r="10" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="18" t="s">
+      <c r="B10" s="22" t="n">
+        <v>42000</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AMJ7" s="15"/>
-    </row>
-    <row r="8" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="AMJ8" s="15"/>
-    </row>
-    <row r="9" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="AMJ9" s="15"/>
-    </row>
-    <row r="10" s="14" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="23" t="n">
-        <v>42000</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="AMJ10" s="15"/>
+      <c r="AMJ10" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3425,65 +3353,65 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="42.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="5" style="28" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="56.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="20.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="5" style="27" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1003" min="29" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>38</v>
+      <c r="A1" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="str">
+      <c r="A2" s="29" t="str">
         <f aca="false">"/path/from/audio/folder"</f>
         <v>/path/from/audio/folder</v>
       </c>
-      <c r="B2" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="32" t="n">
+      <c r="B2" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="31" t="n">
         <v>45089.8854166667</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>14</v>
+      <c r="D2" s="26" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="31"/>
+      <c r="C7" s="30"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3513,44 +3441,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="11.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>41</v>
+      <c r="A1" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="34" t="n">
+      <c r="A2" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="33" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="34" t="n">
+      <c r="C2" s="33" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3580,35 +3508,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="18.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>44</v>
+      <c r="A1" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="34" t="n">
+      <c r="A2" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="33" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="27"/>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="27"/>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="27"/>
+      <c r="B6" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3638,40 +3566,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="20.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1018" style="35" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1018" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>48</v>
+      <c r="A1" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="36" t="n">
+      <c r="A2" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="34" t="n">
         <v>44927</v>
       </c>
-      <c r="C2" s="36" t="n">
+      <c r="C2" s="34" t="n">
         <v>45292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="27"/>
+      <c r="C4" s="26"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3701,60 +3629,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="34" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="33" width="18.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="29" t="s">
+      <c r="A1" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3790,43 +3718,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="10.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="41" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="41" width="15.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="42" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="39" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="15.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1014" style="35" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1014" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>56</v>
+      <c r="A1" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="40" t="n">
+      <c r="A2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="41" t="n">
+      <c r="C2" s="39" t="n">
         <v>1000</v>
       </c>
-      <c r="D2" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="42" t="str">
+      <c r="D2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="40" t="str">
         <f aca="false">VLOOKUP(A2,ListExtractors!$A$2:$B$1048576,2,0)</f>
         <v>The VGGish neural network.</v>
       </c>
@@ -3865,38 +3793,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="42" width="15.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1012" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
-        <v>59</v>
+      <c r="A1" s="41" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="45" t="str">
+      <c r="A2" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="40" t="str">
         <f aca="false">VLOOKUP(A2,ListDigesters!$A$2:$B$1048576,2,0)</f>
         <v>The silhouette between subtypes of a given cluster.</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="45" t="str">
+      <c r="A3" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="40" t="str">
         <f aca="false">VLOOKUP(A3,ListDigesters!$A$2:$B$1048576,2,0)</f>
         <v>The overlap between subtypes of a given cluster.</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="45" t="str">
+      <c r="A4" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="40" t="str">
         <f aca="false">VLOOKUP(A4,ListDigesters!$A$2:$B$1048576,2,0)</f>
         <v>Contingency between two clusters.</v>
       </c>

</xml_diff>

<commit_message>
fix(Examples/Config): Add link to campaign user guide
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -628,7 +628,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="112">
   <si>
     <t xml:space="preserve">SoundScapeExplorer
 Version 12</t>
@@ -651,6 +651,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://sound-scape-explorer.github.io/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campaign user guide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sound-scape-explorer.github.io/docs/modules/campaign/user-guide/</t>
   </si>
   <si>
     <t xml:space="preserve">setting</t>
@@ -1535,7 +1541,7 @@
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMI12"/>
+  <dimension ref="A1:AMI13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1610,6 +1616,14 @@
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B5"/>
@@ -1617,6 +1631,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="https://sound-scape-explorer.github.io/"/>
+    <hyperlink ref="B13" r:id="rId2" display="https://sound-scape-explorer.github.io/docs/modules/campaign/user-guide/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1654,24 +1669,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="37" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B2" s="39" t="n">
         <v>2</v>
@@ -1682,7 +1697,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="37" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B3" s="38" t="n">
         <v>3</v>
@@ -1736,30 +1751,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="37" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B2" s="39" t="n">
         <v>50</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D2" s="39" t="n">
         <v>1</v>
@@ -1815,82 +1830,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="47" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="45" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="45" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="45" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="45" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="45" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="45" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1929,74 +1944,74 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="47" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="45" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="45" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="45" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="45" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="45" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2037,27 +2052,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="47" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="45" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2095,17 +2110,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="47" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2139,22 +2154,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="47" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2192,68 +2207,68 @@
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AMJ1" s="14"/>
     </row>
     <row r="2" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AMJ2" s="14"/>
     </row>
     <row r="3" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AMJ3" s="14"/>
     </row>
     <row r="4" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="16" t="n">
         <v>44100</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AMJ4" s="14"/>
     </row>
     <row r="5" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="18" t="n">
         <v>36526</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AMJ5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -3279,47 +3294,47 @@
     </row>
     <row r="7" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="22"/>
       <c r="C7" s="17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="AMJ7" s="14"/>
     </row>
     <row r="8" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="22" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="AMJ8" s="14"/>
     </row>
     <row r="9" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="22" t="n">
         <v>10</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AMJ9" s="14"/>
     </row>
     <row r="10" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" s="22" t="n">
         <v>42000</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AMJ10" s="14"/>
     </row>
@@ -3363,16 +3378,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3381,13 +3396,13 @@
         <v>/path/from/audio/folder</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" s="31" t="n">
         <v>45089.8854166667</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3448,18 +3463,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" s="33" t="n">
         <v>20</v>
@@ -3515,15 +3530,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2" s="33" t="n">
         <v>15</v>
@@ -3574,18 +3589,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B2" s="34" t="n">
         <v>44927</v>
@@ -3637,22 +3652,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" s="28" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3729,21 +3744,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B1" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="41" t="s">
-        <v>47</v>
-      </c>
       <c r="D1" s="41" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="37" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" s="38" t="n">
         <v>0</v>
@@ -3752,7 +3767,7 @@
         <v>1000</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E2" s="40" t="str">
         <f aca="false">VLOOKUP(A2,ListExtractors!$A$2:$B$1048576,2,0)</f>
@@ -3799,12 +3814,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="42" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" s="40" t="str">
         <f aca="false">VLOOKUP(A2,ListDigesters!$A$2:$B$1048576,2,0)</f>
@@ -3813,7 +3828,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="42" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B3" s="40" t="str">
         <f aca="false">VLOOKUP(A3,ListDigesters!$A$2:$B$1048576,2,0)</f>
@@ -3822,7 +3837,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="42" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B4" s="40" t="str">
         <f aca="false">VLOOKUP(A4,ListDigesters!$A$2:$B$1048576,2,0)</f>

</xml_diff>

<commit_message>
fix(Examples/Config): Fix first column in files tab
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -3361,9 +3361,11 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix(Examples/Config): Remove `vae` and `sparse_pca` reducers to prevent usage
</commit_message>
<xml_diff>
--- a/examples/campaigns/new-campaign/config.xlsx
+++ b/examples/campaigns/new-campaign/config.xlsx
@@ -628,7 +628,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
   <si>
     <t xml:space="preserve">SoundScapeExplorer
 Version 12</t>
@@ -1034,13 +1034,7 @@
     <t xml:space="preserve">Contingency between two clusters.</t>
   </si>
   <si>
-    <t xml:space="preserve">vae</t>
-  </si>
-  <si>
     <t xml:space="preserve">pca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sparse_pca</t>
   </si>
   <si>
     <t xml:space="preserve">hdbscan-leaf</t>
@@ -2034,7 +2028,7 @@
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2063,16 +2057,6 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2120,7 +2104,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2159,17 +2143,17 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>